<commit_message>
bitbucket pipeline generate excel auto go source code ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -59,7 +59,11 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-4秒则填40000</t>
+配速度值。
+com条长度为10000格。
+4秒走完则填2500
+act条长度也是10000。
+2秒走完则在技能表里填5000</t>
         </r>
       </text>
     </comment>
@@ -118,7 +122,8 @@
     <t>米数/秒</t>
   </si>
   <si>
-    <t>走10000格所需秒数</t>
+    <t xml:space="preserve">
+2500格/秒</t>
   </si>
   <si>
     <t>每秒</t>
@@ -714,11 +719,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -759,17 +764,27 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -781,16 +796,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -804,15 +827,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -827,53 +851,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -889,17 +881,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -941,7 +946,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -953,145 +1114,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1103,25 +1126,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1163,6 +1168,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1173,21 +1196,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1219,24 +1227,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1252,11 +1242,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1266,10 +1271,10 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1278,133 +1283,133 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2652,8 +2657,8 @@
   <sheetPr/>
   <dimension ref="A1:AW100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9:O10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -3359,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="12">
-        <v>30000</v>
+        <v>3333</v>
       </c>
       <c r="R7" s="12">
         <v>0</v>
@@ -3506,7 +3511,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="12">
-        <v>38000</v>
+        <v>3000</v>
       </c>
       <c r="R8" s="12">
         <v>0</v>
@@ -3653,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="12">
-        <v>40000</v>
+        <v>2500</v>
       </c>
       <c r="R9" s="12">
         <v>0</v>
@@ -3800,7 +3805,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="12">
-        <v>35000</v>
+        <v>2700</v>
       </c>
       <c r="R10" s="12">
         <v>0</v>

</xml_diff>

<commit_message>
[excel-pipeline]:9dcb555 auto commit ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -773,6 +773,28 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -781,9 +803,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -798,59 +848,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -865,14 +864,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -886,6 +878,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -894,24 +894,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -955,13 +955,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -973,73 +967,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1057,7 +985,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,7 +1045,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1081,31 +1111,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1117,13 +1123,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1186,10 +1186,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1210,21 +1245,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1236,17 +1256,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1265,25 +1274,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1292,133 +1292,133 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2666,8 +2666,8 @@
   <sheetPr/>
   <dimension ref="A1:AX100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -3408,7 +3408,7 @@
         <v>2500</v>
       </c>
       <c r="X7" s="12">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y7" s="16">
         <v>1000</v>
@@ -3558,7 +3558,7 @@
         <v>2500</v>
       </c>
       <c r="X8" s="12">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y8" s="16">
         <v>1000</v>
@@ -3708,7 +3708,7 @@
         <v>2500</v>
       </c>
       <c r="X9" s="12">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y9" s="16">
         <v>1000</v>
@@ -3858,7 +3858,7 @@
         <v>2500</v>
       </c>
       <c r="X10" s="12">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y10" s="16">
         <v>1000</v>
@@ -4008,7 +4008,7 @@
         <v>2500</v>
       </c>
       <c r="X11" s="12">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y11" s="16">
         <v>1000</v>
@@ -4156,7 +4156,7 @@
         <v>2500</v>
       </c>
       <c r="X12" s="12">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y12" s="16">
         <v>1000</v>
@@ -4304,7 +4304,7 @@
         <v>2500</v>
       </c>
       <c r="X13" s="12">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="Y13" s="16">
         <v>1000</v>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:4b97f72 commit_msg:百分比的改成number填小数 ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -37,7 +37,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-每秒的米数，10米则填100000</t>
+每秒的米数</t>
         </r>
       </text>
     </comment>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="207">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -113,13 +113,10 @@
     <t>属性描述</t>
   </si>
   <si>
-    <t>程序除10000转化百分比</t>
-  </si>
-  <si>
     <t>需显示百分比</t>
   </si>
   <si>
-    <t>米数/秒</t>
+    <t>填米数/秒</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -129,7 +126,7 @@
     <t>每秒</t>
   </si>
   <si>
-    <t>米*10000</t>
+    <t>米</t>
   </si>
   <si>
     <t>公式生成，不用填写</t>
@@ -435,7 +432,10 @@
     <t>int32</t>
   </si>
   <si>
-    <t>[]int32</t>
+    <t>number</t>
+  </si>
+  <si>
+    <t>[]number</t>
   </si>
   <si>
     <t>demo版本防战，1级默认值</t>
@@ -729,9 +729,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="27">
@@ -774,7 +774,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -789,22 +813,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -817,23 +826,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -856,15 +880,23 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -878,40 +910,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -955,7 +955,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -967,7 +1021,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -979,13 +1057,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -997,31 +1075,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1033,25 +1087,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1063,55 +1105,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1177,6 +1177,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1204,43 +1234,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1260,17 +1255,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1280,10 +1280,10 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1292,133 +1292,133 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2666,8 +2666,8 @@
   <sheetPr/>
   <dimension ref="A1:AX100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7:X13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C73" workbookViewId="0">
+      <selection activeCell="AB14" sqref="AB14:AB100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -2686,7 +2686,7 @@
     <col min="13" max="13" width="14.5" style="1" customWidth="1"/>
     <col min="14" max="14" width="7.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="12.5416666666667" style="1" customWidth="1"/>
-    <col min="16" max="16" width="19.3833333333333" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.625" style="1" customWidth="1"/>
     <col min="17" max="17" width="10.5416666666667" style="1" customWidth="1"/>
     <col min="18" max="18" width="17.15" style="1" customWidth="1"/>
     <col min="19" max="19" width="12.75" style="1" customWidth="1"/>
@@ -2767,422 +2767,420 @@
         <v>3</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="7" t="s">
-        <v>4</v>
-      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R2" s="6"/>
       <c r="S2" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T2" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Y2" s="3"/>
       <c r="Z2" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA2" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AC2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AT2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AU2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AV2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="AX2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" ht="16.15" customHeight="1" spans="1:50">
       <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="T3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="U3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="V3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="W3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="X3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="Y3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Z3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="AA3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" s="8" t="s">
+      <c r="AB3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AB3" s="8" t="s">
+      <c r="AC3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AD3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AE3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AF3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AG3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AH3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AI3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AJ3" s="8" t="s">
+      <c r="AK3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AL3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AL3" s="8" t="s">
+      <c r="AM3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AN3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AO3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AO3" s="8" t="s">
+      <c r="AP3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AP3" s="8" t="s">
+      <c r="AQ3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AQ3" s="8" t="s">
+      <c r="AR3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AR3" s="8" t="s">
+      <c r="AS3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AS3" s="8" t="s">
+      <c r="AT3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AT3" s="8" t="s">
+      <c r="AU3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AU3" s="8" t="s">
+      <c r="AV3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AV3" s="8" t="s">
+      <c r="AW3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AW3" s="8" t="s">
+      <c r="AX3" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="AX3" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" ht="16.15" customHeight="1" spans="1:50">
       <c r="A4" s="4"/>
       <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="T4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="W4" s="8" t="s">
+      <c r="X4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="Z4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AA4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AB4" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AC4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AD4" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="AE4" s="8" t="s">
+      <c r="AF4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AG4" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="AG4" s="8" t="s">
+      <c r="AH4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="AH4" s="8" t="s">
+      <c r="AI4" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="AI4" s="8" t="s">
+      <c r="AJ4" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="AJ4" s="8" t="s">
+      <c r="AK4" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="AK4" s="8" t="s">
+      <c r="AL4" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AL4" s="8" t="s">
+      <c r="AM4" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AM4" s="8" t="s">
+      <c r="AN4" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AN4" s="8" t="s">
+      <c r="AO4" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AO4" s="8" t="s">
+      <c r="AP4" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AP4" s="8" t="s">
+      <c r="AQ4" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AQ4" s="8" t="s">
+      <c r="AR4" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="AR4" s="8" t="s">
+      <c r="AS4" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="AS4" s="8" t="s">
+      <c r="AT4" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AT4" s="8" t="s">
+      <c r="AU4" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AU4" s="8" t="s">
+      <c r="AV4" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="AV4" s="8" t="s">
+      <c r="AW4" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AW4" s="8" t="s">
+      <c r="AX4" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="AX4" s="8" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" ht="16.15" customHeight="1" spans="1:50">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -3236,41 +3234,41 @@
     <row r="6" ht="16.15" customHeight="1" spans="1:50">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>110</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>110</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>110</v>
@@ -3279,37 +3277,37 @@
         <v>110</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>110</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V6" s="8" t="s">
         <v>110</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Z6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AA6" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AB6" s="8" t="s">
         <v>110</v>
@@ -3381,7 +3379,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="12">
-        <v>120000</v>
+        <v>12</v>
       </c>
       <c r="P7" s="12">
         <v>0</v>
@@ -3420,7 +3418,7 @@
         <v>0</v>
       </c>
       <c r="AB7" s="16">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="AC7" s="12">
         <v>0</v>
@@ -3453,7 +3451,7 @@
         <v>0</v>
       </c>
       <c r="AM7" s="12">
-        <v>1500</v>
+        <v>0.15</v>
       </c>
       <c r="AN7" s="12">
         <v>0</v>
@@ -3488,7 +3486,7 @@
       </c>
       <c r="AX7" s="10" t="str">
         <f>AM1:AM11&amp;","&amp;AN1:AN11&amp;","&amp;AO1:AO11&amp;","&amp;AP1:AP11&amp;","&amp;AQ1:AQ11&amp;","&amp;AR1:AR11&amp;","&amp;AS1:AS11&amp;","&amp;AT1:AT11&amp;","&amp;AU1:AU11&amp;","&amp;AV1:AV11</f>
-        <v>1500,0,0,0,0,0,0,0,0,0</v>
+        <v>0.15,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="8" ht="25" customHeight="1" spans="1:50">
@@ -3531,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="12">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="P8" s="12">
         <v>0</v>
@@ -3570,10 +3568,10 @@
         <v>0</v>
       </c>
       <c r="AB8" s="16">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="AC8" s="12">
-        <v>2000</v>
+        <v>0.2</v>
       </c>
       <c r="AD8" s="12">
         <v>0</v>
@@ -3634,7 +3632,7 @@
       </c>
       <c r="AW8" s="10" t="str">
         <f>AC2:AC12&amp;","&amp;AD2:AD12&amp;","&amp;AE2:AE12&amp;","&amp;AF2:AF12&amp;","&amp;AG2:AG12&amp;","&amp;AH2:AH12&amp;","&amp;AI2:AI12&amp;","&amp;AJ2:AJ12&amp;","&amp;AK2:AK12&amp;","&amp;AL2:AL12</f>
-        <v>2000,0,0,0,0,0,0,0,0,0</v>
+        <v>0.2,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX8" s="10" t="str">
         <f>AM2:AM12&amp;","&amp;AN2:AN12&amp;","&amp;AO2:AO12&amp;","&amp;AP2:AP12&amp;","&amp;AQ2:AQ12&amp;","&amp;AR2:AR12&amp;","&amp;AS2:AS12&amp;","&amp;AT2:AT12&amp;","&amp;AU2:AU12&amp;","&amp;AV2:AV12</f>
@@ -3681,7 +3679,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="12">
-        <v>80000</v>
+        <v>8</v>
       </c>
       <c r="P9" s="12">
         <v>0</v>
@@ -3720,7 +3718,7 @@
         <v>0</v>
       </c>
       <c r="AB9" s="16">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="AC9" s="12">
         <v>0</v>
@@ -3732,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="AF9" s="12">
-        <v>2000</v>
+        <v>0.2</v>
       </c>
       <c r="AG9" s="12">
         <v>0</v>
@@ -3784,7 +3782,7 @@
       </c>
       <c r="AW9" s="10" t="str">
         <f t="shared" ref="AW9:AW13" si="0">AC3:AC14&amp;","&amp;AD3:AD14&amp;","&amp;AE3:AE14&amp;","&amp;AF3:AF14&amp;","&amp;AG3:AG14&amp;","&amp;AH3:AH14&amp;","&amp;AI3:AI14&amp;","&amp;AJ3:AJ14&amp;","&amp;AK3:AK14&amp;","&amp;AL3:AL14</f>
-        <v>0,0,0,2000,0,0,0,0,0,0</v>
+        <v>0,0,0,0.2,0,0,0,0,0,0</v>
       </c>
       <c r="AX9" s="10" t="str">
         <f t="shared" ref="AX9:AX13" si="1">AM3:AM14&amp;","&amp;AN3:AN14&amp;","&amp;AO3:AO14&amp;","&amp;AP3:AP14&amp;","&amp;AQ3:AQ14&amp;","&amp;AR3:AR14&amp;","&amp;AS3:AS14&amp;","&amp;AT3:AT14&amp;","&amp;AU3:AU14&amp;","&amp;AV3:AV14</f>
@@ -3831,7 +3829,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="12">
-        <v>80000</v>
+        <v>8</v>
       </c>
       <c r="P10" s="12">
         <v>0</v>
@@ -3870,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="AB10" s="16">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="AC10" s="12">
         <v>0</v>
@@ -3879,7 +3877,7 @@
         <v>0</v>
       </c>
       <c r="AE10" s="12">
-        <v>500</v>
+        <v>0.005</v>
       </c>
       <c r="AF10" s="12">
         <v>0</v>
@@ -3934,7 +3932,7 @@
       </c>
       <c r="AW10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0,0,500,0,0,0,0,0,0,0</v>
+        <v>0,0,0.005,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX10" s="10" t="str">
         <f t="shared" si="1"/>
@@ -3981,13 +3979,13 @@
         <v>0</v>
       </c>
       <c r="O11" s="12">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="P11" s="12">
         <v>0</v>
       </c>
       <c r="Q11" s="12">
-        <v>40000</v>
+        <v>3000</v>
       </c>
       <c r="R11" s="12">
         <v>0</v>
@@ -4020,7 +4018,7 @@
         <v>0</v>
       </c>
       <c r="AB11" s="16">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="AC11" s="12">
         <v>0</v>
@@ -4129,13 +4127,13 @@
         <v>0</v>
       </c>
       <c r="O12" s="12">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="P12" s="12">
         <v>0</v>
       </c>
       <c r="Q12" s="12">
-        <v>40000</v>
+        <v>3000</v>
       </c>
       <c r="R12" s="12">
         <v>0</v>
@@ -4168,7 +4166,7 @@
         <v>0</v>
       </c>
       <c r="AB12" s="16">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="AC12" s="12">
         <v>0</v>
@@ -4277,13 +4275,13 @@
         <v>0</v>
       </c>
       <c r="O13" s="12">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="P13" s="12">
         <v>0</v>
       </c>
       <c r="Q13" s="12">
-        <v>40000</v>
+        <v>3000</v>
       </c>
       <c r="R13" s="12">
         <v>0</v>
@@ -4316,7 +4314,7 @@
         <v>0</v>
       </c>
       <c r="AB13" s="16">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="AC13" s="12">
         <v>0</v>
@@ -4463,6 +4461,9 @@
       <c r="AA14" s="1">
         <v>0</v>
       </c>
+      <c r="AB14" s="1">
+        <v>0</v>
+      </c>
       <c r="AC14" s="1">
         <v>0</v>
       </c>
@@ -4608,6 +4609,9 @@
       <c r="AA15" s="1">
         <v>0</v>
       </c>
+      <c r="AB15" s="1">
+        <v>0</v>
+      </c>
       <c r="AC15" s="1">
         <v>0</v>
       </c>
@@ -4753,6 +4757,9 @@
       <c r="AA16" s="1">
         <v>0</v>
       </c>
+      <c r="AB16" s="1">
+        <v>0</v>
+      </c>
       <c r="AC16" s="1">
         <v>0</v>
       </c>
@@ -4898,6 +4905,9 @@
       <c r="AA17" s="1">
         <v>0</v>
       </c>
+      <c r="AB17" s="1">
+        <v>0</v>
+      </c>
       <c r="AC17" s="1">
         <v>0</v>
       </c>
@@ -5043,6 +5053,9 @@
       <c r="AA18" s="1">
         <v>0</v>
       </c>
+      <c r="AB18" s="1">
+        <v>0</v>
+      </c>
       <c r="AC18" s="1">
         <v>0</v>
       </c>
@@ -5188,6 +5201,9 @@
       <c r="AA19" s="1">
         <v>0</v>
       </c>
+      <c r="AB19" s="1">
+        <v>0</v>
+      </c>
       <c r="AC19" s="1">
         <v>0</v>
       </c>
@@ -5295,13 +5311,13 @@
         <v>0</v>
       </c>
       <c r="O20" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
       </c>
       <c r="Q20" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="R20" s="1">
         <v>0</v>
@@ -5331,6 +5347,9 @@
         <v>0</v>
       </c>
       <c r="AA20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="1">
         <v>0</v>
       </c>
       <c r="AC20" s="1">
@@ -5440,13 +5459,13 @@
         <v>0</v>
       </c>
       <c r="O21" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="P21" s="12">
         <v>0</v>
       </c>
       <c r="Q21" s="1">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="R21" s="12">
         <v>0</v>
@@ -5478,73 +5497,76 @@
       <c r="AA21" s="1">
         <v>0</v>
       </c>
+      <c r="AB21" s="1">
+        <v>0</v>
+      </c>
       <c r="AC21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AD21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AE21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AF21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AG21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AH21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AI21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AJ21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AK21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AL21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AM21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AN21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AO21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AP21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AQ21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AR21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AS21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AT21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AU21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AV21" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AW21" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>50,50,50,50,50,50,50,50,50,50</v>
+        <v>0.005,0.005,0.005,0.005,0.005,0.005,0.005,0.005,0.005,0.005</v>
       </c>
       <c r="AX21" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>50,50,50,50,50,50,50,50,50,50</v>
+        <v>0.005,0.005,0.005,0.005,0.005,0.005,0.005,0.005,0.005,0.005</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="3:50">
@@ -5623,6 +5645,9 @@
       <c r="AA22" s="1">
         <v>0</v>
       </c>
+      <c r="AB22" s="1">
+        <v>0</v>
+      </c>
       <c r="AC22" s="1">
         <v>0</v>
       </c>
@@ -5768,6 +5793,9 @@
       <c r="AA23" s="1">
         <v>0</v>
       </c>
+      <c r="AB23" s="1">
+        <v>0</v>
+      </c>
       <c r="AC23" s="1">
         <v>0</v>
       </c>
@@ -5913,6 +5941,9 @@
       <c r="AA24" s="1">
         <v>0</v>
       </c>
+      <c r="AB24" s="1">
+        <v>0</v>
+      </c>
       <c r="AC24" s="1">
         <v>0</v>
       </c>
@@ -6058,6 +6089,9 @@
       <c r="AA25" s="1">
         <v>0</v>
       </c>
+      <c r="AB25" s="1">
+        <v>0</v>
+      </c>
       <c r="AC25" s="1">
         <v>0</v>
       </c>
@@ -6138,13 +6172,13 @@
         <v>10</v>
       </c>
       <c r="F26" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="G26" s="1">
         <v>10</v>
       </c>
       <c r="H26" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="I26" s="1">
         <v>25</v>
@@ -6168,13 +6202,13 @@
         <v>0</v>
       </c>
       <c r="P26" s="1">
-        <v>30</v>
+        <v>0.003</v>
       </c>
       <c r="Q26" s="1">
         <v>0</v>
       </c>
       <c r="R26" s="1">
-        <v>30</v>
+        <v>0.003</v>
       </c>
       <c r="S26" s="1">
         <v>30</v>
@@ -6186,7 +6220,7 @@
         <v>100</v>
       </c>
       <c r="V26" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="W26" s="1">
         <v>30</v>
@@ -6203,73 +6237,76 @@
       <c r="AA26" s="1">
         <v>0</v>
       </c>
+      <c r="AB26" s="1">
+        <v>0</v>
+      </c>
       <c r="AC26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AD26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AE26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AF26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AG26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AH26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AI26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AJ26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AK26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AL26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AM26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AN26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AO26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AP26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AQ26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AR26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AS26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AT26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AU26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AV26" s="1">
-        <v>25</v>
+        <v>0.025</v>
       </c>
       <c r="AW26" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>25,25,25,25,25,25,25,25,25,25</v>
+        <v>0.025,0.025,0.025,0.025,0.025,0.025,0.025,0.025,0.025,0.025</v>
       </c>
       <c r="AX26" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>25,25,25,25,25,25,25,25,25,25</v>
+        <v>0.025,0.025,0.025,0.025,0.025,0.025,0.025,0.025,0.025,0.025</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="3:50">
@@ -6348,8 +6385,11 @@
       <c r="AA27" s="1">
         <v>0</v>
       </c>
+      <c r="AB27" s="1">
+        <v>0</v>
+      </c>
       <c r="AC27" s="1">
-        <v>500</v>
+        <v>0.05</v>
       </c>
       <c r="AD27" s="1">
         <v>0</v>
@@ -6410,7 +6450,7 @@
       </c>
       <c r="AW27" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>500,0,0,0,0,0,0,0,0,0</v>
+        <v>0.05,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX27" s="10" t="str">
         <f t="shared" si="5"/>
@@ -6493,8 +6533,11 @@
       <c r="AA28" s="1">
         <v>0</v>
       </c>
+      <c r="AB28" s="1">
+        <v>0</v>
+      </c>
       <c r="AC28" s="1">
-        <v>1000</v>
+        <v>0.1</v>
       </c>
       <c r="AD28" s="1">
         <v>0</v>
@@ -6555,7 +6598,7 @@
       </c>
       <c r="AW28" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>1000,0,0,0,0,0,0,0,0,0</v>
+        <v>0.1,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX28" s="10" t="str">
         <f t="shared" si="5"/>
@@ -6638,8 +6681,11 @@
       <c r="AA29" s="1">
         <v>0</v>
       </c>
+      <c r="AB29" s="1">
+        <v>0</v>
+      </c>
       <c r="AC29" s="1">
-        <v>1500</v>
+        <v>0.15</v>
       </c>
       <c r="AD29" s="1">
         <v>0</v>
@@ -6700,7 +6746,7 @@
       </c>
       <c r="AW29" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>1500,0,0,0,0,0,0,0,0,0</v>
+        <v>0.15,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX29" s="10" t="str">
         <f t="shared" si="5"/>
@@ -6783,8 +6829,11 @@
       <c r="AA30" s="1">
         <v>0</v>
       </c>
+      <c r="AB30" s="1">
+        <v>0</v>
+      </c>
       <c r="AC30" s="1">
-        <v>2000</v>
+        <v>0.2</v>
       </c>
       <c r="AD30" s="1">
         <v>0</v>
@@ -6845,7 +6894,7 @@
       </c>
       <c r="AW30" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>2000,0,0,0,0,0,0,0,0,0</v>
+        <v>0.2,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX30" s="10" t="str">
         <f t="shared" si="5"/>
@@ -6928,8 +6977,11 @@
       <c r="AA31" s="1">
         <v>0</v>
       </c>
+      <c r="AB31" s="1">
+        <v>0</v>
+      </c>
       <c r="AC31" s="1">
-        <v>2500</v>
+        <v>0.25</v>
       </c>
       <c r="AD31" s="1">
         <v>0</v>
@@ -6990,7 +7042,7 @@
       </c>
       <c r="AW31" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>2500,0,0,0,0,0,0,0,0,0</v>
+        <v>0.25,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX31" s="10" t="str">
         <f t="shared" si="5"/>
@@ -7073,6 +7125,9 @@
       <c r="AA32" s="1">
         <v>0</v>
       </c>
+      <c r="AB32" s="1">
+        <v>0</v>
+      </c>
       <c r="AC32" s="1">
         <v>0</v>
       </c>
@@ -7218,6 +7273,9 @@
       <c r="AA33" s="1">
         <v>0</v>
       </c>
+      <c r="AB33" s="1">
+        <v>0</v>
+      </c>
       <c r="AC33" s="1">
         <v>0</v>
       </c>
@@ -7363,6 +7421,9 @@
       <c r="AA34" s="1">
         <v>0</v>
       </c>
+      <c r="AB34" s="1">
+        <v>0</v>
+      </c>
       <c r="AC34" s="1">
         <v>0</v>
       </c>
@@ -7508,6 +7569,9 @@
       <c r="AA35" s="1">
         <v>0</v>
       </c>
+      <c r="AB35" s="1">
+        <v>0</v>
+      </c>
       <c r="AC35" s="1">
         <v>0</v>
       </c>
@@ -7653,6 +7717,9 @@
       <c r="AA36" s="1">
         <v>0</v>
       </c>
+      <c r="AB36" s="1">
+        <v>0</v>
+      </c>
       <c r="AC36" s="1">
         <v>0</v>
       </c>
@@ -7798,6 +7865,9 @@
       <c r="AA37" s="1">
         <v>0</v>
       </c>
+      <c r="AB37" s="1">
+        <v>0</v>
+      </c>
       <c r="AC37" s="1">
         <v>0</v>
       </c>
@@ -7943,6 +8013,9 @@
       <c r="AA38" s="1">
         <v>0</v>
       </c>
+      <c r="AB38" s="1">
+        <v>0</v>
+      </c>
       <c r="AC38" s="1">
         <v>0</v>
       </c>
@@ -8088,6 +8161,9 @@
       <c r="AA39" s="1">
         <v>0</v>
       </c>
+      <c r="AB39" s="1">
+        <v>0</v>
+      </c>
       <c r="AC39" s="1">
         <v>0</v>
       </c>
@@ -8233,6 +8309,9 @@
       <c r="AA40" s="1">
         <v>0</v>
       </c>
+      <c r="AB40" s="1">
+        <v>0</v>
+      </c>
       <c r="AC40" s="1">
         <v>0</v>
       </c>
@@ -8378,6 +8457,9 @@
       <c r="AA41" s="1">
         <v>0</v>
       </c>
+      <c r="AB41" s="1">
+        <v>0</v>
+      </c>
       <c r="AC41" s="1">
         <v>0</v>
       </c>
@@ -8523,6 +8605,9 @@
       <c r="AA42" s="1">
         <v>0</v>
       </c>
+      <c r="AB42" s="1">
+        <v>0</v>
+      </c>
       <c r="AC42" s="1">
         <v>0</v>
       </c>
@@ -8639,7 +8724,7 @@
         <v>0</v>
       </c>
       <c r="R43" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="S43" s="1">
         <v>0</v>
@@ -8666,6 +8751,9 @@
         <v>0</v>
       </c>
       <c r="AA43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="1">
         <v>0</v>
       </c>
       <c r="AC43" s="1">
@@ -8784,7 +8872,7 @@
         <v>0</v>
       </c>
       <c r="R44" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="S44" s="1">
         <v>0</v>
@@ -8811,6 +8899,9 @@
         <v>0</v>
       </c>
       <c r="AA44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="1">
         <v>0</v>
       </c>
       <c r="AC44" s="1">
@@ -8923,7 +9014,7 @@
         <v>0</v>
       </c>
       <c r="P45" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="Q45" s="1">
         <v>0</v>
@@ -8956,6 +9047,9 @@
         <v>0</v>
       </c>
       <c r="AA45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="1">
         <v>0</v>
       </c>
       <c r="AC45" s="1">
@@ -9068,7 +9162,7 @@
         <v>0</v>
       </c>
       <c r="P46" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="Q46" s="1">
         <v>0</v>
@@ -9101,6 +9195,9 @@
         <v>0</v>
       </c>
       <c r="AA46" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="1">
         <v>0</v>
       </c>
       <c r="AC46" s="1">
@@ -9204,7 +9301,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="12">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="N47" s="1">
         <v>0</v>
@@ -9246,6 +9343,9 @@
         <v>0</v>
       </c>
       <c r="AA47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="1">
         <v>0</v>
       </c>
       <c r="AC47" s="1">
@@ -9349,7 +9449,7 @@
         <v>0</v>
       </c>
       <c r="M48" s="12">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="N48" s="1">
         <v>0</v>
@@ -9391,6 +9491,9 @@
         <v>0</v>
       </c>
       <c r="AA48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="1">
         <v>0</v>
       </c>
       <c r="AC48" s="1">
@@ -9538,6 +9641,9 @@
       <c r="AA49" s="1">
         <v>0</v>
       </c>
+      <c r="AB49" s="1">
+        <v>0</v>
+      </c>
       <c r="AC49" s="1">
         <v>0</v>
       </c>
@@ -9683,6 +9789,9 @@
       <c r="AA50" s="1">
         <v>0</v>
       </c>
+      <c r="AB50" s="1">
+        <v>0</v>
+      </c>
       <c r="AC50" s="1">
         <v>0</v>
       </c>
@@ -9828,11 +9937,14 @@
       <c r="AA51" s="1">
         <v>0</v>
       </c>
+      <c r="AB51" s="1">
+        <v>0</v>
+      </c>
       <c r="AC51" s="1">
         <v>0</v>
       </c>
       <c r="AD51" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="AE51" s="1">
         <v>0</v>
@@ -9890,7 +10002,7 @@
       </c>
       <c r="AW51" s="10" t="str">
         <f t="shared" ref="AW51:AW56" si="8">AC43:AC55&amp;","&amp;AD43:AD55&amp;","&amp;AE43:AE55&amp;","&amp;AF43:AF55&amp;","&amp;AG43:AG55&amp;","&amp;AH43:AH55&amp;","&amp;AI43:AI55&amp;","&amp;AJ43:AJ55&amp;","&amp;AK43:AK55&amp;","&amp;AL43:AL55</f>
-        <v>0,20,0,0,0,0,0,0,0,0</v>
+        <v>0,0.002,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX51" s="10" t="str">
         <f t="shared" ref="AX51:AX56" si="9">AM43:AM55&amp;","&amp;AN43:AN55&amp;","&amp;AO43:AO55&amp;","&amp;AP43:AP55&amp;","&amp;AQ43:AQ55&amp;","&amp;AR43:AR55&amp;","&amp;AS43:AS55&amp;","&amp;AT43:AT55&amp;","&amp;AU43:AU55&amp;","&amp;AV43:AV55</f>
@@ -9973,6 +10085,9 @@
       <c r="AA52" s="1">
         <v>0</v>
       </c>
+      <c r="AB52" s="1">
+        <v>0</v>
+      </c>
       <c r="AC52" s="1">
         <v>0</v>
       </c>
@@ -9980,7 +10095,7 @@
         <v>0</v>
       </c>
       <c r="AE52" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="AF52" s="1">
         <v>0</v>
@@ -10035,7 +10150,7 @@
       </c>
       <c r="AW52" s="10" t="str">
         <f t="shared" si="8"/>
-        <v>0,0,20,0,0,0,0,0,0,0</v>
+        <v>0,0,0.002,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX52" s="10" t="str">
         <f t="shared" si="9"/>
@@ -10118,6 +10233,9 @@
       <c r="AA53" s="1">
         <v>0</v>
       </c>
+      <c r="AB53" s="1">
+        <v>0</v>
+      </c>
       <c r="AC53" s="1">
         <v>0</v>
       </c>
@@ -10128,7 +10246,7 @@
         <v>0</v>
       </c>
       <c r="AF53" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="AG53" s="1">
         <v>0</v>
@@ -10180,7 +10298,7 @@
       </c>
       <c r="AW53" s="10" t="str">
         <f t="shared" si="8"/>
-        <v>0,0,0,20,0,0,0,0,0,0</v>
+        <v>0,0,0,0.002,0,0,0,0,0,0</v>
       </c>
       <c r="AX53" s="10" t="str">
         <f t="shared" si="9"/>
@@ -10263,6 +10381,9 @@
       <c r="AA54" s="1">
         <v>0</v>
       </c>
+      <c r="AB54" s="1">
+        <v>0</v>
+      </c>
       <c r="AC54" s="1">
         <v>0</v>
       </c>
@@ -10276,7 +10397,7 @@
         <v>0</v>
       </c>
       <c r="AG54" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="AH54" s="1">
         <v>0</v>
@@ -10325,7 +10446,7 @@
       </c>
       <c r="AW54" s="10" t="str">
         <f t="shared" si="8"/>
-        <v>0,0,0,0,20,0,0,0,0,0</v>
+        <v>0,0,0,0,0.002,0,0,0,0,0</v>
       </c>
       <c r="AX54" s="10" t="str">
         <f t="shared" si="9"/>
@@ -10408,6 +10529,9 @@
       <c r="AA55" s="1">
         <v>0</v>
       </c>
+      <c r="AB55" s="1">
+        <v>0</v>
+      </c>
       <c r="AC55" s="1">
         <v>0</v>
       </c>
@@ -10424,7 +10548,7 @@
         <v>0</v>
       </c>
       <c r="AH55" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="AI55" s="1">
         <v>0</v>
@@ -10470,7 +10594,7 @@
       </c>
       <c r="AW55" s="10" t="str">
         <f t="shared" si="8"/>
-        <v>0,0,0,0,0,20,0,0,0,0</v>
+        <v>0,0,0,0,0,0.002,0,0,0,0</v>
       </c>
       <c r="AX55" s="10" t="str">
         <f t="shared" si="9"/>
@@ -10553,6 +10677,9 @@
       <c r="AA56" s="1">
         <v>0</v>
       </c>
+      <c r="AB56" s="1">
+        <v>0</v>
+      </c>
       <c r="AC56" s="1">
         <v>0</v>
       </c>
@@ -10572,7 +10699,7 @@
         <v>0</v>
       </c>
       <c r="AI56" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="AJ56" s="1">
         <v>0</v>
@@ -10615,7 +10742,7 @@
       </c>
       <c r="AW56" s="10" t="str">
         <f t="shared" si="8"/>
-        <v>0,0,0,0,0,0,20,0,0,0</v>
+        <v>0,0,0,0,0,0,0.002,0,0,0</v>
       </c>
       <c r="AX56" s="10" t="str">
         <f t="shared" si="9"/>
@@ -10698,6 +10825,9 @@
       <c r="AA57" s="1">
         <v>0</v>
       </c>
+      <c r="AB57" s="1">
+        <v>0</v>
+      </c>
       <c r="AC57" s="1">
         <v>0</v>
       </c>
@@ -10720,7 +10850,7 @@
         <v>0</v>
       </c>
       <c r="AJ57" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="AK57" s="1">
         <v>0</v>
@@ -10760,7 +10890,7 @@
       </c>
       <c r="AW57" s="10" t="str">
         <f t="shared" ref="AW52:AW86" si="10">AC51:AC61&amp;","&amp;AD51:AD61&amp;","&amp;AE51:AE61&amp;","&amp;AF51:AF61&amp;","&amp;AG51:AG61&amp;","&amp;AH51:AH61&amp;","&amp;AI51:AI61&amp;","&amp;AJ51:AJ61&amp;","&amp;AK51:AK61&amp;","&amp;AL51:AL61</f>
-        <v>0,0,0,0,0,0,0,20,0,0</v>
+        <v>0,0,0,0,0,0,0,0.002,0,0</v>
       </c>
       <c r="AX57" s="10" t="str">
         <f t="shared" ref="AX52:AX86" si="11">AM51:AM61&amp;","&amp;AN51:AN61&amp;","&amp;AO51:AO61&amp;","&amp;AP51:AP61&amp;","&amp;AQ51:AQ61&amp;","&amp;AR51:AR61&amp;","&amp;AS51:AS61&amp;","&amp;AT51:AT61&amp;","&amp;AU51:AU61&amp;","&amp;AV51:AV61</f>
@@ -10843,6 +10973,9 @@
       <c r="AA58" s="1">
         <v>0</v>
       </c>
+      <c r="AB58" s="1">
+        <v>0</v>
+      </c>
       <c r="AC58" s="1">
         <v>0</v>
       </c>
@@ -10868,7 +11001,7 @@
         <v>0</v>
       </c>
       <c r="AK58" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="AL58" s="1">
         <v>0</v>
@@ -10905,7 +11038,7 @@
       </c>
       <c r="AW58" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,0,0,0,0,0,0,0,20,0</v>
+        <v>0,0,0,0,0,0,0,0,0.002,0</v>
       </c>
       <c r="AX58" s="10" t="str">
         <f t="shared" si="11"/>
@@ -10988,6 +11121,9 @@
       <c r="AA59" s="1">
         <v>0</v>
       </c>
+      <c r="AB59" s="1">
+        <v>0</v>
+      </c>
       <c r="AC59" s="1">
         <v>0</v>
       </c>
@@ -11016,7 +11152,7 @@
         <v>0</v>
       </c>
       <c r="AL59" s="1">
-        <v>20</v>
+        <v>0.002</v>
       </c>
       <c r="AM59" s="1">
         <v>0</v>
@@ -11050,7 +11186,7 @@
       </c>
       <c r="AW59" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,0,0,0,0,0,0,0,0,20</v>
+        <v>0,0,0,0,0,0,0,0,0,0.002</v>
       </c>
       <c r="AX59" s="10" t="str">
         <f t="shared" si="11"/>
@@ -11133,11 +11269,14 @@
       <c r="AA60" s="1">
         <v>0</v>
       </c>
+      <c r="AB60" s="1">
+        <v>0</v>
+      </c>
       <c r="AC60" s="1">
         <v>0</v>
       </c>
       <c r="AD60" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AE60" s="1">
         <v>0</v>
@@ -11195,7 +11334,7 @@
       </c>
       <c r="AW60" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,50,0,0,0,0,0,0,0,0</v>
+        <v>0,0.005,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX60" s="10" t="str">
         <f t="shared" si="11"/>
@@ -11278,6 +11417,9 @@
       <c r="AA61" s="1">
         <v>0</v>
       </c>
+      <c r="AB61" s="1">
+        <v>0</v>
+      </c>
       <c r="AC61" s="1">
         <v>0</v>
       </c>
@@ -11285,7 +11427,7 @@
         <v>0</v>
       </c>
       <c r="AE61" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AF61" s="1">
         <v>0</v>
@@ -11340,7 +11482,7 @@
       </c>
       <c r="AW61" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,0,50,0,0,0,0,0,0,0</v>
+        <v>0,0,0.005,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX61" s="10" t="str">
         <f t="shared" si="11"/>
@@ -11423,6 +11565,9 @@
       <c r="AA62" s="1">
         <v>0</v>
       </c>
+      <c r="AB62" s="1">
+        <v>0</v>
+      </c>
       <c r="AC62" s="1">
         <v>0</v>
       </c>
@@ -11433,7 +11578,7 @@
         <v>0</v>
       </c>
       <c r="AF62" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AG62" s="1">
         <v>0</v>
@@ -11485,7 +11630,7 @@
       </c>
       <c r="AW62" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,0,0,50,0,0,0,0,0,0</v>
+        <v>0,0,0,0.005,0,0,0,0,0,0</v>
       </c>
       <c r="AX62" s="10" t="str">
         <f t="shared" si="11"/>
@@ -11568,6 +11713,9 @@
       <c r="AA63" s="1">
         <v>0</v>
       </c>
+      <c r="AB63" s="1">
+        <v>0</v>
+      </c>
       <c r="AC63" s="1">
         <v>0</v>
       </c>
@@ -11581,7 +11729,7 @@
         <v>0</v>
       </c>
       <c r="AG63" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AH63" s="1">
         <v>0</v>
@@ -11630,7 +11778,7 @@
       </c>
       <c r="AW63" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,0,0,0,50,0,0,0,0,0</v>
+        <v>0,0,0,0,0.005,0,0,0,0,0</v>
       </c>
       <c r="AX63" s="10" t="str">
         <f t="shared" si="11"/>
@@ -11713,6 +11861,9 @@
       <c r="AA64" s="1">
         <v>0</v>
       </c>
+      <c r="AB64" s="1">
+        <v>0</v>
+      </c>
       <c r="AC64" s="1">
         <v>0</v>
       </c>
@@ -11729,7 +11880,7 @@
         <v>0</v>
       </c>
       <c r="AH64" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AI64" s="1">
         <v>0</v>
@@ -11775,7 +11926,7 @@
       </c>
       <c r="AW64" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,0,0,0,0,50,0,0,0,0</v>
+        <v>0,0,0,0,0,0.005,0,0,0,0</v>
       </c>
       <c r="AX64" s="10" t="str">
         <f t="shared" si="11"/>
@@ -11858,6 +12009,9 @@
       <c r="AA65" s="1">
         <v>0</v>
       </c>
+      <c r="AB65" s="1">
+        <v>0</v>
+      </c>
       <c r="AC65" s="1">
         <v>0</v>
       </c>
@@ -11877,7 +12031,7 @@
         <v>0</v>
       </c>
       <c r="AI65" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AJ65" s="1">
         <v>0</v>
@@ -11920,7 +12074,7 @@
       </c>
       <c r="AW65" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,0,0,0,0,0,50,0,0,0</v>
+        <v>0,0,0,0,0,0,0.005,0,0,0</v>
       </c>
       <c r="AX65" s="10" t="str">
         <f t="shared" si="11"/>
@@ -12003,6 +12157,9 @@
       <c r="AA66" s="1">
         <v>0</v>
       </c>
+      <c r="AB66" s="1">
+        <v>0</v>
+      </c>
       <c r="AC66" s="1">
         <v>0</v>
       </c>
@@ -12025,7 +12182,7 @@
         <v>0</v>
       </c>
       <c r="AJ66" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AK66" s="1">
         <v>0</v>
@@ -12065,7 +12222,7 @@
       </c>
       <c r="AW66" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,0,0,0,0,0,0,50,0,0</v>
+        <v>0,0,0,0,0,0,0,0.005,0,0</v>
       </c>
       <c r="AX66" s="10" t="str">
         <f t="shared" si="11"/>
@@ -12148,6 +12305,9 @@
       <c r="AA67" s="1">
         <v>0</v>
       </c>
+      <c r="AB67" s="1">
+        <v>0</v>
+      </c>
       <c r="AC67" s="1">
         <v>0</v>
       </c>
@@ -12173,7 +12333,7 @@
         <v>0</v>
       </c>
       <c r="AK67" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AL67" s="1">
         <v>0</v>
@@ -12210,7 +12370,7 @@
       </c>
       <c r="AW67" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,0,0,0,0,0,0,0,50,0</v>
+        <v>0,0,0,0,0,0,0,0,0.005,0</v>
       </c>
       <c r="AX67" s="10" t="str">
         <f t="shared" si="11"/>
@@ -12293,6 +12453,9 @@
       <c r="AA68" s="1">
         <v>0</v>
       </c>
+      <c r="AB68" s="1">
+        <v>0</v>
+      </c>
       <c r="AC68" s="1">
         <v>0</v>
       </c>
@@ -12321,7 +12484,7 @@
         <v>0</v>
       </c>
       <c r="AL68" s="1">
-        <v>50</v>
+        <v>0.005</v>
       </c>
       <c r="AM68" s="1">
         <v>0</v>
@@ -12355,7 +12518,7 @@
       </c>
       <c r="AW68" s="10" t="str">
         <f t="shared" si="10"/>
-        <v>0,0,0,0,0,0,0,0,0,50</v>
+        <v>0,0,0,0,0,0,0,0,0,0.005</v>
       </c>
       <c r="AX68" s="10" t="str">
         <f t="shared" si="11"/>
@@ -12438,6 +12601,9 @@
       <c r="AA69" s="2">
         <v>0</v>
       </c>
+      <c r="AB69" s="1">
+        <v>0</v>
+      </c>
       <c r="AC69" s="2">
         <v>0</v>
       </c>
@@ -12471,8 +12637,8 @@
       <c r="AM69" s="2">
         <v>0</v>
       </c>
-      <c r="AN69" s="2">
-        <v>20</v>
+      <c r="AN69" s="1">
+        <v>0.002</v>
       </c>
       <c r="AO69" s="2">
         <v>0</v>
@@ -12504,7 +12670,7 @@
       </c>
       <c r="AX69" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,20,0,0,0,0,0,0,0,0</v>
+        <v>0,0.002,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="70" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -12583,6 +12749,9 @@
       <c r="AA70" s="2">
         <v>0</v>
       </c>
+      <c r="AB70" s="1">
+        <v>0</v>
+      </c>
       <c r="AC70" s="2">
         <v>0</v>
       </c>
@@ -12619,8 +12788,8 @@
       <c r="AN70" s="2">
         <v>0</v>
       </c>
-      <c r="AO70" s="2">
-        <v>20</v>
+      <c r="AO70" s="1">
+        <v>0.002</v>
       </c>
       <c r="AP70" s="2">
         <v>0</v>
@@ -12649,7 +12818,7 @@
       </c>
       <c r="AX70" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,20,0,0,0,0,0,0,0</v>
+        <v>0,0,0.002,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="71" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -12728,6 +12897,9 @@
       <c r="AA71" s="2">
         <v>0</v>
       </c>
+      <c r="AB71" s="1">
+        <v>0</v>
+      </c>
       <c r="AC71" s="2">
         <v>0</v>
       </c>
@@ -12767,8 +12939,8 @@
       <c r="AO71" s="2">
         <v>0</v>
       </c>
-      <c r="AP71" s="2">
-        <v>20</v>
+      <c r="AP71" s="1">
+        <v>0.002</v>
       </c>
       <c r="AQ71" s="2">
         <v>0</v>
@@ -12794,7 +12966,7 @@
       </c>
       <c r="AX71" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,20,0,0,0,0,0,0</v>
+        <v>0,0,0,0.002,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="72" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -12873,6 +13045,9 @@
       <c r="AA72" s="2">
         <v>0</v>
       </c>
+      <c r="AB72" s="1">
+        <v>0</v>
+      </c>
       <c r="AC72" s="2">
         <v>0</v>
       </c>
@@ -12915,8 +13090,8 @@
       <c r="AP72" s="2">
         <v>0</v>
       </c>
-      <c r="AQ72" s="2">
-        <v>20</v>
+      <c r="AQ72" s="1">
+        <v>0.002</v>
       </c>
       <c r="AR72" s="2">
         <v>0</v>
@@ -12939,7 +13114,7 @@
       </c>
       <c r="AX72" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,0,20,0,0,0,0,0</v>
+        <v>0,0,0,0,0.002,0,0,0,0,0</v>
       </c>
     </row>
     <row r="73" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -13018,6 +13193,9 @@
       <c r="AA73" s="2">
         <v>0</v>
       </c>
+      <c r="AB73" s="1">
+        <v>0</v>
+      </c>
       <c r="AC73" s="2">
         <v>0</v>
       </c>
@@ -13063,8 +13241,8 @@
       <c r="AQ73" s="2">
         <v>0</v>
       </c>
-      <c r="AR73" s="2">
-        <v>20</v>
+      <c r="AR73" s="1">
+        <v>0.002</v>
       </c>
       <c r="AS73" s="2">
         <v>0</v>
@@ -13084,7 +13262,7 @@
       </c>
       <c r="AX73" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,0,0,20,0,0,0,0</v>
+        <v>0,0,0,0,0,0.002,0,0,0,0</v>
       </c>
     </row>
     <row r="74" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -13163,6 +13341,9 @@
       <c r="AA74" s="2">
         <v>0</v>
       </c>
+      <c r="AB74" s="1">
+        <v>0</v>
+      </c>
       <c r="AC74" s="2">
         <v>0</v>
       </c>
@@ -13211,8 +13392,8 @@
       <c r="AR74" s="2">
         <v>0</v>
       </c>
-      <c r="AS74" s="2">
-        <v>20</v>
+      <c r="AS74" s="1">
+        <v>0.002</v>
       </c>
       <c r="AT74" s="2">
         <v>0</v>
@@ -13229,7 +13410,7 @@
       </c>
       <c r="AX74" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,0,0,0,20,0,0,0</v>
+        <v>0,0,0,0,0,0,0.002,0,0,0</v>
       </c>
     </row>
     <row r="75" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -13308,6 +13489,9 @@
       <c r="AA75" s="2">
         <v>0</v>
       </c>
+      <c r="AB75" s="1">
+        <v>0</v>
+      </c>
       <c r="AC75" s="2">
         <v>0</v>
       </c>
@@ -13359,8 +13543,8 @@
       <c r="AS75" s="2">
         <v>0</v>
       </c>
-      <c r="AT75" s="2">
-        <v>20</v>
+      <c r="AT75" s="1">
+        <v>0.002</v>
       </c>
       <c r="AU75" s="2">
         <v>0</v>
@@ -13374,7 +13558,7 @@
       </c>
       <c r="AX75" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,0,0,0,0,20,0,0</v>
+        <v>0,0,0,0,0,0,0,0.002,0,0</v>
       </c>
     </row>
     <row r="76" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -13453,6 +13637,9 @@
       <c r="AA76" s="2">
         <v>0</v>
       </c>
+      <c r="AB76" s="1">
+        <v>0</v>
+      </c>
       <c r="AC76" s="2">
         <v>0</v>
       </c>
@@ -13507,8 +13694,8 @@
       <c r="AT76" s="2">
         <v>0</v>
       </c>
-      <c r="AU76" s="2">
-        <v>20</v>
+      <c r="AU76" s="1">
+        <v>0.002</v>
       </c>
       <c r="AV76" s="2">
         <v>0</v>
@@ -13519,7 +13706,7 @@
       </c>
       <c r="AX76" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,0,0,0,0,0,20,0</v>
+        <v>0,0,0,0,0,0,0,0,0.002,0</v>
       </c>
     </row>
     <row r="77" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -13598,6 +13785,9 @@
       <c r="AA77" s="2">
         <v>0</v>
       </c>
+      <c r="AB77" s="1">
+        <v>0</v>
+      </c>
       <c r="AC77" s="2">
         <v>0</v>
       </c>
@@ -13743,6 +13933,9 @@
       <c r="AA78" s="2">
         <v>0</v>
       </c>
+      <c r="AB78" s="1">
+        <v>0</v>
+      </c>
       <c r="AC78" s="2">
         <v>0</v>
       </c>
@@ -13773,8 +13966,11 @@
       <c r="AL78" s="2">
         <v>0</v>
       </c>
-      <c r="AN78" s="2">
-        <v>50</v>
+      <c r="AM78" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN78" s="1">
+        <v>0.005</v>
       </c>
       <c r="AO78" s="2">
         <v>0</v>
@@ -13806,7 +14002,7 @@
       </c>
       <c r="AX78" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>,50,0,0,0,0,0,0,0,0</v>
+        <v>0,0.005,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="79" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -13885,6 +14081,9 @@
       <c r="AA79" s="2">
         <v>0</v>
       </c>
+      <c r="AB79" s="1">
+        <v>0</v>
+      </c>
       <c r="AC79" s="2">
         <v>0</v>
       </c>
@@ -13921,8 +14120,8 @@
       <c r="AN79" s="2">
         <v>0</v>
       </c>
-      <c r="AO79" s="2">
-        <v>50</v>
+      <c r="AO79" s="1">
+        <v>0.005</v>
       </c>
       <c r="AP79" s="2">
         <v>0</v>
@@ -13951,7 +14150,7 @@
       </c>
       <c r="AX79" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,50,0,0,0,0,0,0,0</v>
+        <v>0,0,0.005,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="80" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -14030,6 +14229,9 @@
       <c r="AA80" s="2">
         <v>0</v>
       </c>
+      <c r="AB80" s="1">
+        <v>0</v>
+      </c>
       <c r="AC80" s="2">
         <v>0</v>
       </c>
@@ -14069,8 +14271,8 @@
       <c r="AO80" s="2">
         <v>0</v>
       </c>
-      <c r="AP80" s="2">
-        <v>50</v>
+      <c r="AP80" s="1">
+        <v>0.005</v>
       </c>
       <c r="AQ80" s="2">
         <v>0</v>
@@ -14096,7 +14298,7 @@
       </c>
       <c r="AX80" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,50,0,0,0,0,0,0</v>
+        <v>0,0,0,0.005,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="81" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -14175,6 +14377,9 @@
       <c r="AA81" s="2">
         <v>0</v>
       </c>
+      <c r="AB81" s="1">
+        <v>0</v>
+      </c>
       <c r="AC81" s="2">
         <v>0</v>
       </c>
@@ -14217,8 +14422,8 @@
       <c r="AP81" s="2">
         <v>0</v>
       </c>
-      <c r="AQ81" s="2">
-        <v>50</v>
+      <c r="AQ81" s="1">
+        <v>0.005</v>
       </c>
       <c r="AR81" s="2">
         <v>0</v>
@@ -14241,7 +14446,7 @@
       </c>
       <c r="AX81" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,0,50,0,0,0,0,0</v>
+        <v>0,0,0,0,0.005,0,0,0,0,0</v>
       </c>
     </row>
     <row r="82" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -14320,6 +14525,9 @@
       <c r="AA82" s="2">
         <v>0</v>
       </c>
+      <c r="AB82" s="1">
+        <v>0</v>
+      </c>
       <c r="AC82" s="2">
         <v>0</v>
       </c>
@@ -14365,8 +14573,8 @@
       <c r="AQ82" s="2">
         <v>0</v>
       </c>
-      <c r="AR82" s="2">
-        <v>50</v>
+      <c r="AR82" s="1">
+        <v>0.005</v>
       </c>
       <c r="AS82" s="2">
         <v>0</v>
@@ -14386,7 +14594,7 @@
       </c>
       <c r="AX82" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,0,0,50,0,0,0,0</v>
+        <v>0,0,0,0,0,0.005,0,0,0,0</v>
       </c>
     </row>
     <row r="83" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -14465,6 +14673,9 @@
       <c r="AA83" s="2">
         <v>0</v>
       </c>
+      <c r="AB83" s="1">
+        <v>0</v>
+      </c>
       <c r="AC83" s="2">
         <v>0</v>
       </c>
@@ -14513,8 +14724,8 @@
       <c r="AR83" s="2">
         <v>0</v>
       </c>
-      <c r="AS83" s="2">
-        <v>50</v>
+      <c r="AS83" s="1">
+        <v>0.005</v>
       </c>
       <c r="AT83" s="2">
         <v>0</v>
@@ -14531,7 +14742,7 @@
       </c>
       <c r="AX83" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,0,0,0,50,0,0,0</v>
+        <v>0,0,0,0,0,0,0.005,0,0,0</v>
       </c>
     </row>
     <row r="84" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -14610,6 +14821,9 @@
       <c r="AA84" s="2">
         <v>0</v>
       </c>
+      <c r="AB84" s="1">
+        <v>0</v>
+      </c>
       <c r="AC84" s="2">
         <v>0</v>
       </c>
@@ -14661,8 +14875,8 @@
       <c r="AS84" s="2">
         <v>0</v>
       </c>
-      <c r="AT84" s="2">
-        <v>50</v>
+      <c r="AT84" s="1">
+        <v>0.005</v>
       </c>
       <c r="AU84" s="2">
         <v>0</v>
@@ -14676,7 +14890,7 @@
       </c>
       <c r="AX84" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,0,0,0,0,50,0,0</v>
+        <v>0,0,0,0,0,0,0,0.005,0,0</v>
       </c>
     </row>
     <row r="85" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -14755,6 +14969,9 @@
       <c r="AA85" s="2">
         <v>0</v>
       </c>
+      <c r="AB85" s="1">
+        <v>0</v>
+      </c>
       <c r="AC85" s="2">
         <v>0</v>
       </c>
@@ -14809,8 +15026,8 @@
       <c r="AT85" s="2">
         <v>0</v>
       </c>
-      <c r="AU85" s="2">
-        <v>50</v>
+      <c r="AU85" s="1">
+        <v>0.005</v>
       </c>
       <c r="AV85" s="2">
         <v>0</v>
@@ -14821,7 +15038,7 @@
       </c>
       <c r="AX85" s="20" t="str">
         <f t="shared" si="11"/>
-        <v>0,0,0,0,0,0,0,0,50,0</v>
+        <v>0,0,0,0,0,0,0,0,0.005,0</v>
       </c>
     </row>
     <row r="86" s="2" customFormat="1" customHeight="1" spans="3:50">
@@ -14900,6 +15117,9 @@
       <c r="AA86" s="2">
         <v>0</v>
       </c>
+      <c r="AB86" s="1">
+        <v>0</v>
+      </c>
       <c r="AC86" s="2">
         <v>0</v>
       </c>
@@ -15045,6 +15265,9 @@
       <c r="AA87" s="1">
         <v>0</v>
       </c>
+      <c r="AB87" s="1">
+        <v>0</v>
+      </c>
       <c r="AC87" s="1">
         <v>0</v>
       </c>
@@ -15190,6 +15413,9 @@
       <c r="AA88" s="1">
         <v>0</v>
       </c>
+      <c r="AB88" s="1">
+        <v>0</v>
+      </c>
       <c r="AC88" s="1">
         <v>0</v>
       </c>
@@ -15335,6 +15561,9 @@
       <c r="AA89" s="1">
         <v>0</v>
       </c>
+      <c r="AB89" s="1">
+        <v>0</v>
+      </c>
       <c r="AC89" s="1">
         <v>0</v>
       </c>
@@ -15415,7 +15644,7 @@
         <v>0</v>
       </c>
       <c r="F90" s="1">
-        <v>450</v>
+        <v>0.045</v>
       </c>
       <c r="G90" s="1">
         <v>0</v>
@@ -15478,6 +15707,9 @@
         <v>0</v>
       </c>
       <c r="AA90" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB90" s="1">
         <v>0</v>
       </c>
       <c r="AC90" s="1">
@@ -15566,7 +15798,7 @@
         <v>0</v>
       </c>
       <c r="H91" s="1">
-        <v>450</v>
+        <v>0.045</v>
       </c>
       <c r="I91" s="1">
         <v>0</v>
@@ -15623,6 +15855,9 @@
         <v>0</v>
       </c>
       <c r="AA91" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB91" s="1">
         <v>0</v>
       </c>
       <c r="AC91" s="1">
@@ -15753,7 +15988,7 @@
         <v>0</v>
       </c>
       <c r="V92" s="1">
-        <v>450</v>
+        <v>0.045</v>
       </c>
       <c r="W92" s="1">
         <v>0</v>
@@ -15768,6 +16003,9 @@
         <v>0</v>
       </c>
       <c r="AA92" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB92" s="1">
         <v>0</v>
       </c>
       <c r="AC92" s="1">
@@ -15915,6 +16153,9 @@
       <c r="AA93" s="1">
         <v>0</v>
       </c>
+      <c r="AB93" s="1">
+        <v>0</v>
+      </c>
       <c r="AC93" s="1">
         <v>0</v>
       </c>
@@ -16060,6 +16301,9 @@
       <c r="AA94" s="1">
         <v>0</v>
       </c>
+      <c r="AB94" s="1">
+        <v>0</v>
+      </c>
       <c r="AC94" s="1">
         <v>0</v>
       </c>
@@ -16205,6 +16449,9 @@
       <c r="AA95" s="1">
         <v>0</v>
       </c>
+      <c r="AB95" s="1">
+        <v>0</v>
+      </c>
       <c r="AC95" s="1">
         <v>0</v>
       </c>
@@ -16350,6 +16597,9 @@
       <c r="AA96" s="1">
         <v>0</v>
       </c>
+      <c r="AB96" s="1">
+        <v>0</v>
+      </c>
       <c r="AC96" s="1">
         <v>0</v>
       </c>
@@ -16495,6 +16745,9 @@
       <c r="AA97" s="1">
         <v>0</v>
       </c>
+      <c r="AB97" s="1">
+        <v>0</v>
+      </c>
       <c r="AC97" s="1">
         <v>0</v>
       </c>
@@ -16611,7 +16864,7 @@
         <v>0</v>
       </c>
       <c r="R98" s="1">
-        <v>450</v>
+        <v>0.045</v>
       </c>
       <c r="S98" s="1">
         <v>0</v>
@@ -16638,6 +16891,9 @@
         <v>0</v>
       </c>
       <c r="AA98" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB98" s="1">
         <v>0</v>
       </c>
       <c r="AC98" s="1">
@@ -16750,7 +17006,7 @@
         <v>0</v>
       </c>
       <c r="P99" s="1">
-        <v>450</v>
+        <v>0.045</v>
       </c>
       <c r="Q99" s="1">
         <v>0</v>
@@ -16783,6 +17039,9 @@
         <v>0</v>
       </c>
       <c r="AA99" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB99" s="1">
         <v>0</v>
       </c>
       <c r="AC99" s="1">
@@ -16886,7 +17145,7 @@
         <v>0</v>
       </c>
       <c r="M100" s="12">
-        <v>450</v>
+        <v>0.045</v>
       </c>
       <c r="N100" s="1">
         <v>0</v>
@@ -16894,6 +17153,9 @@
       <c r="O100" s="1">
         <v>0</v>
       </c>
+      <c r="P100" s="1">
+        <v>0</v>
+      </c>
       <c r="Q100" s="1">
         <v>0</v>
       </c>
@@ -16925,6 +17187,9 @@
         <v>0</v>
       </c>
       <c r="AA100" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB100" s="1">
         <v>0</v>
       </c>
       <c r="AC100" s="1">

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:57a8739 commit_msg:Merge branch 'dev' of https://bitbucket.org/funplus/excel into dev ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -60,10 +60,9 @@
           </rPr>
           <t xml:space="preserve">
 配速度值。
-com条长度为10000格。
-4秒走完则填2500
-act条长度也是10000。
-2秒走完则在技能表里填5000</t>
+com和act程序都是1
+填每秒的进度百分比，比如4秒走完com，就填0.25
+</t>
         </r>
       </text>
     </comment>
@@ -142,7 +141,7 @@
   </si>
   <si>
     <t xml:space="preserve">
-2500格/秒</t>
+每秒进度百分比</t>
   </si>
   <si>
     <t>每秒</t>
@@ -777,8 +776,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -791,38 +835,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -836,25 +850,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -870,31 +868,32 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -907,15 +906,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -959,25 +958,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -995,7 +994,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1007,13 +1006,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,13 +1084,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1049,31 +1114,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1091,55 +1132,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1182,60 +1181,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1259,6 +1204,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1278,16 +1253,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1296,133 +1295,133 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2670,8 +2669,8 @@
   <sheetPr/>
   <dimension ref="A1:AX96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -3281,7 +3280,7 @@
         <v>110</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>110</v>
@@ -3389,7 +3388,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="12">
-        <v>3333</v>
+        <v>0.33</v>
       </c>
       <c r="R7" s="12">
         <v>0</v>
@@ -3539,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="12">
-        <v>3000</v>
+        <v>0.3</v>
       </c>
       <c r="R8" s="12">
         <v>0</v>
@@ -3689,7 +3688,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="12">
-        <v>2500</v>
+        <v>0.25</v>
       </c>
       <c r="R9" s="12">
         <v>0</v>
@@ -3839,7 +3838,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="12">
-        <v>2700</v>
+        <v>0.27</v>
       </c>
       <c r="R10" s="12">
         <v>0</v>
@@ -3989,7 +3988,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="12">
-        <v>3000</v>
+        <v>0.3</v>
       </c>
       <c r="R11" s="12">
         <v>0</v>
@@ -4137,7 +4136,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="12">
-        <v>3000</v>
+        <v>0.3</v>
       </c>
       <c r="R12" s="12">
         <v>0</v>
@@ -4285,7 +4284,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="12">
-        <v>3000</v>
+        <v>0.3</v>
       </c>
       <c r="R13" s="12">
         <v>0</v>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:aede131 commit_msg:Merge branch 'dev' of https://bitbucket.org/funplus/excel into dev ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -88,7 +88,30 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0">
+    <comment ref="D19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+关联globalconfig表英雄升级成长率attid。
+这里填了值的属性才会生效走公式。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="202">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -499,9 +522,6 @@
   </si>
   <si>
     <t>卡牌升级成长率</t>
-  </si>
-  <si>
-    <t>卡牌升级固定值，1级默认值</t>
   </si>
   <si>
     <t>武器升级攻击力固定值</t>
@@ -1454,19 +1474,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2667,10 +2687,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AX96"/>
+  <dimension ref="A1:AX95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -3400,7 +3420,7 @@
         <v>5000</v>
       </c>
       <c r="U7" s="12">
-        <v>6600</v>
+        <v>12000</v>
       </c>
       <c r="V7" s="12">
         <v>0</v>
@@ -3411,16 +3431,16 @@
       <c r="X7" s="12">
         <v>200</v>
       </c>
-      <c r="Y7" s="16">
+      <c r="Y7" s="17">
         <v>1000</v>
       </c>
-      <c r="Z7" s="16">
+      <c r="Z7" s="17">
         <v>10000</v>
       </c>
-      <c r="AA7" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="16">
+      <c r="AA7" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="17">
         <v>10</v>
       </c>
       <c r="AC7" s="12">
@@ -3550,7 +3570,7 @@
         <v>0</v>
       </c>
       <c r="U8" s="12">
-        <v>5500</v>
+        <v>10000</v>
       </c>
       <c r="V8" s="12">
         <v>0</v>
@@ -3561,16 +3581,16 @@
       <c r="X8" s="12">
         <v>200</v>
       </c>
-      <c r="Y8" s="16">
+      <c r="Y8" s="17">
         <v>1000</v>
       </c>
-      <c r="Z8" s="16">
+      <c r="Z8" s="17">
         <v>10000</v>
       </c>
-      <c r="AA8" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="16">
+      <c r="AA8" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="17">
         <v>10</v>
       </c>
       <c r="AC8" s="12">
@@ -3700,7 +3720,7 @@
         <v>0</v>
       </c>
       <c r="U9" s="12">
-        <v>4400</v>
+        <v>8500</v>
       </c>
       <c r="V9" s="12">
         <v>0</v>
@@ -3711,16 +3731,16 @@
       <c r="X9" s="12">
         <v>200</v>
       </c>
-      <c r="Y9" s="16">
+      <c r="Y9" s="17">
         <v>1000</v>
       </c>
-      <c r="Z9" s="16">
+      <c r="Z9" s="17">
         <v>10000</v>
       </c>
-      <c r="AA9" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="16">
+      <c r="AA9" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="17">
         <v>10</v>
       </c>
       <c r="AC9" s="12">
@@ -3753,31 +3773,31 @@
       <c r="AL9" s="12">
         <v>0</v>
       </c>
-      <c r="AM9" s="17" t="s">
+      <c r="AM9" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="AN9" s="17" t="s">
+      <c r="AN9" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="AO9" s="17" t="s">
+      <c r="AO9" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="AP9" s="17" t="s">
+      <c r="AP9" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="AQ9" s="17" t="s">
+      <c r="AQ9" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="AR9" s="17" t="s">
+      <c r="AR9" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="AS9" s="17" t="s">
+      <c r="AS9" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="AT9" s="17" t="s">
+      <c r="AT9" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="AU9" s="17" t="s">
+      <c r="AU9" s="18" t="s">
         <v>115</v>
       </c>
       <c r="AV9" s="12">
@@ -3850,7 +3870,7 @@
         <v>0</v>
       </c>
       <c r="U10" s="12">
-        <v>4400</v>
+        <v>8500</v>
       </c>
       <c r="V10" s="12">
         <v>0</v>
@@ -3861,16 +3881,16 @@
       <c r="X10" s="12">
         <v>200</v>
       </c>
-      <c r="Y10" s="16">
+      <c r="Y10" s="17">
         <v>1000</v>
       </c>
-      <c r="Z10" s="16">
+      <c r="Z10" s="17">
         <v>10000</v>
       </c>
-      <c r="AA10" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="16">
+      <c r="AA10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="17">
         <v>10</v>
       </c>
       <c r="AC10" s="12">
@@ -4000,7 +4020,7 @@
         <v>0</v>
       </c>
       <c r="U11" s="12">
-        <v>3600</v>
+        <v>9000</v>
       </c>
       <c r="V11" s="12">
         <v>0</v>
@@ -4011,16 +4031,16 @@
       <c r="X11" s="12">
         <v>200</v>
       </c>
-      <c r="Y11" s="16">
+      <c r="Y11" s="17">
         <v>1000</v>
       </c>
-      <c r="Z11" s="16">
+      <c r="Z11" s="17">
         <v>10000</v>
       </c>
-      <c r="AA11" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="16">
+      <c r="AA11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="17">
         <v>10</v>
       </c>
       <c r="AC11" s="12">
@@ -4148,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="U12" s="12">
-        <v>3000</v>
+        <v>8500</v>
       </c>
       <c r="V12" s="12">
         <v>0</v>
@@ -4159,16 +4179,16 @@
       <c r="X12" s="12">
         <v>200</v>
       </c>
-      <c r="Y12" s="16">
+      <c r="Y12" s="17">
         <v>1000</v>
       </c>
-      <c r="Z12" s="16">
+      <c r="Z12" s="17">
         <v>10000</v>
       </c>
-      <c r="AA12" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="16">
+      <c r="AA12" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="17">
         <v>10</v>
       </c>
       <c r="AC12" s="12">
@@ -4296,7 +4316,7 @@
         <v>0</v>
       </c>
       <c r="U13" s="12">
-        <v>3600</v>
+        <v>8000</v>
       </c>
       <c r="V13" s="12">
         <v>0</v>
@@ -4307,16 +4327,16 @@
       <c r="X13" s="12">
         <v>200</v>
       </c>
-      <c r="Y13" s="16">
+      <c r="Y13" s="17">
         <v>1000</v>
       </c>
-      <c r="Z13" s="16">
+      <c r="Z13" s="17">
         <v>10000</v>
       </c>
-      <c r="AA13" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="16">
+      <c r="AA13" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="17">
         <v>10</v>
       </c>
       <c r="AC13" s="12">
@@ -4824,11 +4844,11 @@
         <v>0</v>
       </c>
       <c r="AW16" s="10" t="str">
-        <f>AC9:AC20&amp;","&amp;AD9:AD20&amp;","&amp;AE9:AE20&amp;","&amp;AF9:AF20&amp;","&amp;AG9:AG20&amp;","&amp;AH9:AH20&amp;","&amp;AI9:AI20&amp;","&amp;AJ9:AJ20&amp;","&amp;AK9:AK20&amp;","&amp;AL9:AL20</f>
+        <f>AC9:AC19&amp;","&amp;AD9:AD19&amp;","&amp;AE9:AE19&amp;","&amp;AF9:AF19&amp;","&amp;AG9:AG19&amp;","&amp;AH9:AH19&amp;","&amp;AI9:AI19&amp;","&amp;AJ9:AJ19&amp;","&amp;AK9:AK19&amp;","&amp;AL9:AL19</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX16" s="10" t="str">
-        <f>AM9:AM20&amp;","&amp;AN9:AN20&amp;","&amp;AO9:AO20&amp;","&amp;AP9:AP20&amp;","&amp;AQ9:AQ20&amp;","&amp;AR9:AR20&amp;","&amp;AS9:AS20&amp;","&amp;AT9:AT20&amp;","&amp;AU9:AU20&amp;","&amp;AV9:AV20</f>
+        <f>AM9:AM19&amp;","&amp;AN9:AN19&amp;","&amp;AO9:AO19&amp;","&amp;AP9:AP19&amp;","&amp;AQ9:AQ19&amp;","&amp;AR9:AR19&amp;","&amp;AS9:AS19&amp;","&amp;AT9:AT19&amp;","&amp;AU9:AU19&amp;","&amp;AV9:AV19</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
@@ -4972,11 +4992,11 @@
         <v>0</v>
       </c>
       <c r="AW17" s="10" t="str">
-        <f>AC10:AC20&amp;","&amp;AD10:AD20&amp;","&amp;AE10:AE20&amp;","&amp;AF10:AF20&amp;","&amp;AG10:AG20&amp;","&amp;AH10:AH20&amp;","&amp;AI10:AI20&amp;","&amp;AJ10:AJ20&amp;","&amp;AK10:AK20&amp;","&amp;AL10:AL20</f>
+        <f>AC10:AC19&amp;","&amp;AD10:AD19&amp;","&amp;AE10:AE19&amp;","&amp;AF10:AF19&amp;","&amp;AG10:AG19&amp;","&amp;AH10:AH19&amp;","&amp;AI10:AI19&amp;","&amp;AJ10:AJ19&amp;","&amp;AK10:AK19&amp;","&amp;AL10:AL19</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX17" s="10" t="str">
-        <f>AM10:AM20&amp;","&amp;AN10:AN20&amp;","&amp;AO10:AO20&amp;","&amp;AP10:AP20&amp;","&amp;AQ10:AQ20&amp;","&amp;AR10:AR20&amp;","&amp;AS10:AS20&amp;","&amp;AT10:AT20&amp;","&amp;AU10:AU20&amp;","&amp;AV10:AV20</f>
+        <f>AM10:AM19&amp;","&amp;AN10:AN19&amp;","&amp;AO10:AO19&amp;","&amp;AP10:AP19&amp;","&amp;AQ10:AQ19&amp;","&amp;AR10:AR19&amp;","&amp;AS10:AS19&amp;","&amp;AT10:AT19&amp;","&amp;AU10:AU19&amp;","&amp;AV10:AV19</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
@@ -5120,11 +5140,11 @@
         <v>0</v>
       </c>
       <c r="AW18" s="10" t="str">
-        <f>AC11:AC21&amp;","&amp;AD11:AD21&amp;","&amp;AE11:AE21&amp;","&amp;AF11:AF21&amp;","&amp;AG11:AG21&amp;","&amp;AH11:AH21&amp;","&amp;AI11:AI21&amp;","&amp;AJ11:AJ21&amp;","&amp;AK11:AK21&amp;","&amp;AL11:AL21</f>
+        <f>AC11:AC20&amp;","&amp;AD11:AD20&amp;","&amp;AE11:AE20&amp;","&amp;AF11:AF20&amp;","&amp;AG11:AG20&amp;","&amp;AH11:AH20&amp;","&amp;AI11:AI20&amp;","&amp;AJ11:AJ20&amp;","&amp;AK11:AK20&amp;","&amp;AL11:AL20</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX18" s="10" t="str">
-        <f>AM11:AM21&amp;","&amp;AN11:AN21&amp;","&amp;AO11:AO21&amp;","&amp;AP11:AP21&amp;","&amp;AQ11:AQ21&amp;","&amp;AR11:AR21&amp;","&amp;AS11:AS21&amp;","&amp;AT11:AT21&amp;","&amp;AU11:AU21&amp;","&amp;AV11:AV21</f>
+        <f>AM11:AM20&amp;","&amp;AN11:AN20&amp;","&amp;AO11:AO20&amp;","&amp;AP11:AP20&amp;","&amp;AQ11:AQ20&amp;","&amp;AR11:AR20&amp;","&amp;AS11:AS20&amp;","&amp;AT11:AT20&amp;","&amp;AU11:AU20&amp;","&amp;AV11:AV20</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
@@ -5184,13 +5204,13 @@
         <v>0</v>
       </c>
       <c r="U19" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="V19" s="1">
         <v>0</v>
       </c>
       <c r="W19" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="X19" s="1">
         <v>0</v>
@@ -5268,17 +5288,17 @@
         <v>0</v>
       </c>
       <c r="AW19" s="10" t="str">
-        <f>AC12:AC21&amp;","&amp;AD12:AD21&amp;","&amp;AE12:AE21&amp;","&amp;AF12:AF21&amp;","&amp;AG12:AG21&amp;","&amp;AH12:AH21&amp;","&amp;AI12:AI21&amp;","&amp;AJ12:AJ21&amp;","&amp;AK12:AK21&amp;","&amp;AL12:AL21</f>
+        <f>AC12:AC20&amp;","&amp;AD12:AD20&amp;","&amp;AE12:AE20&amp;","&amp;AF12:AF20&amp;","&amp;AG12:AG20&amp;","&amp;AH12:AH20&amp;","&amp;AI12:AI20&amp;","&amp;AJ12:AJ20&amp;","&amp;AK12:AK20&amp;","&amp;AL12:AL20</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX19" s="10" t="str">
-        <f>AM12:AM21&amp;","&amp;AN12:AN21&amp;","&amp;AO12:AO21&amp;","&amp;AP12:AP21&amp;","&amp;AQ12:AQ21&amp;","&amp;AR12:AR21&amp;","&amp;AS12:AS21&amp;","&amp;AT12:AT21&amp;","&amp;AU12:AU21&amp;","&amp;AV12:AV21</f>
+        <f>AM12:AM20&amp;","&amp;AN12:AN20&amp;","&amp;AO12:AO20&amp;","&amp;AP12:AP20&amp;","&amp;AQ12:AQ20&amp;","&amp;AR12:AR20&amp;","&amp;AS12:AS20&amp;","&amp;AT12:AT20&amp;","&amp;AU12:AU20&amp;","&amp;AV12:AV20</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="3:50">
       <c r="C20" s="1">
-        <v>21</v>
+        <v>2000</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>126</v>
@@ -5286,23 +5306,23 @@
       <c r="E20" s="1">
         <v>50</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="11">
         <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>30</v>
-      </c>
-      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="12">
         <v>0</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
       </c>
       <c r="J20" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="K20" s="1">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
@@ -5314,37 +5334,37 @@
         <v>0</v>
       </c>
       <c r="O20" s="1">
-        <v>10</v>
-      </c>
-      <c r="P20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="12">
         <v>0</v>
       </c>
       <c r="Q20" s="1">
         <v>0</v>
       </c>
-      <c r="R20" s="1">
+      <c r="R20" s="12">
         <v>0</v>
       </c>
       <c r="S20" s="1">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>
       </c>
       <c r="U20" s="1">
-        <v>500</v>
-      </c>
-      <c r="V20" s="1">
+        <v>0</v>
+      </c>
+      <c r="V20" s="12">
         <v>0</v>
       </c>
       <c r="W20" s="1">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="X20" s="1">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="Z20" s="1">
         <v>0</v>
@@ -5416,31 +5436,31 @@
         <v>0</v>
       </c>
       <c r="AW20" s="10" t="str">
-        <f>AC14:AC21&amp;","&amp;AD14:AD21&amp;","&amp;AE14:AE21&amp;","&amp;AF14:AF21&amp;","&amp;AG14:AG21&amp;","&amp;AH14:AH21&amp;","&amp;AI14:AI21&amp;","&amp;AJ14:AJ21&amp;","&amp;AK14:AK21&amp;","&amp;AL14:AL21</f>
+        <f>AC16:AC21&amp;","&amp;AD16:AD21&amp;","&amp;AE16:AE21&amp;","&amp;AF16:AF21&amp;","&amp;AG16:AG21&amp;","&amp;AH16:AH21&amp;","&amp;AI16:AI21&amp;","&amp;AJ16:AJ21&amp;","&amp;AK16:AK21&amp;","&amp;AL16:AL21</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX20" s="10" t="str">
-        <f>AM14:AM21&amp;","&amp;AN14:AN21&amp;","&amp;AO14:AO21&amp;","&amp;AP14:AP21&amp;","&amp;AQ14:AQ21&amp;","&amp;AR14:AR21&amp;","&amp;AS14:AS21&amp;","&amp;AT14:AT21&amp;","&amp;AU14:AU21&amp;","&amp;AV14:AV21</f>
+        <f>AM16:AM21&amp;","&amp;AN16:AN21&amp;","&amp;AO16:AO21&amp;","&amp;AP16:AP21&amp;","&amp;AQ16:AQ21&amp;","&amp;AR16:AR21&amp;","&amp;AS16:AS21&amp;","&amp;AT16:AT21&amp;","&amp;AU16:AU21&amp;","&amp;AV16:AV21</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="3:50">
       <c r="C21" s="1">
-        <v>2000</v>
-      </c>
-      <c r="D21" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>127</v>
       </c>
       <c r="E21" s="1">
-        <v>50</v>
-      </c>
-      <c r="F21" s="11">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21" s="1">
@@ -5455,7 +5475,7 @@
       <c r="L21" s="1">
         <v>0</v>
       </c>
-      <c r="M21" s="12">
+      <c r="M21" s="1">
         <v>0</v>
       </c>
       <c r="N21" s="1">
@@ -5464,13 +5484,13 @@
       <c r="O21" s="1">
         <v>0</v>
       </c>
-      <c r="P21" s="12">
+      <c r="P21" s="1">
         <v>0</v>
       </c>
       <c r="Q21" s="1">
         <v>0</v>
       </c>
-      <c r="R21" s="12">
+      <c r="R21" s="1">
         <v>0</v>
       </c>
       <c r="S21" s="1">
@@ -5482,7 +5502,7 @@
       <c r="U21" s="1">
         <v>0</v>
       </c>
-      <c r="V21" s="12">
+      <c r="V21" s="1">
         <v>0</v>
       </c>
       <c r="W21" s="1">
@@ -5564,31 +5584,31 @@
         <v>0</v>
       </c>
       <c r="AW21" s="10" t="str">
-        <f>AC16:AC22&amp;","&amp;AD16:AD22&amp;","&amp;AE16:AE22&amp;","&amp;AF16:AF22&amp;","&amp;AG16:AG22&amp;","&amp;AH16:AH22&amp;","&amp;AI16:AI22&amp;","&amp;AJ16:AJ22&amp;","&amp;AK16:AK22&amp;","&amp;AL16:AL22</f>
+        <f>AC20:AC25&amp;","&amp;AD20:AD25&amp;","&amp;AE20:AE25&amp;","&amp;AF20:AF25&amp;","&amp;AG20:AG25&amp;","&amp;AH20:AH25&amp;","&amp;AI20:AI25&amp;","&amp;AJ20:AJ25&amp;","&amp;AK20:AK25&amp;","&amp;AL20:AL25</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX21" s="10" t="str">
-        <f>AM16:AM22&amp;","&amp;AN16:AN22&amp;","&amp;AO16:AO22&amp;","&amp;AP16:AP22&amp;","&amp;AQ16:AQ22&amp;","&amp;AR16:AR22&amp;","&amp;AS16:AS22&amp;","&amp;AT16:AT22&amp;","&amp;AU16:AU22&amp;","&amp;AV16:AV22</f>
+        <f>AM20:AM25&amp;","&amp;AN20:AN25&amp;","&amp;AO20:AO25&amp;","&amp;AP20:AP25&amp;","&amp;AQ20:AQ25&amp;","&amp;AR20:AR25&amp;","&amp;AS20:AS25&amp;","&amp;AT20:AT25&amp;","&amp;AU20:AU25&amp;","&amp;AV20:AV25</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="3:50">
       <c r="C22" s="1">
-        <v>2001</v>
-      </c>
-      <c r="D22" s="14" t="s">
+        <v>2010</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E22" s="1">
-        <v>10</v>
-      </c>
-      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
         <v>0</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="12">
         <v>0</v>
       </c>
       <c r="I22" s="1">
@@ -5603,7 +5623,7 @@
       <c r="L22" s="1">
         <v>0</v>
       </c>
-      <c r="M22" s="1">
+      <c r="M22" s="12">
         <v>0</v>
       </c>
       <c r="N22" s="1">
@@ -5612,13 +5632,13 @@
       <c r="O22" s="1">
         <v>0</v>
       </c>
-      <c r="P22" s="1">
+      <c r="P22" s="12">
         <v>0</v>
       </c>
       <c r="Q22" s="1">
         <v>0</v>
       </c>
-      <c r="R22" s="1">
+      <c r="R22" s="12">
         <v>0</v>
       </c>
       <c r="S22" s="1">
@@ -5630,7 +5650,7 @@
       <c r="U22" s="1">
         <v>0</v>
       </c>
-      <c r="V22" s="1">
+      <c r="V22" s="12">
         <v>0</v>
       </c>
       <c r="W22" s="1">
@@ -5652,7 +5672,7 @@
         <v>0</v>
       </c>
       <c r="AC22" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AD22" s="1">
         <v>0</v>
@@ -5713,7 +5733,7 @@
       </c>
       <c r="AW22" s="10" t="str">
         <f>AC20:AC26&amp;","&amp;AD20:AD26&amp;","&amp;AE20:AE26&amp;","&amp;AF20:AF26&amp;","&amp;AG20:AG26&amp;","&amp;AH20:AH26&amp;","&amp;AI20:AI26&amp;","&amp;AJ20:AJ26&amp;","&amp;AK20:AK26&amp;","&amp;AL20:AL26</f>
-        <v>0,0,0,0,0,0,0,0,0,0</v>
+        <v>0.05,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX22" s="10" t="str">
         <f>AM20:AM26&amp;","&amp;AN20:AN26&amp;","&amp;AO20:AO26&amp;","&amp;AP20:AP26&amp;","&amp;AQ20:AQ26&amp;","&amp;AR20:AR26&amp;","&amp;AS20:AS26&amp;","&amp;AT20:AT26&amp;","&amp;AU20:AU26&amp;","&amp;AV20:AV26</f>
@@ -5722,7 +5742,7 @@
     </row>
     <row r="23" customHeight="1" spans="3:50">
       <c r="C23" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>129</v>
@@ -5800,7 +5820,7 @@
         <v>0</v>
       </c>
       <c r="AC23" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="AD23" s="1">
         <v>0</v>
@@ -5860,17 +5880,17 @@
         <v>0</v>
       </c>
       <c r="AW23" s="10" t="str">
-        <f>AC21:AC27&amp;","&amp;AD21:AD27&amp;","&amp;AE21:AE27&amp;","&amp;AF21:AF27&amp;","&amp;AG21:AG27&amp;","&amp;AH21:AH27&amp;","&amp;AI21:AI27&amp;","&amp;AJ21:AJ27&amp;","&amp;AK21:AK27&amp;","&amp;AL21:AL27</f>
-        <v>0.05,0,0,0,0,0,0,0,0,0</v>
+        <f>AC20:AC27&amp;","&amp;AD20:AD27&amp;","&amp;AE20:AE27&amp;","&amp;AF20:AF27&amp;","&amp;AG20:AG27&amp;","&amp;AH20:AH27&amp;","&amp;AI20:AI27&amp;","&amp;AJ20:AJ27&amp;","&amp;AK20:AK27&amp;","&amp;AL20:AL27</f>
+        <v>0.1,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX23" s="10" t="str">
-        <f>AM21:AM27&amp;","&amp;AN21:AN27&amp;","&amp;AO21:AO27&amp;","&amp;AP21:AP27&amp;","&amp;AQ21:AQ27&amp;","&amp;AR21:AR27&amp;","&amp;AS21:AS27&amp;","&amp;AT21:AT27&amp;","&amp;AU21:AU27&amp;","&amp;AV21:AV27</f>
+        <f>AM20:AM27&amp;","&amp;AN20:AN27&amp;","&amp;AO20:AO27&amp;","&amp;AP20:AP27&amp;","&amp;AQ20:AQ27&amp;","&amp;AR20:AR27&amp;","&amp;AS20:AS27&amp;","&amp;AT20:AT27&amp;","&amp;AU20:AU27&amp;","&amp;AV20:AV27</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="3:50">
       <c r="C24" s="1">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>130</v>
@@ -5948,7 +5968,7 @@
         <v>0</v>
       </c>
       <c r="AC24" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="AD24" s="1">
         <v>0</v>
@@ -6009,7 +6029,7 @@
       </c>
       <c r="AW24" s="10" t="str">
         <f>AC21:AC28&amp;","&amp;AD21:AD28&amp;","&amp;AE21:AE28&amp;","&amp;AF21:AF28&amp;","&amp;AG21:AG28&amp;","&amp;AH21:AH28&amp;","&amp;AI21:AI28&amp;","&amp;AJ21:AJ28&amp;","&amp;AK21:AK28&amp;","&amp;AL21:AL28</f>
-        <v>0.1,0,0,0,0,0,0,0,0,0</v>
+        <v>0.15,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX24" s="10" t="str">
         <f>AM21:AM28&amp;","&amp;AN21:AN28&amp;","&amp;AO21:AO28&amp;","&amp;AP21:AP28&amp;","&amp;AQ21:AQ28&amp;","&amp;AR21:AR28&amp;","&amp;AS21:AS28&amp;","&amp;AT21:AT28&amp;","&amp;AU21:AU28&amp;","&amp;AV21:AV28</f>
@@ -6018,7 +6038,7 @@
     </row>
     <row r="25" customHeight="1" spans="3:50">
       <c r="C25" s="1">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>131</v>
@@ -6096,7 +6116,7 @@
         <v>0</v>
       </c>
       <c r="AC25" s="1">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="AD25" s="1">
         <v>0</v>
@@ -6156,17 +6176,17 @@
         <v>0</v>
       </c>
       <c r="AW25" s="10" t="str">
-        <f>AC22:AC29&amp;","&amp;AD22:AD29&amp;","&amp;AE22:AE29&amp;","&amp;AF22:AF29&amp;","&amp;AG22:AG29&amp;","&amp;AH22:AH29&amp;","&amp;AI22:AI29&amp;","&amp;AJ22:AJ29&amp;","&amp;AK22:AK29&amp;","&amp;AL22:AL29</f>
-        <v>0.15,0,0,0,0,0,0,0,0,0</v>
+        <f>AC21:AC29&amp;","&amp;AD21:AD29&amp;","&amp;AE21:AE29&amp;","&amp;AF21:AF29&amp;","&amp;AG21:AG29&amp;","&amp;AH21:AH29&amp;","&amp;AI21:AI29&amp;","&amp;AJ21:AJ29&amp;","&amp;AK21:AK29&amp;","&amp;AL21:AL29</f>
+        <v>0.2,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX25" s="10" t="str">
-        <f>AM22:AM29&amp;","&amp;AN22:AN29&amp;","&amp;AO22:AO29&amp;","&amp;AP22:AP29&amp;","&amp;AQ22:AQ29&amp;","&amp;AR22:AR29&amp;","&amp;AS22:AS29&amp;","&amp;AT22:AT29&amp;","&amp;AU22:AU29&amp;","&amp;AV22:AV29</f>
+        <f>AM21:AM29&amp;","&amp;AN21:AN29&amp;","&amp;AO21:AO29&amp;","&amp;AP21:AP29&amp;","&amp;AQ21:AQ29&amp;","&amp;AR21:AR29&amp;","&amp;AS21:AS29&amp;","&amp;AT21:AT29&amp;","&amp;AU21:AU29&amp;","&amp;AV21:AV29</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="3:50">
       <c r="C26" s="1">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>132</v>
@@ -6244,7 +6264,7 @@
         <v>0</v>
       </c>
       <c r="AC26" s="1">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="AD26" s="1">
         <v>0</v>
@@ -6304,17 +6324,17 @@
         <v>0</v>
       </c>
       <c r="AW26" s="10" t="str">
-        <f>AC22:AC30&amp;","&amp;AD22:AD30&amp;","&amp;AE22:AE30&amp;","&amp;AF22:AF30&amp;","&amp;AG22:AG30&amp;","&amp;AH22:AH30&amp;","&amp;AI22:AI30&amp;","&amp;AJ22:AJ30&amp;","&amp;AK22:AK30&amp;","&amp;AL22:AL30</f>
-        <v>0.2,0,0,0,0,0,0,0,0,0</v>
+        <f>AC21:AC30&amp;","&amp;AD21:AD30&amp;","&amp;AE21:AE30&amp;","&amp;AF21:AF30&amp;","&amp;AG21:AG30&amp;","&amp;AH21:AH30&amp;","&amp;AI21:AI30&amp;","&amp;AJ21:AJ30&amp;","&amp;AK21:AK30&amp;","&amp;AL21:AL30</f>
+        <v>0.25,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX26" s="10" t="str">
-        <f>AM22:AM30&amp;","&amp;AN22:AN30&amp;","&amp;AO22:AO30&amp;","&amp;AP22:AP30&amp;","&amp;AQ22:AQ30&amp;","&amp;AR22:AR30&amp;","&amp;AS22:AS30&amp;","&amp;AT22:AT30&amp;","&amp;AU22:AU30&amp;","&amp;AV22:AV30</f>
+        <f>AM21:AM30&amp;","&amp;AN21:AN30&amp;","&amp;AO21:AO30&amp;","&amp;AP21:AP30&amp;","&amp;AQ21:AQ30&amp;","&amp;AR21:AR30&amp;","&amp;AS21:AS30&amp;","&amp;AT21:AT30&amp;","&amp;AU21:AU30&amp;","&amp;AV21:AV30</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="3:50">
       <c r="C27" s="1">
-        <v>2014</v>
+        <v>2020</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>133</v>
@@ -6374,7 +6394,7 @@
         <v>0</v>
       </c>
       <c r="W27" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="X27" s="1">
         <v>0</v>
@@ -6392,7 +6412,7 @@
         <v>0</v>
       </c>
       <c r="AC27" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AD27" s="1">
         <v>0</v>
@@ -6452,17 +6472,17 @@
         <v>0</v>
       </c>
       <c r="AW27" s="10" t="str">
-        <f>AC22:AC31&amp;","&amp;AD22:AD31&amp;","&amp;AE22:AE31&amp;","&amp;AF22:AF31&amp;","&amp;AG22:AG31&amp;","&amp;AH22:AH31&amp;","&amp;AI22:AI31&amp;","&amp;AJ22:AJ31&amp;","&amp;AK22:AK31&amp;","&amp;AL22:AL31</f>
-        <v>0.25,0,0,0,0,0,0,0,0,0</v>
+        <f>AC21:AC31&amp;","&amp;AD21:AD31&amp;","&amp;AE21:AE31&amp;","&amp;AF21:AF31&amp;","&amp;AG21:AG31&amp;","&amp;AH21:AH31&amp;","&amp;AI21:AI31&amp;","&amp;AJ21:AJ31&amp;","&amp;AK21:AK31&amp;","&amp;AL21:AL31</f>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX27" s="10" t="str">
-        <f>AM22:AM31&amp;","&amp;AN22:AN31&amp;","&amp;AO22:AO31&amp;","&amp;AP22:AP31&amp;","&amp;AQ22:AQ31&amp;","&amp;AR22:AR31&amp;","&amp;AS22:AS31&amp;","&amp;AT22:AT31&amp;","&amp;AU22:AU31&amp;","&amp;AV22:AV31</f>
+        <f>AM21:AM31&amp;","&amp;AN21:AN31&amp;","&amp;AO21:AO31&amp;","&amp;AP21:AP31&amp;","&amp;AQ21:AQ31&amp;","&amp;AR21:AR31&amp;","&amp;AS21:AS31&amp;","&amp;AT21:AT31&amp;","&amp;AU21:AU31&amp;","&amp;AV21:AV31</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="3:50">
       <c r="C28" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>134</v>
@@ -6522,7 +6542,7 @@
         <v>0</v>
       </c>
       <c r="W28" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="X28" s="1">
         <v>0</v>
@@ -6600,17 +6620,17 @@
         <v>0</v>
       </c>
       <c r="AW28" s="10" t="str">
-        <f>AC22:AC32&amp;","&amp;AD22:AD32&amp;","&amp;AE22:AE32&amp;","&amp;AF22:AF32&amp;","&amp;AG22:AG32&amp;","&amp;AH22:AH32&amp;","&amp;AI22:AI32&amp;","&amp;AJ22:AJ32&amp;","&amp;AK22:AK32&amp;","&amp;AL22:AL32</f>
+        <f>AC22:AC31&amp;","&amp;AD22:AD31&amp;","&amp;AE22:AE31&amp;","&amp;AF22:AF31&amp;","&amp;AG22:AG31&amp;","&amp;AH22:AH31&amp;","&amp;AI22:AI31&amp;","&amp;AJ22:AJ31&amp;","&amp;AK22:AK31&amp;","&amp;AL22:AL31</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX28" s="10" t="str">
-        <f>AM22:AM32&amp;","&amp;AN22:AN32&amp;","&amp;AO22:AO32&amp;","&amp;AP22:AP32&amp;","&amp;AQ22:AQ32&amp;","&amp;AR22:AR32&amp;","&amp;AS22:AS32&amp;","&amp;AT22:AT32&amp;","&amp;AU22:AU32&amp;","&amp;AV22:AV32</f>
+        <f>AM22:AM31&amp;","&amp;AN22:AN31&amp;","&amp;AO22:AO31&amp;","&amp;AP22:AP31&amp;","&amp;AQ22:AQ31&amp;","&amp;AR22:AR31&amp;","&amp;AS22:AS31&amp;","&amp;AT22:AT31&amp;","&amp;AU22:AU31&amp;","&amp;AV22:AV31</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="3:50">
       <c r="C29" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>135</v>
@@ -6670,7 +6690,7 @@
         <v>0</v>
       </c>
       <c r="W29" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="X29" s="1">
         <v>0</v>
@@ -6748,17 +6768,17 @@
         <v>0</v>
       </c>
       <c r="AW29" s="10" t="str">
-        <f>AC23:AC32&amp;","&amp;AD23:AD32&amp;","&amp;AE23:AE32&amp;","&amp;AF23:AF32&amp;","&amp;AG23:AG32&amp;","&amp;AH23:AH32&amp;","&amp;AI23:AI32&amp;","&amp;AJ23:AJ32&amp;","&amp;AK23:AK32&amp;","&amp;AL23:AL32</f>
+        <f>AC23:AC31&amp;","&amp;AD23:AD31&amp;","&amp;AE23:AE31&amp;","&amp;AF23:AF31&amp;","&amp;AG23:AG31&amp;","&amp;AH23:AH31&amp;","&amp;AI23:AI31&amp;","&amp;AJ23:AJ31&amp;","&amp;AK23:AK31&amp;","&amp;AL23:AL31</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX29" s="10" t="str">
-        <f>AM23:AM32&amp;","&amp;AN23:AN32&amp;","&amp;AO23:AO32&amp;","&amp;AP23:AP32&amp;","&amp;AQ23:AQ32&amp;","&amp;AR23:AR32&amp;","&amp;AS23:AS32&amp;","&amp;AT23:AT32&amp;","&amp;AU23:AU32&amp;","&amp;AV23:AV32</f>
+        <f>AM23:AM31&amp;","&amp;AN23:AN31&amp;","&amp;AO23:AO31&amp;","&amp;AP23:AP31&amp;","&amp;AQ23:AQ31&amp;","&amp;AR23:AR31&amp;","&amp;AS23:AS31&amp;","&amp;AT23:AT31&amp;","&amp;AU23:AU31&amp;","&amp;AV23:AV31</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="3:50">
       <c r="C30" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>136</v>
@@ -6818,7 +6838,7 @@
         <v>0</v>
       </c>
       <c r="W30" s="1">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="X30" s="1">
         <v>0</v>
@@ -6906,7 +6926,7 @@
     </row>
     <row r="31" customHeight="1" spans="3:50">
       <c r="C31" s="1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>137</v>
@@ -6966,7 +6986,7 @@
         <v>0</v>
       </c>
       <c r="W31" s="1">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="X31" s="1">
         <v>0</v>
@@ -7054,21 +7074,21 @@
     </row>
     <row r="32" customHeight="1" spans="3:50">
       <c r="C32" s="1">
-        <v>2024</v>
+        <v>3000</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E32" s="1">
-        <v>0</v>
-      </c>
-      <c r="F32" s="11">
+        <v>6</v>
+      </c>
+      <c r="F32" s="1">
         <v>0</v>
       </c>
       <c r="G32" s="1">
         <v>0</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="1">
         <v>0</v>
       </c>
       <c r="I32" s="1">
@@ -7092,13 +7112,13 @@
       <c r="O32" s="1">
         <v>0</v>
       </c>
-      <c r="P32" s="12">
+      <c r="P32" s="1">
         <v>0</v>
       </c>
       <c r="Q32" s="1">
         <v>0</v>
       </c>
-      <c r="R32" s="12">
+      <c r="R32" s="1">
         <v>0</v>
       </c>
       <c r="S32" s="1">
@@ -7110,11 +7130,11 @@
       <c r="U32" s="1">
         <v>0</v>
       </c>
-      <c r="V32" s="12">
+      <c r="V32" s="1">
         <v>0</v>
       </c>
       <c r="W32" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="X32" s="1">
         <v>0</v>
@@ -7192,23 +7212,23 @@
         <v>0</v>
       </c>
       <c r="AW32" s="10" t="str">
-        <f>AC26:AC34&amp;","&amp;AD26:AD34&amp;","&amp;AE26:AE34&amp;","&amp;AF26:AF34&amp;","&amp;AG26:AG34&amp;","&amp;AH26:AH34&amp;","&amp;AI26:AI34&amp;","&amp;AJ26:AJ34&amp;","&amp;AK26:AK34&amp;","&amp;AL26:AL34</f>
+        <f>AC28:AC36&amp;","&amp;AD28:AD36&amp;","&amp;AE28:AE36&amp;","&amp;AF28:AF36&amp;","&amp;AG28:AG36&amp;","&amp;AH28:AH36&amp;","&amp;AI28:AI36&amp;","&amp;AJ28:AJ36&amp;","&amp;AK28:AK36&amp;","&amp;AL28:AL36</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX32" s="10" t="str">
-        <f>AM26:AM34&amp;","&amp;AN26:AN34&amp;","&amp;AO26:AO34&amp;","&amp;AP26:AP34&amp;","&amp;AQ26:AQ34&amp;","&amp;AR26:AR34&amp;","&amp;AS26:AS34&amp;","&amp;AT26:AT34&amp;","&amp;AU26:AU34&amp;","&amp;AV26:AV34</f>
+        <f>AM28:AM36&amp;","&amp;AN28:AN36&amp;","&amp;AO28:AO36&amp;","&amp;AP28:AP36&amp;","&amp;AQ28:AQ36&amp;","&amp;AR28:AR36&amp;","&amp;AS28:AS36&amp;","&amp;AT28:AT36&amp;","&amp;AU28:AU36&amp;","&amp;AV28:AV36</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="3:50">
       <c r="C33" s="1">
-        <v>3000</v>
+        <v>3001</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E33" s="1">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
@@ -7350,7 +7370,7 @@
     </row>
     <row r="34" customHeight="1" spans="3:50">
       <c r="C34" s="1">
-        <v>3001</v>
+        <v>3010</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>140</v>
@@ -7498,13 +7518,13 @@
     </row>
     <row r="35" customHeight="1" spans="3:50">
       <c r="C35" s="1">
-        <v>3010</v>
+        <v>3011</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>141</v>
       </c>
       <c r="E35" s="1">
-        <v>60</v>
+        <v>600</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -7646,13 +7666,13 @@
     </row>
     <row r="36" customHeight="1" spans="3:50">
       <c r="C36" s="1">
-        <v>3011</v>
+        <v>3020</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>142</v>
       </c>
       <c r="E36" s="1">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
@@ -7794,13 +7814,13 @@
     </row>
     <row r="37" customHeight="1" spans="3:50">
       <c r="C37" s="1">
-        <v>3020</v>
+        <v>3021</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E37" s="1">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -7932,23 +7952,23 @@
         <v>0</v>
       </c>
       <c r="AW37" s="10" t="str">
-        <f>AC33:AC41&amp;","&amp;AD33:AD41&amp;","&amp;AE33:AE41&amp;","&amp;AF33:AF41&amp;","&amp;AG33:AG41&amp;","&amp;AH33:AH41&amp;","&amp;AI33:AI41&amp;","&amp;AJ33:AJ41&amp;","&amp;AK33:AK41&amp;","&amp;AL33:AL41</f>
+        <f>AC32:AC41&amp;","&amp;AD32:AD41&amp;","&amp;AE32:AE41&amp;","&amp;AF32:AF41&amp;","&amp;AG32:AG41&amp;","&amp;AH32:AH41&amp;","&amp;AI32:AI41&amp;","&amp;AJ32:AJ41&amp;","&amp;AK32:AK41&amp;","&amp;AL32:AL41</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX37" s="10" t="str">
-        <f>AM33:AM41&amp;","&amp;AN33:AN41&amp;","&amp;AO33:AO41&amp;","&amp;AP33:AP41&amp;","&amp;AQ33:AQ41&amp;","&amp;AR33:AR41&amp;","&amp;AS33:AS41&amp;","&amp;AT33:AT41&amp;","&amp;AU33:AU41&amp;","&amp;AV33:AV41</f>
+        <f>AM32:AM41&amp;","&amp;AN32:AN41&amp;","&amp;AO32:AO41&amp;","&amp;AP32:AP41&amp;","&amp;AQ32:AQ41&amp;","&amp;AR32:AR41&amp;","&amp;AS32:AS41&amp;","&amp;AT32:AT41&amp;","&amp;AU32:AU41&amp;","&amp;AV32:AV41</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="38" customHeight="1" spans="3:50">
       <c r="C38" s="1">
-        <v>3021</v>
+        <v>3030</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E38" s="1">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
@@ -7987,7 +8007,7 @@
         <v>0</v>
       </c>
       <c r="R38" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="S38" s="1">
         <v>0</v>
@@ -8080,17 +8100,17 @@
         <v>0</v>
       </c>
       <c r="AW38" s="10" t="str">
-        <f>AC33:AC42&amp;","&amp;AD33:AD42&amp;","&amp;AE33:AE42&amp;","&amp;AF33:AF42&amp;","&amp;AG33:AG42&amp;","&amp;AH33:AH42&amp;","&amp;AI33:AI42&amp;","&amp;AJ33:AJ42&amp;","&amp;AK33:AK42&amp;","&amp;AL33:AL42</f>
+        <f>AC32:AC42&amp;","&amp;AD32:AD42&amp;","&amp;AE32:AE42&amp;","&amp;AF32:AF42&amp;","&amp;AG32:AG42&amp;","&amp;AH32:AH42&amp;","&amp;AI32:AI42&amp;","&amp;AJ32:AJ42&amp;","&amp;AK32:AK42&amp;","&amp;AL32:AL42</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX38" s="10" t="str">
-        <f>AM33:AM42&amp;","&amp;AN33:AN42&amp;","&amp;AO33:AO42&amp;","&amp;AP33:AP42&amp;","&amp;AQ33:AQ42&amp;","&amp;AR33:AR42&amp;","&amp;AS33:AS42&amp;","&amp;AT33:AT42&amp;","&amp;AU33:AU42&amp;","&amp;AV33:AV42</f>
+        <f>AM32:AM42&amp;","&amp;AN32:AN42&amp;","&amp;AO32:AO42&amp;","&amp;AP32:AP42&amp;","&amp;AQ32:AQ42&amp;","&amp;AR32:AR42&amp;","&amp;AS32:AS42&amp;","&amp;AT32:AT42&amp;","&amp;AU32:AU42&amp;","&amp;AV32:AV42</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="39" customHeight="1" spans="3:50">
       <c r="C39" s="1">
-        <v>3030</v>
+        <v>3031</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>145</v>
@@ -8135,7 +8155,7 @@
         <v>0</v>
       </c>
       <c r="R39" s="1">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="S39" s="1">
         <v>0</v>
@@ -8238,7 +8258,7 @@
     </row>
     <row r="40" customHeight="1" spans="3:50">
       <c r="C40" s="1">
-        <v>3031</v>
+        <v>3032</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>146</v>
@@ -8277,13 +8297,13 @@
         <v>0</v>
       </c>
       <c r="P40" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="Q40" s="1">
         <v>0</v>
       </c>
       <c r="R40" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="S40" s="1">
         <v>0</v>
@@ -8376,17 +8396,17 @@
         <v>0</v>
       </c>
       <c r="AW40" s="10" t="str">
-        <f>AC34:AC44&amp;","&amp;AD34:AD44&amp;","&amp;AE34:AE44&amp;","&amp;AF34:AF44&amp;","&amp;AG34:AG44&amp;","&amp;AH34:AH44&amp;","&amp;AI34:AI44&amp;","&amp;AJ34:AJ44&amp;","&amp;AK34:AK44&amp;","&amp;AL34:AL44</f>
+        <f t="shared" ref="AW40:AW45" si="2">AC34:AC46&amp;","&amp;AD34:AD46&amp;","&amp;AE34:AE46&amp;","&amp;AF34:AF46&amp;","&amp;AG34:AG46&amp;","&amp;AH34:AH46&amp;","&amp;AI34:AI46&amp;","&amp;AJ34:AJ46&amp;","&amp;AK34:AK46&amp;","&amp;AL34:AL46</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX40" s="10" t="str">
-        <f>AM34:AM44&amp;","&amp;AN34:AN44&amp;","&amp;AO34:AO44&amp;","&amp;AP34:AP44&amp;","&amp;AQ34:AQ44&amp;","&amp;AR34:AR44&amp;","&amp;AS34:AS44&amp;","&amp;AT34:AT44&amp;","&amp;AU34:AU44&amp;","&amp;AV34:AV44</f>
+        <f t="shared" ref="AX40:AX45" si="3">AM34:AM46&amp;","&amp;AN34:AN46&amp;","&amp;AO34:AO46&amp;","&amp;AP34:AP46&amp;","&amp;AQ34:AQ46&amp;","&amp;AR34:AR46&amp;","&amp;AS34:AS46&amp;","&amp;AT34:AT46&amp;","&amp;AU34:AU46&amp;","&amp;AV34:AV46</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="41" customHeight="1" spans="3:50">
       <c r="C41" s="1">
-        <v>3032</v>
+        <v>3033</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>147</v>
@@ -8425,7 +8445,7 @@
         <v>0</v>
       </c>
       <c r="P41" s="1">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="Q41" s="1">
         <v>0</v>
@@ -8524,17 +8544,17 @@
         <v>0</v>
       </c>
       <c r="AW41" s="10" t="str">
-        <f t="shared" ref="AW41:AW46" si="2">AC35:AC47&amp;","&amp;AD35:AD47&amp;","&amp;AE35:AE47&amp;","&amp;AF35:AF47&amp;","&amp;AG35:AG47&amp;","&amp;AH35:AH47&amp;","&amp;AI35:AI47&amp;","&amp;AJ35:AJ47&amp;","&amp;AK35:AK47&amp;","&amp;AL35:AL47</f>
+        <f t="shared" si="2"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX41" s="10" t="str">
-        <f t="shared" ref="AX41:AX46" si="3">AM35:AM47&amp;","&amp;AN35:AN47&amp;","&amp;AO35:AO47&amp;","&amp;AP35:AP47&amp;","&amp;AQ35:AQ47&amp;","&amp;AR35:AR47&amp;","&amp;AS35:AS47&amp;","&amp;AT35:AT47&amp;","&amp;AU35:AU47&amp;","&amp;AV35:AV47</f>
+        <f t="shared" si="3"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="42" customHeight="1" spans="3:50">
       <c r="C42" s="1">
-        <v>3033</v>
+        <v>3034</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>148</v>
@@ -8564,7 +8584,7 @@
         <v>0</v>
       </c>
       <c r="M42" s="12">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="N42" s="1">
         <v>0</v>
@@ -8573,7 +8593,7 @@
         <v>0</v>
       </c>
       <c r="P42" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="Q42" s="1">
         <v>0</v>
@@ -8682,7 +8702,7 @@
     </row>
     <row r="43" customHeight="1" spans="3:50">
       <c r="C43" s="1">
-        <v>3034</v>
+        <v>3035</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>149</v>
@@ -8712,7 +8732,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="12">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="N43" s="1">
         <v>0</v>
@@ -8830,7 +8850,7 @@
     </row>
     <row r="44" customHeight="1" spans="3:50">
       <c r="C44" s="1">
-        <v>3035</v>
+        <v>3036</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>150</v>
@@ -8851,7 +8871,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K44" s="1">
         <v>0</v>
@@ -8859,8 +8879,8 @@
       <c r="L44" s="1">
         <v>0</v>
       </c>
-      <c r="M44" s="12">
-        <v>0.005</v>
+      <c r="M44" s="1">
+        <v>0</v>
       </c>
       <c r="N44" s="1">
         <v>0</v>
@@ -8978,7 +8998,7 @@
     </row>
     <row r="45" customHeight="1" spans="3:50">
       <c r="C45" s="1">
-        <v>3036</v>
+        <v>3037</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>151</v>
@@ -8999,7 +9019,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="1">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="K45" s="1">
         <v>0</v>
@@ -9126,7 +9146,7 @@
     </row>
     <row r="46" customHeight="1" spans="3:50">
       <c r="C46" s="1">
-        <v>3037</v>
+        <v>3050</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>152</v>
@@ -9147,7 +9167,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="K46" s="1">
         <v>0</v>
@@ -9155,7 +9175,7 @@
       <c r="L46" s="1">
         <v>0</v>
       </c>
-      <c r="M46" s="1">
+      <c r="M46" s="12">
         <v>0</v>
       </c>
       <c r="N46" s="1">
@@ -9207,7 +9227,7 @@
         <v>0</v>
       </c>
       <c r="AD46" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="AE46" s="1">
         <v>0</v>
@@ -9264,17 +9284,17 @@
         <v>0</v>
       </c>
       <c r="AW46" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>0,0,0,0,0,0,0,0,0,0</v>
+        <f t="shared" ref="AW46:AW51" si="4">AC38:AC50&amp;","&amp;AD38:AD50&amp;","&amp;AE38:AE50&amp;","&amp;AF38:AF50&amp;","&amp;AG38:AG50&amp;","&amp;AH38:AH50&amp;","&amp;AI38:AI50&amp;","&amp;AJ38:AJ50&amp;","&amp;AK38:AK50&amp;","&amp;AL38:AL50</f>
+        <v>0,0.002,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX46" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AX46:AX51" si="5">AM38:AM50&amp;","&amp;AN38:AN50&amp;","&amp;AO38:AO50&amp;","&amp;AP38:AP50&amp;","&amp;AQ38:AQ50&amp;","&amp;AR38:AR50&amp;","&amp;AS38:AS50&amp;","&amp;AT38:AT50&amp;","&amp;AU38:AU50&amp;","&amp;AV38:AV50</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="47" customHeight="1" spans="3:50">
       <c r="C47" s="1">
-        <v>3050</v>
+        <v>3051</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>153</v>
@@ -9355,11 +9375,11 @@
         <v>0</v>
       </c>
       <c r="AD47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="1">
         <v>0.002</v>
       </c>
-      <c r="AE47" s="1">
-        <v>0</v>
-      </c>
       <c r="AF47" s="1">
         <v>0</v>
       </c>
@@ -9412,17 +9432,17 @@
         <v>0</v>
       </c>
       <c r="AW47" s="10" t="str">
-        <f t="shared" ref="AW47:AW52" si="4">AC39:AC51&amp;","&amp;AD39:AD51&amp;","&amp;AE39:AE51&amp;","&amp;AF39:AF51&amp;","&amp;AG39:AG51&amp;","&amp;AH39:AH51&amp;","&amp;AI39:AI51&amp;","&amp;AJ39:AJ51&amp;","&amp;AK39:AK51&amp;","&amp;AL39:AL51</f>
-        <v>0,0.002,0,0,0,0,0,0,0,0</v>
+        <f t="shared" si="4"/>
+        <v>0,0,0.002,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX47" s="10" t="str">
-        <f t="shared" ref="AX47:AX52" si="5">AM39:AM51&amp;","&amp;AN39:AN51&amp;","&amp;AO39:AO51&amp;","&amp;AP39:AP51&amp;","&amp;AQ39:AQ51&amp;","&amp;AR39:AR51&amp;","&amp;AS39:AS51&amp;","&amp;AT39:AT51&amp;","&amp;AU39:AU51&amp;","&amp;AV39:AV51</f>
+        <f t="shared" si="5"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="48" customHeight="1" spans="3:50">
       <c r="C48" s="1">
-        <v>3051</v>
+        <v>3052</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>154</v>
@@ -9506,10 +9526,10 @@
         <v>0</v>
       </c>
       <c r="AE48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF48" s="1">
         <v>0.002</v>
-      </c>
-      <c r="AF48" s="1">
-        <v>0</v>
       </c>
       <c r="AG48" s="1">
         <v>0</v>
@@ -9561,7 +9581,7 @@
       </c>
       <c r="AW48" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0.002,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0.002,0,0,0,0,0,0</v>
       </c>
       <c r="AX48" s="10" t="str">
         <f t="shared" si="5"/>
@@ -9570,7 +9590,7 @@
     </row>
     <row r="49" customHeight="1" spans="3:50">
       <c r="C49" s="1">
-        <v>3052</v>
+        <v>3053</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>155</v>
@@ -9657,10 +9677,10 @@
         <v>0</v>
       </c>
       <c r="AF49" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG49" s="1">
         <v>0.002</v>
-      </c>
-      <c r="AG49" s="1">
-        <v>0</v>
       </c>
       <c r="AH49" s="1">
         <v>0</v>
@@ -9709,7 +9729,7 @@
       </c>
       <c r="AW49" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0.002,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0.002,0,0,0,0,0</v>
       </c>
       <c r="AX49" s="10" t="str">
         <f t="shared" si="5"/>
@@ -9718,7 +9738,7 @@
     </row>
     <row r="50" customHeight="1" spans="3:50">
       <c r="C50" s="1">
-        <v>3053</v>
+        <v>3054</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>156</v>
@@ -9808,10 +9828,10 @@
         <v>0</v>
       </c>
       <c r="AG50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH50" s="1">
         <v>0.002</v>
-      </c>
-      <c r="AH50" s="1">
-        <v>0</v>
       </c>
       <c r="AI50" s="1">
         <v>0</v>
@@ -9857,7 +9877,7 @@
       </c>
       <c r="AW50" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,0.002,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0.002,0,0,0,0</v>
       </c>
       <c r="AX50" s="10" t="str">
         <f t="shared" si="5"/>
@@ -9866,7 +9886,7 @@
     </row>
     <row r="51" customHeight="1" spans="3:50">
       <c r="C51" s="1">
-        <v>3054</v>
+        <v>3055</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>157</v>
@@ -9959,10 +9979,10 @@
         <v>0</v>
       </c>
       <c r="AH51" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI51" s="1">
         <v>0.002</v>
-      </c>
-      <c r="AI51" s="1">
-        <v>0</v>
       </c>
       <c r="AJ51" s="1">
         <v>0</v>
@@ -10005,7 +10025,7 @@
       </c>
       <c r="AW51" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,0,0.002,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0.002,0,0,0</v>
       </c>
       <c r="AX51" s="10" t="str">
         <f t="shared" si="5"/>
@@ -10014,7 +10034,7 @@
     </row>
     <row r="52" customHeight="1" spans="3:50">
       <c r="C52" s="1">
-        <v>3055</v>
+        <v>3056</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>158</v>
@@ -10110,11 +10130,11 @@
         <v>0</v>
       </c>
       <c r="AI52" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ52" s="1">
         <v>0.002</v>
       </c>
-      <c r="AJ52" s="1">
-        <v>0</v>
-      </c>
       <c r="AK52" s="1">
         <v>0</v>
       </c>
@@ -10152,17 +10172,17 @@
         <v>0</v>
       </c>
       <c r="AW52" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>0,0,0,0,0,0,0.002,0,0,0</v>
+        <f t="shared" ref="AW47:AW81" si="6">AC46:AC56&amp;","&amp;AD46:AD56&amp;","&amp;AE46:AE56&amp;","&amp;AF46:AF56&amp;","&amp;AG46:AG56&amp;","&amp;AH46:AH56&amp;","&amp;AI46:AI56&amp;","&amp;AJ46:AJ56&amp;","&amp;AK46:AK56&amp;","&amp;AL46:AL56</f>
+        <v>0,0,0,0,0,0,0,0.002,0,0</v>
       </c>
       <c r="AX52" s="10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AX47:AX81" si="7">AM46:AM56&amp;","&amp;AN46:AN56&amp;","&amp;AO46:AO56&amp;","&amp;AP46:AP56&amp;","&amp;AQ46:AQ56&amp;","&amp;AR46:AR56&amp;","&amp;AS46:AS56&amp;","&amp;AT46:AT56&amp;","&amp;AU46:AU56&amp;","&amp;AV46:AV56</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="53" customHeight="1" spans="3:50">
       <c r="C53" s="1">
-        <v>3056</v>
+        <v>3057</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>159</v>
@@ -10261,11 +10281,11 @@
         <v>0</v>
       </c>
       <c r="AJ53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK53" s="1">
         <v>0.002</v>
       </c>
-      <c r="AK53" s="1">
-        <v>0</v>
-      </c>
       <c r="AL53" s="1">
         <v>0</v>
       </c>
@@ -10300,17 +10320,17 @@
         <v>0</v>
       </c>
       <c r="AW53" s="10" t="str">
-        <f t="shared" ref="AW48:AW82" si="6">AC47:AC57&amp;","&amp;AD47:AD57&amp;","&amp;AE47:AE57&amp;","&amp;AF47:AF57&amp;","&amp;AG47:AG57&amp;","&amp;AH47:AH57&amp;","&amp;AI47:AI57&amp;","&amp;AJ47:AJ57&amp;","&amp;AK47:AK57&amp;","&amp;AL47:AL57</f>
-        <v>0,0,0,0,0,0,0,0.002,0,0</v>
+        <f t="shared" si="6"/>
+        <v>0,0,0,0,0,0,0,0,0.002,0</v>
       </c>
       <c r="AX53" s="10" t="str">
-        <f t="shared" ref="AX48:AX82" si="7">AM47:AM57&amp;","&amp;AN47:AN57&amp;","&amp;AO47:AO57&amp;","&amp;AP47:AP57&amp;","&amp;AQ47:AQ57&amp;","&amp;AR47:AR57&amp;","&amp;AS47:AS57&amp;","&amp;AT47:AT57&amp;","&amp;AU47:AU57&amp;","&amp;AV47:AV57</f>
+        <f t="shared" si="7"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="54" customHeight="1" spans="3:50">
       <c r="C54" s="1">
-        <v>3057</v>
+        <v>3058</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>160</v>
@@ -10412,10 +10432,10 @@
         <v>0</v>
       </c>
       <c r="AK54" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL54" s="1">
         <v>0.002</v>
-      </c>
-      <c r="AL54" s="1">
-        <v>0</v>
       </c>
       <c r="AM54" s="1">
         <v>0</v>
@@ -10449,7 +10469,7 @@
       </c>
       <c r="AW54" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0,0.002,0</v>
+        <v>0,0,0,0,0,0,0,0,0,0.002</v>
       </c>
       <c r="AX54" s="10" t="str">
         <f t="shared" si="7"/>
@@ -10458,7 +10478,7 @@
     </row>
     <row r="55" customHeight="1" spans="3:50">
       <c r="C55" s="1">
-        <v>3058</v>
+        <v>3059</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>161</v>
@@ -10539,7 +10559,7 @@
         <v>0</v>
       </c>
       <c r="AD55" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="AE55" s="1">
         <v>0</v>
@@ -10563,7 +10583,7 @@
         <v>0</v>
       </c>
       <c r="AL55" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AM55" s="1">
         <v>0</v>
@@ -10597,7 +10617,7 @@
       </c>
       <c r="AW55" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0,0,0.002</v>
+        <v>0,0.005,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX55" s="10" t="str">
         <f t="shared" si="7"/>
@@ -10606,7 +10626,7 @@
     </row>
     <row r="56" customHeight="1" spans="3:50">
       <c r="C56" s="1">
-        <v>3059</v>
+        <v>3060</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>162</v>
@@ -10687,10 +10707,10 @@
         <v>0</v>
       </c>
       <c r="AD56" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE56" s="1">
         <v>0.005</v>
-      </c>
-      <c r="AE56" s="1">
-        <v>0</v>
       </c>
       <c r="AF56" s="1">
         <v>0</v>
@@ -10745,7 +10765,7 @@
       </c>
       <c r="AW56" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0.005,0,0,0,0,0,0,0,0</v>
+        <v>0,0,0.005,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX56" s="10" t="str">
         <f t="shared" si="7"/>
@@ -10754,7 +10774,7 @@
     </row>
     <row r="57" customHeight="1" spans="3:50">
       <c r="C57" s="1">
-        <v>3060</v>
+        <v>3061</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>163</v>
@@ -10838,10 +10858,10 @@
         <v>0</v>
       </c>
       <c r="AE57" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF57" s="1">
         <v>0.005</v>
-      </c>
-      <c r="AF57" s="1">
-        <v>0</v>
       </c>
       <c r="AG57" s="1">
         <v>0</v>
@@ -10893,7 +10913,7 @@
       </c>
       <c r="AW57" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0.005,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0.005,0,0,0,0,0,0</v>
       </c>
       <c r="AX57" s="10" t="str">
         <f t="shared" si="7"/>
@@ -10902,7 +10922,7 @@
     </row>
     <row r="58" customHeight="1" spans="3:50">
       <c r="C58" s="1">
-        <v>3061</v>
+        <v>3062</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>164</v>
@@ -10989,10 +11009,10 @@
         <v>0</v>
       </c>
       <c r="AF58" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG58" s="1">
         <v>0.005</v>
-      </c>
-      <c r="AG58" s="1">
-        <v>0</v>
       </c>
       <c r="AH58" s="1">
         <v>0</v>
@@ -11041,7 +11061,7 @@
       </c>
       <c r="AW58" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0.005,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0.005,0,0,0,0,0</v>
       </c>
       <c r="AX58" s="10" t="str">
         <f t="shared" si="7"/>
@@ -11050,7 +11070,7 @@
     </row>
     <row r="59" customHeight="1" spans="3:50">
       <c r="C59" s="1">
-        <v>3062</v>
+        <v>3063</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>165</v>
@@ -11140,10 +11160,10 @@
         <v>0</v>
       </c>
       <c r="AG59" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH59" s="1">
         <v>0.005</v>
-      </c>
-      <c r="AH59" s="1">
-        <v>0</v>
       </c>
       <c r="AI59" s="1">
         <v>0</v>
@@ -11189,7 +11209,7 @@
       </c>
       <c r="AW59" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0.005,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0.005,0,0,0,0</v>
       </c>
       <c r="AX59" s="10" t="str">
         <f t="shared" si="7"/>
@@ -11198,7 +11218,7 @@
     </row>
     <row r="60" customHeight="1" spans="3:50">
       <c r="C60" s="1">
-        <v>3063</v>
+        <v>3064</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>166</v>
@@ -11291,10 +11311,10 @@
         <v>0</v>
       </c>
       <c r="AH60" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI60" s="1">
         <v>0.005</v>
-      </c>
-      <c r="AI60" s="1">
-        <v>0</v>
       </c>
       <c r="AJ60" s="1">
         <v>0</v>
@@ -11337,7 +11357,7 @@
       </c>
       <c r="AW60" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0.005,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0.005,0,0,0</v>
       </c>
       <c r="AX60" s="10" t="str">
         <f t="shared" si="7"/>
@@ -11346,7 +11366,7 @@
     </row>
     <row r="61" customHeight="1" spans="3:50">
       <c r="C61" s="1">
-        <v>3064</v>
+        <v>3065</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>167</v>
@@ -11442,10 +11462,10 @@
         <v>0</v>
       </c>
       <c r="AI61" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ61" s="1">
         <v>0.005</v>
-      </c>
-      <c r="AJ61" s="1">
-        <v>0</v>
       </c>
       <c r="AK61" s="1">
         <v>0</v>
@@ -11485,7 +11505,7 @@
       </c>
       <c r="AW61" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0.005,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0.005,0,0</v>
       </c>
       <c r="AX61" s="10" t="str">
         <f t="shared" si="7"/>
@@ -11494,7 +11514,7 @@
     </row>
     <row r="62" customHeight="1" spans="3:50">
       <c r="C62" s="1">
-        <v>3065</v>
+        <v>3066</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>168</v>
@@ -11593,10 +11613,10 @@
         <v>0</v>
       </c>
       <c r="AJ62" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK62" s="1">
         <v>0.005</v>
-      </c>
-      <c r="AK62" s="1">
-        <v>0</v>
       </c>
       <c r="AL62" s="1">
         <v>0</v>
@@ -11633,7 +11653,7 @@
       </c>
       <c r="AW62" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0.005,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0.005,0</v>
       </c>
       <c r="AX62" s="10" t="str">
         <f t="shared" si="7"/>
@@ -11642,7 +11662,7 @@
     </row>
     <row r="63" customHeight="1" spans="3:50">
       <c r="C63" s="1">
-        <v>3066</v>
+        <v>3067</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>169</v>
@@ -11744,10 +11764,10 @@
         <v>0</v>
       </c>
       <c r="AK63" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL63" s="1">
         <v>0.005</v>
-      </c>
-      <c r="AL63" s="1">
-        <v>0</v>
       </c>
       <c r="AM63" s="1">
         <v>0</v>
@@ -11781,164 +11801,164 @@
       </c>
       <c r="AW63" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0,0.005,0</v>
+        <v>0,0,0,0,0,0,0,0,0,0.005</v>
       </c>
       <c r="AX63" s="10" t="str">
         <f t="shared" si="7"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="64" customHeight="1" spans="3:50">
-      <c r="C64" s="1">
-        <v>3067</v>
-      </c>
-      <c r="D64" s="1" t="s">
+    <row r="64" s="2" customFormat="1" customHeight="1" spans="3:50">
+      <c r="C64" s="2">
+        <v>3068</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
-      <c r="F64" s="1">
-        <v>0</v>
-      </c>
-      <c r="G64" s="1">
-        <v>0</v>
-      </c>
-      <c r="H64" s="1">
-        <v>0</v>
-      </c>
-      <c r="I64" s="1">
-        <v>0</v>
-      </c>
-      <c r="J64" s="1">
-        <v>0</v>
-      </c>
-      <c r="K64" s="1">
-        <v>0</v>
-      </c>
-      <c r="L64" s="1">
-        <v>0</v>
-      </c>
-      <c r="M64" s="12">
-        <v>0</v>
-      </c>
-      <c r="N64" s="1">
-        <v>0</v>
-      </c>
-      <c r="O64" s="1">
-        <v>0</v>
-      </c>
-      <c r="P64" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q64" s="1">
-        <v>0</v>
-      </c>
-      <c r="R64" s="1">
-        <v>0</v>
-      </c>
-      <c r="S64" s="1">
-        <v>0</v>
-      </c>
-      <c r="T64" s="1">
-        <v>0</v>
-      </c>
-      <c r="U64" s="1">
-        <v>0</v>
-      </c>
-      <c r="V64" s="1">
-        <v>0</v>
-      </c>
-      <c r="W64" s="1">
-        <v>0</v>
-      </c>
-      <c r="X64" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y64" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA64" s="1">
+      <c r="E64" s="2">
+        <v>0</v>
+      </c>
+      <c r="F64" s="2">
+        <v>0</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2">
+        <v>0</v>
+      </c>
+      <c r="I64" s="2">
+        <v>0</v>
+      </c>
+      <c r="J64" s="2">
+        <v>0</v>
+      </c>
+      <c r="K64" s="2">
+        <v>0</v>
+      </c>
+      <c r="L64" s="2">
+        <v>0</v>
+      </c>
+      <c r="M64" s="16">
+        <v>0</v>
+      </c>
+      <c r="N64" s="2">
+        <v>0</v>
+      </c>
+      <c r="O64" s="2">
+        <v>0</v>
+      </c>
+      <c r="P64" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="2">
+        <v>0</v>
+      </c>
+      <c r="R64" s="2">
+        <v>0</v>
+      </c>
+      <c r="S64" s="2">
+        <v>0</v>
+      </c>
+      <c r="T64" s="2">
+        <v>0</v>
+      </c>
+      <c r="U64" s="2">
+        <v>0</v>
+      </c>
+      <c r="V64" s="2">
+        <v>0</v>
+      </c>
+      <c r="W64" s="2">
+        <v>0</v>
+      </c>
+      <c r="X64" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y64" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA64" s="2">
         <v>0</v>
       </c>
       <c r="AB64" s="1">
         <v>0</v>
       </c>
-      <c r="AC64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL64" s="1">
-        <v>0.005</v>
-      </c>
-      <c r="AM64" s="1">
+      <c r="AC64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM64" s="2">
         <v>0</v>
       </c>
       <c r="AN64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV64" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW64" s="10" t="str">
+        <v>0.002</v>
+      </c>
+      <c r="AO64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV64" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW64" s="19" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0,0,0.005</v>
-      </c>
-      <c r="AX64" s="10" t="str">
+        <v>0,0,0,0,0,0,0,0,0,0</v>
+      </c>
+      <c r="AX64" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0,0,0</v>
+        <v>0,0.002,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="65" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C65" s="2">
-        <v>3068</v>
+        <v>3069</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>171</v>
@@ -11967,7 +11987,7 @@
       <c r="L65" s="2">
         <v>0</v>
       </c>
-      <c r="M65" s="19">
+      <c r="M65" s="16">
         <v>0</v>
       </c>
       <c r="N65" s="2">
@@ -12048,12 +12068,12 @@
       <c r="AM65" s="2">
         <v>0</v>
       </c>
-      <c r="AN65" s="1">
+      <c r="AN65" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO65" s="1">
         <v>0.002</v>
       </c>
-      <c r="AO65" s="2">
-        <v>0</v>
-      </c>
       <c r="AP65" s="2">
         <v>0</v>
       </c>
@@ -12075,18 +12095,18 @@
       <c r="AV65" s="2">
         <v>0</v>
       </c>
-      <c r="AW65" s="20" t="str">
+      <c r="AW65" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX65" s="20" t="str">
+      <c r="AX65" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0.002,0,0,0,0,0,0,0,0</v>
+        <v>0,0,0.002,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="66" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C66" s="2">
-        <v>3069</v>
+        <v>3070</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>172</v>
@@ -12115,7 +12135,7 @@
       <c r="L66" s="2">
         <v>0</v>
       </c>
-      <c r="M66" s="19">
+      <c r="M66" s="16">
         <v>0</v>
       </c>
       <c r="N66" s="2">
@@ -12199,12 +12219,12 @@
       <c r="AN66" s="2">
         <v>0</v>
       </c>
-      <c r="AO66" s="1">
+      <c r="AO66" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP66" s="1">
         <v>0.002</v>
       </c>
-      <c r="AP66" s="2">
-        <v>0</v>
-      </c>
       <c r="AQ66" s="2">
         <v>0</v>
       </c>
@@ -12223,18 +12243,18 @@
       <c r="AV66" s="2">
         <v>0</v>
       </c>
-      <c r="AW66" s="20" t="str">
+      <c r="AW66" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX66" s="20" t="str">
+      <c r="AX66" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0.002,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0.002,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="67" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C67" s="2">
-        <v>3070</v>
+        <v>3071</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>173</v>
@@ -12263,7 +12283,7 @@
       <c r="L67" s="2">
         <v>0</v>
       </c>
-      <c r="M67" s="19">
+      <c r="M67" s="16">
         <v>0</v>
       </c>
       <c r="N67" s="2">
@@ -12350,12 +12370,12 @@
       <c r="AO67" s="2">
         <v>0</v>
       </c>
-      <c r="AP67" s="1">
+      <c r="AP67" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ67" s="1">
         <v>0.002</v>
       </c>
-      <c r="AQ67" s="2">
-        <v>0</v>
-      </c>
       <c r="AR67" s="2">
         <v>0</v>
       </c>
@@ -12371,18 +12391,18 @@
       <c r="AV67" s="2">
         <v>0</v>
       </c>
-      <c r="AW67" s="20" t="str">
+      <c r="AW67" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX67" s="20" t="str">
+      <c r="AX67" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0.002,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0.002,0,0,0,0,0</v>
       </c>
     </row>
     <row r="68" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C68" s="2">
-        <v>3071</v>
+        <v>3072</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>174</v>
@@ -12411,7 +12431,7 @@
       <c r="L68" s="2">
         <v>0</v>
       </c>
-      <c r="M68" s="19">
+      <c r="M68" s="16">
         <v>0</v>
       </c>
       <c r="N68" s="2">
@@ -12501,12 +12521,12 @@
       <c r="AP68" s="2">
         <v>0</v>
       </c>
-      <c r="AQ68" s="1">
+      <c r="AQ68" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR68" s="1">
         <v>0.002</v>
       </c>
-      <c r="AR68" s="2">
-        <v>0</v>
-      </c>
       <c r="AS68" s="2">
         <v>0</v>
       </c>
@@ -12519,18 +12539,18 @@
       <c r="AV68" s="2">
         <v>0</v>
       </c>
-      <c r="AW68" s="20" t="str">
+      <c r="AW68" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX68" s="20" t="str">
+      <c r="AX68" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0.002,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0.002,0,0,0,0</v>
       </c>
     </row>
     <row r="69" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C69" s="2">
-        <v>3072</v>
+        <v>3073</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>175</v>
@@ -12559,7 +12579,7 @@
       <c r="L69" s="2">
         <v>0</v>
       </c>
-      <c r="M69" s="19">
+      <c r="M69" s="16">
         <v>0</v>
       </c>
       <c r="N69" s="2">
@@ -12652,12 +12672,12 @@
       <c r="AQ69" s="2">
         <v>0</v>
       </c>
-      <c r="AR69" s="1">
+      <c r="AR69" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS69" s="1">
         <v>0.002</v>
       </c>
-      <c r="AS69" s="2">
-        <v>0</v>
-      </c>
       <c r="AT69" s="2">
         <v>0</v>
       </c>
@@ -12667,18 +12687,18 @@
       <c r="AV69" s="2">
         <v>0</v>
       </c>
-      <c r="AW69" s="20" t="str">
+      <c r="AW69" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX69" s="20" t="str">
+      <c r="AX69" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0.002,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0.002,0,0,0</v>
       </c>
     </row>
     <row r="70" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C70" s="2">
-        <v>3073</v>
+        <v>3074</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>176</v>
@@ -12707,7 +12727,7 @@
       <c r="L70" s="2">
         <v>0</v>
       </c>
-      <c r="M70" s="19">
+      <c r="M70" s="16">
         <v>0</v>
       </c>
       <c r="N70" s="2">
@@ -12803,30 +12823,30 @@
       <c r="AR70" s="2">
         <v>0</v>
       </c>
-      <c r="AS70" s="1">
+      <c r="AS70" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT70" s="1">
         <v>0.002</v>
       </c>
-      <c r="AT70" s="2">
-        <v>0</v>
-      </c>
       <c r="AU70" s="2">
         <v>0</v>
       </c>
       <c r="AV70" s="2">
         <v>0</v>
       </c>
-      <c r="AW70" s="20" t="str">
+      <c r="AW70" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX70" s="20" t="str">
+      <c r="AX70" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0.002,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0.002,0,0</v>
       </c>
     </row>
     <row r="71" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C71" s="2">
-        <v>3074</v>
+        <v>3075</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>177</v>
@@ -12855,7 +12875,7 @@
       <c r="L71" s="2">
         <v>0</v>
       </c>
-      <c r="M71" s="19">
+      <c r="M71" s="16">
         <v>0</v>
       </c>
       <c r="N71" s="2">
@@ -12954,27 +12974,27 @@
       <c r="AS71" s="2">
         <v>0</v>
       </c>
-      <c r="AT71" s="1">
+      <c r="AT71" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU71" s="1">
         <v>0.002</v>
       </c>
-      <c r="AU71" s="2">
-        <v>0</v>
-      </c>
       <c r="AV71" s="2">
         <v>0</v>
       </c>
-      <c r="AW71" s="20" t="str">
+      <c r="AW71" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX71" s="20" t="str">
+      <c r="AX71" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0.002,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0.002,0</v>
       </c>
     </row>
     <row r="72" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C72" s="2">
-        <v>3075</v>
+        <v>3076</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>178</v>
@@ -13003,7 +13023,7 @@
       <c r="L72" s="2">
         <v>0</v>
       </c>
-      <c r="M72" s="19">
+      <c r="M72" s="16">
         <v>0</v>
       </c>
       <c r="N72" s="2">
@@ -13105,24 +13125,24 @@
       <c r="AT72" s="2">
         <v>0</v>
       </c>
-      <c r="AU72" s="1">
-        <v>0.002</v>
+      <c r="AU72" s="2">
+        <v>0</v>
       </c>
       <c r="AV72" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW72" s="20" t="str">
+        <v>20</v>
+      </c>
+      <c r="AW72" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX72" s="20" t="str">
+      <c r="AX72" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0,0.002,0</v>
+        <v>0,0,0,0,0,0,0,0,0,20</v>
       </c>
     </row>
     <row r="73" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C73" s="2">
-        <v>3076</v>
+        <v>3077</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>179</v>
@@ -13151,7 +13171,7 @@
       <c r="L73" s="2">
         <v>0</v>
       </c>
-      <c r="M73" s="19">
+      <c r="M73" s="12">
         <v>0</v>
       </c>
       <c r="N73" s="2">
@@ -13232,8 +13252,8 @@
       <c r="AM73" s="2">
         <v>0</v>
       </c>
-      <c r="AN73" s="2">
-        <v>0</v>
+      <c r="AN73" s="1">
+        <v>0.005</v>
       </c>
       <c r="AO73" s="2">
         <v>0</v>
@@ -13257,20 +13277,20 @@
         <v>0</v>
       </c>
       <c r="AV73" s="2">
-        <v>20</v>
-      </c>
-      <c r="AW73" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AW73" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX73" s="20" t="str">
+      <c r="AX73" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0,0,20</v>
+        <v>0,0.005,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="74" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C74" s="2">
-        <v>3077</v>
+        <v>3078</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>180</v>
@@ -13380,12 +13400,12 @@
       <c r="AM74" s="2">
         <v>0</v>
       </c>
-      <c r="AN74" s="1">
+      <c r="AN74" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO74" s="1">
         <v>0.005</v>
       </c>
-      <c r="AO74" s="2">
-        <v>0</v>
-      </c>
       <c r="AP74" s="2">
         <v>0</v>
       </c>
@@ -13407,18 +13427,18 @@
       <c r="AV74" s="2">
         <v>0</v>
       </c>
-      <c r="AW74" s="20" t="str">
+      <c r="AW74" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX74" s="20" t="str">
+      <c r="AX74" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0.005,0,0,0,0,0,0,0,0</v>
+        <v>0,0,0.005,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="75" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C75" s="2">
-        <v>3078</v>
+        <v>3079</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>181</v>
@@ -13531,12 +13551,12 @@
       <c r="AN75" s="2">
         <v>0</v>
       </c>
-      <c r="AO75" s="1">
+      <c r="AO75" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP75" s="1">
         <v>0.005</v>
       </c>
-      <c r="AP75" s="2">
-        <v>0</v>
-      </c>
       <c r="AQ75" s="2">
         <v>0</v>
       </c>
@@ -13555,18 +13575,18 @@
       <c r="AV75" s="2">
         <v>0</v>
       </c>
-      <c r="AW75" s="20" t="str">
+      <c r="AW75" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX75" s="20" t="str">
+      <c r="AX75" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0.005,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0.005,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="76" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C76" s="2">
-        <v>3079</v>
+        <v>3080</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>182</v>
@@ -13682,12 +13702,12 @@
       <c r="AO76" s="2">
         <v>0</v>
       </c>
-      <c r="AP76" s="1">
+      <c r="AP76" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ76" s="1">
         <v>0.005</v>
       </c>
-      <c r="AQ76" s="2">
-        <v>0</v>
-      </c>
       <c r="AR76" s="2">
         <v>0</v>
       </c>
@@ -13703,18 +13723,18 @@
       <c r="AV76" s="2">
         <v>0</v>
       </c>
-      <c r="AW76" s="20" t="str">
+      <c r="AW76" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX76" s="20" t="str">
+      <c r="AX76" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0.005,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0.005,0,0,0,0,0</v>
       </c>
     </row>
     <row r="77" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C77" s="2">
-        <v>3080</v>
+        <v>3081</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>183</v>
@@ -13833,12 +13853,12 @@
       <c r="AP77" s="2">
         <v>0</v>
       </c>
-      <c r="AQ77" s="1">
+      <c r="AQ77" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR77" s="1">
         <v>0.005</v>
       </c>
-      <c r="AR77" s="2">
-        <v>0</v>
-      </c>
       <c r="AS77" s="2">
         <v>0</v>
       </c>
@@ -13851,18 +13871,18 @@
       <c r="AV77" s="2">
         <v>0</v>
       </c>
-      <c r="AW77" s="20" t="str">
+      <c r="AW77" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX77" s="20" t="str">
+      <c r="AX77" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0.005,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0.005,0,0,0,0</v>
       </c>
     </row>
     <row r="78" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C78" s="2">
-        <v>3081</v>
+        <v>3082</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>184</v>
@@ -13984,12 +14004,12 @@
       <c r="AQ78" s="2">
         <v>0</v>
       </c>
-      <c r="AR78" s="1">
+      <c r="AR78" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS78" s="1">
         <v>0.005</v>
       </c>
-      <c r="AS78" s="2">
-        <v>0</v>
-      </c>
       <c r="AT78" s="2">
         <v>0</v>
       </c>
@@ -13999,18 +14019,18 @@
       <c r="AV78" s="2">
         <v>0</v>
       </c>
-      <c r="AW78" s="20" t="str">
+      <c r="AW78" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX78" s="20" t="str">
+      <c r="AX78" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0.005,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0.005,0,0,0</v>
       </c>
     </row>
     <row r="79" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C79" s="2">
-        <v>3082</v>
+        <v>3083</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>185</v>
@@ -14135,30 +14155,30 @@
       <c r="AR79" s="2">
         <v>0</v>
       </c>
-      <c r="AS79" s="1">
+      <c r="AS79" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT79" s="1">
         <v>0.005</v>
       </c>
-      <c r="AT79" s="2">
-        <v>0</v>
-      </c>
       <c r="AU79" s="2">
         <v>0</v>
       </c>
       <c r="AV79" s="2">
         <v>0</v>
       </c>
-      <c r="AW79" s="20" t="str">
+      <c r="AW79" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX79" s="20" t="str">
+      <c r="AX79" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0.005,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0.005,0,0</v>
       </c>
     </row>
     <row r="80" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C80" s="2">
-        <v>3083</v>
+        <v>3084</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>186</v>
@@ -14286,27 +14306,27 @@
       <c r="AS80" s="2">
         <v>0</v>
       </c>
-      <c r="AT80" s="1">
+      <c r="AT80" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU80" s="1">
         <v>0.005</v>
       </c>
-      <c r="AU80" s="2">
-        <v>0</v>
-      </c>
       <c r="AV80" s="2">
         <v>0</v>
       </c>
-      <c r="AW80" s="20" t="str">
+      <c r="AW80" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX80" s="20" t="str">
+      <c r="AX80" s="19" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0.005,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0.005,0</v>
       </c>
     </row>
     <row r="81" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C81" s="2">
-        <v>3084</v>
+        <v>3085</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>187</v>
@@ -14437,185 +14457,185 @@
       <c r="AT81" s="2">
         <v>0</v>
       </c>
-      <c r="AU81" s="1">
-        <v>0.005</v>
+      <c r="AU81" s="2">
+        <v>0</v>
       </c>
       <c r="AV81" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW81" s="20" t="str">
+        <v>50</v>
+      </c>
+      <c r="AW81" s="19" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX81" s="20" t="str">
-        <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0,0.005,0</v>
-      </c>
-    </row>
-    <row r="82" s="2" customFormat="1" customHeight="1" spans="3:50">
-      <c r="C82" s="2">
-        <v>3085</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E82" s="2">
-        <v>0</v>
-      </c>
-      <c r="F82" s="2">
-        <v>0</v>
-      </c>
-      <c r="G82" s="2">
-        <v>0</v>
-      </c>
-      <c r="H82" s="2">
-        <v>0</v>
-      </c>
-      <c r="I82" s="2">
-        <v>0</v>
-      </c>
-      <c r="J82" s="2">
-        <v>0</v>
-      </c>
-      <c r="K82" s="2">
-        <v>0</v>
-      </c>
-      <c r="L82" s="2">
-        <v>0</v>
-      </c>
-      <c r="M82" s="12">
-        <v>0</v>
-      </c>
-      <c r="N82" s="2">
-        <v>0</v>
-      </c>
-      <c r="O82" s="2">
-        <v>0</v>
-      </c>
-      <c r="P82" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q82" s="2">
-        <v>0</v>
-      </c>
-      <c r="R82" s="2">
-        <v>0</v>
-      </c>
-      <c r="S82" s="2">
-        <v>0</v>
-      </c>
-      <c r="T82" s="2">
-        <v>0</v>
-      </c>
-      <c r="U82" s="2">
-        <v>0</v>
-      </c>
-      <c r="V82" s="2">
-        <v>0</v>
-      </c>
-      <c r="W82" s="2">
-        <v>0</v>
-      </c>
-      <c r="X82" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y82" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV82" s="2">
-        <v>50</v>
-      </c>
-      <c r="AW82" s="20" t="str">
-        <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0,0,0</v>
-      </c>
-      <c r="AX82" s="20" t="str">
+      <c r="AX81" s="19" t="str">
         <f t="shared" si="7"/>
         <v>0,0,0,0,0,0,0,0,0,50</v>
+      </c>
+    </row>
+    <row r="82" customHeight="1" spans="3:50">
+      <c r="C82" s="1">
+        <v>3200</v>
+      </c>
+      <c r="D82" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E82" s="1">
+        <v>180</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1">
+        <v>0</v>
+      </c>
+      <c r="H82" s="1">
+        <v>0</v>
+      </c>
+      <c r="I82" s="1">
+        <v>0</v>
+      </c>
+      <c r="J82" s="1">
+        <v>0</v>
+      </c>
+      <c r="K82" s="1">
+        <v>0</v>
+      </c>
+      <c r="L82" s="1">
+        <v>0</v>
+      </c>
+      <c r="M82" s="12">
+        <v>0</v>
+      </c>
+      <c r="N82" s="1">
+        <v>0</v>
+      </c>
+      <c r="O82" s="1">
+        <v>0</v>
+      </c>
+      <c r="P82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>0</v>
+      </c>
+      <c r="R82" s="1">
+        <v>0</v>
+      </c>
+      <c r="S82" s="1">
+        <v>0</v>
+      </c>
+      <c r="T82" s="1">
+        <v>0</v>
+      </c>
+      <c r="U82" s="1">
+        <v>0</v>
+      </c>
+      <c r="V82" s="1">
+        <v>0</v>
+      </c>
+      <c r="W82" s="1">
+        <v>0</v>
+      </c>
+      <c r="X82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW82" s="10" t="str">
+        <f t="shared" ref="AW82:AW95" si="8">AC76:AC86&amp;","&amp;AD76:AD86&amp;","&amp;AE76:AE86&amp;","&amp;AF76:AF86&amp;","&amp;AG76:AG86&amp;","&amp;AH76:AH86&amp;","&amp;AI76:AI86&amp;","&amp;AJ76:AJ86&amp;","&amp;AK76:AK86&amp;","&amp;AL76:AL86</f>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
+      </c>
+      <c r="AX82" s="10" t="str">
+        <f t="shared" ref="AX82:AX95" si="9">AM76:AM86&amp;","&amp;AN76:AN86&amp;","&amp;AO76:AO86&amp;","&amp;AP76:AP86&amp;","&amp;AQ76:AQ86&amp;","&amp;AR76:AR86&amp;","&amp;AS76:AS86&amp;","&amp;AT76:AT86&amp;","&amp;AU76:AU86&amp;","&amp;AV76:AV86</f>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="83" customHeight="1" spans="3:50">
       <c r="C83" s="1">
-        <v>3200</v>
-      </c>
-      <c r="D83" s="18" t="s">
+        <v>3201</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>189</v>
       </c>
       <c r="E83" s="1">
+        <v>0</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1">
         <v>180</v>
       </c>
-      <c r="F83" s="1">
-        <v>0</v>
-      </c>
-      <c r="G83" s="1">
-        <v>0</v>
-      </c>
       <c r="H83" s="1">
         <v>0</v>
       </c>
@@ -14740,17 +14760,17 @@
         <v>0</v>
       </c>
       <c r="AW83" s="10" t="str">
-        <f t="shared" ref="AW83:AW96" si="8">AC77:AC87&amp;","&amp;AD77:AD87&amp;","&amp;AE77:AE87&amp;","&amp;AF77:AF87&amp;","&amp;AG77:AG87&amp;","&amp;AH77:AH87&amp;","&amp;AI77:AI87&amp;","&amp;AJ77:AJ87&amp;","&amp;AK77:AK87&amp;","&amp;AL77:AL87</f>
+        <f t="shared" si="8"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX83" s="10" t="str">
-        <f t="shared" ref="AX83:AX96" si="9">AM77:AM87&amp;","&amp;AN77:AN87&amp;","&amp;AO77:AO87&amp;","&amp;AP77:AP87&amp;","&amp;AQ77:AQ87&amp;","&amp;AR77:AR87&amp;","&amp;AS77:AS87&amp;","&amp;AT77:AT87&amp;","&amp;AU77:AU87&amp;","&amp;AV77:AV87</f>
+        <f t="shared" si="9"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="84" customHeight="1" spans="3:50">
       <c r="C84" s="1">
-        <v>3201</v>
+        <v>3202</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>190</v>
@@ -14762,7 +14782,7 @@
         <v>0</v>
       </c>
       <c r="G84" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="H84" s="1">
         <v>0</v>
@@ -14804,7 +14824,7 @@
         <v>0</v>
       </c>
       <c r="U84" s="1">
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="V84" s="1">
         <v>0</v>
@@ -14898,7 +14918,7 @@
     </row>
     <row r="85" customHeight="1" spans="3:50">
       <c r="C85" s="1">
-        <v>3202</v>
+        <v>3203</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>191</v>
@@ -14907,7 +14927,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="1">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="G85" s="1">
         <v>0</v>
@@ -14952,7 +14972,7 @@
         <v>0</v>
       </c>
       <c r="U85" s="1">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="V85" s="1">
         <v>0</v>
@@ -14978,7 +14998,7 @@
       <c r="AC85" s="1">
         <v>0</v>
       </c>
-      <c r="AD85" s="2">
+      <c r="AD85" s="1">
         <v>0</v>
       </c>
       <c r="AE85" s="1">
@@ -15046,7 +15066,7 @@
     </row>
     <row r="86" customHeight="1" spans="3:50">
       <c r="C86" s="1">
-        <v>3203</v>
+        <v>3204</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>192</v>
@@ -15055,13 +15075,13 @@
         <v>0</v>
       </c>
       <c r="F86" s="1">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1">
+        <v>0</v>
+      </c>
+      <c r="H86" s="1">
         <v>0.045</v>
-      </c>
-      <c r="G86" s="1">
-        <v>0</v>
-      </c>
-      <c r="H86" s="1">
-        <v>0</v>
       </c>
       <c r="I86" s="1">
         <v>0</v>
@@ -15194,7 +15214,7 @@
     </row>
     <row r="87" customHeight="1" spans="3:50">
       <c r="C87" s="1">
-        <v>3204</v>
+        <v>3205</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>193</v>
@@ -15209,49 +15229,49 @@
         <v>0</v>
       </c>
       <c r="H87" s="1">
+        <v>0</v>
+      </c>
+      <c r="I87" s="1">
+        <v>0</v>
+      </c>
+      <c r="J87" s="1">
+        <v>0</v>
+      </c>
+      <c r="K87" s="1">
+        <v>0</v>
+      </c>
+      <c r="L87" s="1">
+        <v>0</v>
+      </c>
+      <c r="M87" s="12">
+        <v>0</v>
+      </c>
+      <c r="N87" s="1">
+        <v>0</v>
+      </c>
+      <c r="O87" s="1">
+        <v>0</v>
+      </c>
+      <c r="P87" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q87" s="1">
+        <v>0</v>
+      </c>
+      <c r="R87" s="1">
+        <v>0</v>
+      </c>
+      <c r="S87" s="1">
+        <v>0</v>
+      </c>
+      <c r="T87" s="1">
+        <v>0</v>
+      </c>
+      <c r="U87" s="1">
+        <v>0</v>
+      </c>
+      <c r="V87" s="1">
         <v>0.045</v>
-      </c>
-      <c r="I87" s="1">
-        <v>0</v>
-      </c>
-      <c r="J87" s="1">
-        <v>0</v>
-      </c>
-      <c r="K87" s="1">
-        <v>0</v>
-      </c>
-      <c r="L87" s="1">
-        <v>0</v>
-      </c>
-      <c r="M87" s="12">
-        <v>0</v>
-      </c>
-      <c r="N87" s="1">
-        <v>0</v>
-      </c>
-      <c r="O87" s="1">
-        <v>0</v>
-      </c>
-      <c r="P87" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q87" s="1">
-        <v>0</v>
-      </c>
-      <c r="R87" s="1">
-        <v>0</v>
-      </c>
-      <c r="S87" s="1">
-        <v>0</v>
-      </c>
-      <c r="T87" s="1">
-        <v>0</v>
-      </c>
-      <c r="U87" s="1">
-        <v>0</v>
-      </c>
-      <c r="V87" s="1">
-        <v>0</v>
       </c>
       <c r="W87" s="1">
         <v>0</v>
@@ -15342,7 +15362,7 @@
     </row>
     <row r="88" customHeight="1" spans="3:50">
       <c r="C88" s="1">
-        <v>3205</v>
+        <v>3206</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>194</v>
@@ -15390,7 +15410,7 @@
         <v>0</v>
       </c>
       <c r="S88" s="1">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="T88" s="1">
         <v>0</v>
@@ -15399,7 +15419,7 @@
         <v>0</v>
       </c>
       <c r="V88" s="1">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="W88" s="1">
         <v>0</v>
@@ -15490,7 +15510,7 @@
     </row>
     <row r="89" customHeight="1" spans="3:50">
       <c r="C89" s="1">
-        <v>3206</v>
+        <v>3207</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>195</v>
@@ -15538,10 +15558,10 @@
         <v>0</v>
       </c>
       <c r="S89" s="1">
+        <v>0</v>
+      </c>
+      <c r="T89" s="1">
         <v>850</v>
-      </c>
-      <c r="T89" s="1">
-        <v>0</v>
       </c>
       <c r="U89" s="1">
         <v>0</v>
@@ -15638,7 +15658,7 @@
     </row>
     <row r="90" customHeight="1" spans="3:50">
       <c r="C90" s="1">
-        <v>3207</v>
+        <v>3208</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>196</v>
@@ -15656,7 +15676,7 @@
         <v>0</v>
       </c>
       <c r="I90" s="1">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="J90" s="1">
         <v>0</v>
@@ -15689,7 +15709,7 @@
         <v>0</v>
       </c>
       <c r="T90" s="1">
-        <v>850</v>
+        <v>0</v>
       </c>
       <c r="U90" s="1">
         <v>0</v>
@@ -15786,7 +15806,7 @@
     </row>
     <row r="91" customHeight="1" spans="3:50">
       <c r="C91" s="1">
-        <v>3208</v>
+        <v>3209</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>197</v>
@@ -15804,10 +15824,10 @@
         <v>0</v>
       </c>
       <c r="I91" s="1">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="J91" s="1">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="K91" s="1">
         <v>0</v>
@@ -15934,7 +15954,7 @@
     </row>
     <row r="92" customHeight="1" spans="3:50">
       <c r="C92" s="1">
-        <v>3209</v>
+        <v>3210</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>198</v>
@@ -15955,7 +15975,7 @@
         <v>0</v>
       </c>
       <c r="J92" s="1">
-        <v>210</v>
+        <v>1025</v>
       </c>
       <c r="K92" s="1">
         <v>0</v>
@@ -16082,7 +16102,7 @@
     </row>
     <row r="93" customHeight="1" spans="3:50">
       <c r="C93" s="1">
-        <v>3210</v>
+        <v>3211</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>199</v>
@@ -16103,7 +16123,7 @@
         <v>0</v>
       </c>
       <c r="J93" s="1">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="K93" s="1">
         <v>0</v>
@@ -16127,7 +16147,7 @@
         <v>0</v>
       </c>
       <c r="R93" s="1">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="S93" s="1">
         <v>0</v>
@@ -16230,7 +16250,7 @@
     </row>
     <row r="94" customHeight="1" spans="3:50">
       <c r="C94" s="1">
-        <v>3211</v>
+        <v>3212</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>200</v>
@@ -16269,13 +16289,13 @@
         <v>0</v>
       </c>
       <c r="P94" s="1">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="Q94" s="1">
         <v>0</v>
       </c>
       <c r="R94" s="1">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="S94" s="1">
         <v>0</v>
@@ -16378,7 +16398,7 @@
     </row>
     <row r="95" customHeight="1" spans="3:50">
       <c r="C95" s="1">
-        <v>3212</v>
+        <v>3213</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>201</v>
@@ -16408,7 +16428,7 @@
         <v>0</v>
       </c>
       <c r="M95" s="12">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="N95" s="1">
         <v>0</v>
@@ -16417,7 +16437,7 @@
         <v>0</v>
       </c>
       <c r="P95" s="1">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="Q95" s="1">
         <v>0</v>
@@ -16520,154 +16540,6 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX95" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>0,0,0,0,0,0,0,0,0,0</v>
-      </c>
-    </row>
-    <row r="96" customHeight="1" spans="3:50">
-      <c r="C96" s="1">
-        <v>3213</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E96" s="1">
-        <v>0</v>
-      </c>
-      <c r="F96" s="1">
-        <v>0</v>
-      </c>
-      <c r="G96" s="1">
-        <v>0</v>
-      </c>
-      <c r="H96" s="1">
-        <v>0</v>
-      </c>
-      <c r="I96" s="1">
-        <v>0</v>
-      </c>
-      <c r="J96" s="1">
-        <v>0</v>
-      </c>
-      <c r="K96" s="1">
-        <v>0</v>
-      </c>
-      <c r="L96" s="1">
-        <v>0</v>
-      </c>
-      <c r="M96" s="12">
-        <v>0.045</v>
-      </c>
-      <c r="N96" s="1">
-        <v>0</v>
-      </c>
-      <c r="O96" s="1">
-        <v>0</v>
-      </c>
-      <c r="P96" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q96" s="1">
-        <v>0</v>
-      </c>
-      <c r="R96" s="1">
-        <v>0</v>
-      </c>
-      <c r="S96" s="1">
-        <v>0</v>
-      </c>
-      <c r="T96" s="1">
-        <v>0</v>
-      </c>
-      <c r="U96" s="1">
-        <v>0</v>
-      </c>
-      <c r="V96" s="1">
-        <v>0</v>
-      </c>
-      <c r="W96" s="1">
-        <v>0</v>
-      </c>
-      <c r="X96" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y96" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV96" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW96" s="10" t="str">
-        <f t="shared" si="8"/>
-        <v>0,0,0,0,0,0,0,0,0,0</v>
-      </c>
-      <c r="AX96" s="10" t="str">
         <f t="shared" si="9"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:61309fd commit_msg:Merge branch 'dev' of https://bitbucket.org/funplus/excel into dev
# Conflicts:
#	global/Hero.xlsx ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -66,6 +66,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="C7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+关联hero表attId列。不同角色卡牌1级的</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E7" authorId="0">
       <text>
         <r>
@@ -84,7 +106,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-取卡牌升级50级数值</t>
+取卡牌升级50级数值，注意不是最终值，最终值走公式，还要乘品质和职业系数。所以这里的固定值需要填相同</t>
         </r>
       </text>
     </comment>
@@ -111,7 +133,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0">
+    <comment ref="D20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+此行为卡牌升级固定值，在卡牌升级公式中会被读取。
+但注意此行填的攻防血数值，并不是卡牌1级时的最终值。最终值会根据卡牌升级公式走，还要乘品质系数、职业系数等形成差异。
+此行同时兼顾1级默认值，比如暴击值初始为5%，移动速度初始为每秒10米等，需要填入。升级时只有填了成长率的属性（目前是攻防血）才会走公式。其他没有填成长率的属性为1级的默认值。
+如果想要初始1级时，不同卡牌的默认值有差异，比如卡牌A和卡牌B的初始速度不同。那就只能填多个固定值即多行，分别对应hero表了</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -138,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="203">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -524,6 +571,9 @@
     <t>卡牌升级成长率</t>
   </si>
   <si>
+    <t>卡牌升级固定值+1级默认值</t>
+  </si>
+  <si>
     <t>武器升级攻击力固定值</t>
   </si>
   <si>
@@ -757,9 +807,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
@@ -796,14 +846,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -813,15 +855,30 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -835,21 +892,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -862,9 +905,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -886,16 +929,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -919,14 +962,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
@@ -935,6 +970,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -978,7 +1028,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,13 +1040,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1008,13 +1058,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1032,13 +1082,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1050,49 +1094,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1104,31 +1118,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1140,7 +1130,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1158,7 +1160,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1200,41 +1250,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1263,13 +1283,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1297,16 +1336,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1315,7 +1365,7 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1324,124 +1374,124 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1474,19 +1524,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2687,10 +2737,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AX95"/>
+  <dimension ref="A1:AX96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83:K96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -3372,13 +3422,13 @@
         <v>112</v>
       </c>
       <c r="E7" s="11">
-        <v>440</v>
+        <v>550</v>
       </c>
       <c r="F7" s="11">
         <v>0</v>
       </c>
       <c r="G7" s="12">
-        <v>636</v>
+        <v>550</v>
       </c>
       <c r="H7" s="12">
         <v>0</v>
@@ -3420,7 +3470,7 @@
         <v>5000</v>
       </c>
       <c r="U7" s="12">
-        <v>12000</v>
+        <v>11000</v>
       </c>
       <c r="V7" s="12">
         <v>0</v>
@@ -3431,16 +3481,16 @@
       <c r="X7" s="12">
         <v>200</v>
       </c>
-      <c r="Y7" s="17">
+      <c r="Y7" s="16">
         <v>1000</v>
       </c>
-      <c r="Z7" s="17">
+      <c r="Z7" s="16">
         <v>10000</v>
       </c>
-      <c r="AA7" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="17">
+      <c r="AA7" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="16">
         <v>10</v>
       </c>
       <c r="AC7" s="12">
@@ -3521,14 +3571,14 @@
       <c r="D8" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="11">
         <v>550</v>
       </c>
       <c r="F8" s="11">
         <v>0</v>
       </c>
       <c r="G8" s="12">
-        <v>530</v>
+        <v>550</v>
       </c>
       <c r="H8" s="12">
         <v>0</v>
@@ -3570,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="U8" s="12">
-        <v>10000</v>
+        <v>11000</v>
       </c>
       <c r="V8" s="12">
         <v>0</v>
@@ -3581,16 +3631,16 @@
       <c r="X8" s="12">
         <v>200</v>
       </c>
-      <c r="Y8" s="17">
+      <c r="Y8" s="16">
         <v>1000</v>
       </c>
-      <c r="Z8" s="17">
+      <c r="Z8" s="16">
         <v>10000</v>
       </c>
-      <c r="AA8" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="17">
+      <c r="AA8" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="16">
         <v>10</v>
       </c>
       <c r="AC8" s="12">
@@ -3671,14 +3721,14 @@
       <c r="D9" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="12">
-        <v>660</v>
+      <c r="E9" s="11">
+        <v>550</v>
       </c>
       <c r="F9" s="11">
         <v>0</v>
       </c>
       <c r="G9" s="12">
-        <v>424</v>
+        <v>550</v>
       </c>
       <c r="H9" s="12">
         <v>0</v>
@@ -3720,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="U9" s="12">
-        <v>8500</v>
+        <v>11000</v>
       </c>
       <c r="V9" s="12">
         <v>0</v>
@@ -3731,16 +3781,16 @@
       <c r="X9" s="12">
         <v>200</v>
       </c>
-      <c r="Y9" s="17">
+      <c r="Y9" s="16">
         <v>1000</v>
       </c>
-      <c r="Z9" s="17">
+      <c r="Z9" s="16">
         <v>10000</v>
       </c>
-      <c r="AA9" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="17">
+      <c r="AA9" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="16">
         <v>10</v>
       </c>
       <c r="AC9" s="12">
@@ -3773,31 +3823,31 @@
       <c r="AL9" s="12">
         <v>0</v>
       </c>
-      <c r="AM9" s="18" t="s">
+      <c r="AM9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AN9" s="18" t="s">
+      <c r="AN9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AO9" s="18" t="s">
+      <c r="AO9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AP9" s="18" t="s">
+      <c r="AP9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AQ9" s="18" t="s">
+      <c r="AQ9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AR9" s="18" t="s">
+      <c r="AR9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AS9" s="18" t="s">
+      <c r="AS9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AT9" s="18" t="s">
+      <c r="AT9" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="AU9" s="18" t="s">
+      <c r="AU9" s="17" t="s">
         <v>115</v>
       </c>
       <c r="AV9" s="12">
@@ -3821,14 +3871,14 @@
       <c r="D10" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>550</v>
       </c>
       <c r="F10" s="11">
         <v>0</v>
       </c>
       <c r="G10" s="12">
-        <v>424</v>
+        <v>550</v>
       </c>
       <c r="H10" s="12">
         <v>0</v>
@@ -3870,7 +3920,7 @@
         <v>0</v>
       </c>
       <c r="U10" s="12">
-        <v>8500</v>
+        <v>11000</v>
       </c>
       <c r="V10" s="12">
         <v>0</v>
@@ -3881,16 +3931,16 @@
       <c r="X10" s="12">
         <v>200</v>
       </c>
-      <c r="Y10" s="17">
+      <c r="Y10" s="16">
         <v>1000</v>
       </c>
-      <c r="Z10" s="17">
+      <c r="Z10" s="16">
         <v>10000</v>
       </c>
-      <c r="AA10" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="17">
+      <c r="AA10" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="16">
         <v>10</v>
       </c>
       <c r="AC10" s="12">
@@ -4031,16 +4081,16 @@
       <c r="X11" s="12">
         <v>200</v>
       </c>
-      <c r="Y11" s="17">
+      <c r="Y11" s="16">
         <v>1000</v>
       </c>
-      <c r="Z11" s="17">
+      <c r="Z11" s="16">
         <v>10000</v>
       </c>
-      <c r="AA11" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="17">
+      <c r="AA11" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="16">
         <v>10</v>
       </c>
       <c r="AC11" s="12">
@@ -4179,16 +4229,16 @@
       <c r="X12" s="12">
         <v>200</v>
       </c>
-      <c r="Y12" s="17">
+      <c r="Y12" s="16">
         <v>1000</v>
       </c>
-      <c r="Z12" s="17">
+      <c r="Z12" s="16">
         <v>10000</v>
       </c>
-      <c r="AA12" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="17">
+      <c r="AA12" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="16">
         <v>10</v>
       </c>
       <c r="AC12" s="12">
@@ -4327,16 +4377,16 @@
       <c r="X13" s="12">
         <v>200</v>
       </c>
-      <c r="Y13" s="17">
+      <c r="Y13" s="16">
         <v>1000</v>
       </c>
-      <c r="Z13" s="17">
+      <c r="Z13" s="16">
         <v>10000</v>
       </c>
-      <c r="AA13" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="17">
+      <c r="AA13" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="16">
         <v>10</v>
       </c>
       <c r="AC13" s="12">
@@ -4464,7 +4514,7 @@
         <v>350</v>
       </c>
       <c r="U14" s="1">
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="V14" s="1">
         <v>0</v>
@@ -4612,7 +4662,7 @@
         <v>650</v>
       </c>
       <c r="U15" s="1">
-        <v>1250</v>
+        <v>2500</v>
       </c>
       <c r="V15" s="1">
         <v>0</v>
@@ -4760,7 +4810,7 @@
         <v>950</v>
       </c>
       <c r="U16" s="1">
-        <v>1750</v>
+        <v>3500</v>
       </c>
       <c r="V16" s="1">
         <v>0</v>
@@ -4908,7 +4958,7 @@
         <v>1250</v>
       </c>
       <c r="U17" s="1">
-        <v>2250</v>
+        <v>4500</v>
       </c>
       <c r="V17" s="1">
         <v>0</v>
@@ -5056,7 +5106,7 @@
         <v>1550</v>
       </c>
       <c r="U18" s="1">
-        <v>2750</v>
+        <v>5500</v>
       </c>
       <c r="V18" s="1">
         <v>0</v>
@@ -5140,11 +5190,11 @@
         <v>0</v>
       </c>
       <c r="AW18" s="10" t="str">
-        <f>AC11:AC20&amp;","&amp;AD11:AD20&amp;","&amp;AE11:AE20&amp;","&amp;AF11:AF20&amp;","&amp;AG11:AG20&amp;","&amp;AH11:AH20&amp;","&amp;AI11:AI20&amp;","&amp;AJ11:AJ20&amp;","&amp;AK11:AK20&amp;","&amp;AL11:AL20</f>
+        <f>AC11:AC21&amp;","&amp;AD11:AD21&amp;","&amp;AE11:AE21&amp;","&amp;AF11:AF21&amp;","&amp;AG11:AG21&amp;","&amp;AH11:AH21&amp;","&amp;AI11:AI21&amp;","&amp;AJ11:AJ21&amp;","&amp;AK11:AK21&amp;","&amp;AL11:AL21</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX18" s="10" t="str">
-        <f>AM11:AM20&amp;","&amp;AN11:AN20&amp;","&amp;AO11:AO20&amp;","&amp;AP11:AP20&amp;","&amp;AQ11:AQ20&amp;","&amp;AR11:AR20&amp;","&amp;AS11:AS20&amp;","&amp;AT11:AT20&amp;","&amp;AU11:AU20&amp;","&amp;AV11:AV20</f>
+        <f>AM11:AM21&amp;","&amp;AN11:AN21&amp;","&amp;AO11:AO21&amp;","&amp;AP11:AP21&amp;","&amp;AQ11:AQ21&amp;","&amp;AR11:AR21&amp;","&amp;AS11:AS21&amp;","&amp;AT11:AT21&amp;","&amp;AU11:AU21&amp;","&amp;AV11:AV21</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
@@ -5288,179 +5338,179 @@
         <v>0</v>
       </c>
       <c r="AW19" s="10" t="str">
-        <f>AC12:AC20&amp;","&amp;AD12:AD20&amp;","&amp;AE12:AE20&amp;","&amp;AF12:AF20&amp;","&amp;AG12:AG20&amp;","&amp;AH12:AH20&amp;","&amp;AI12:AI20&amp;","&amp;AJ12:AJ20&amp;","&amp;AK12:AK20&amp;","&amp;AL12:AL20</f>
+        <f>AC12:AC21&amp;","&amp;AD12:AD21&amp;","&amp;AE12:AE21&amp;","&amp;AF12:AF21&amp;","&amp;AG12:AG21&amp;","&amp;AH12:AH21&amp;","&amp;AI12:AI21&amp;","&amp;AJ12:AJ21&amp;","&amp;AK12:AK21&amp;","&amp;AL12:AL21</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX19" s="10" t="str">
-        <f>AM12:AM20&amp;","&amp;AN12:AN20&amp;","&amp;AO12:AO20&amp;","&amp;AP12:AP20&amp;","&amp;AQ12:AQ20&amp;","&amp;AR12:AR20&amp;","&amp;AS12:AS20&amp;","&amp;AT12:AT20&amp;","&amp;AU12:AU20&amp;","&amp;AV12:AV20</f>
+        <f>AM12:AM21&amp;","&amp;AN12:AN21&amp;","&amp;AO12:AO21&amp;","&amp;AP12:AP21&amp;","&amp;AQ12:AQ21&amp;","&amp;AR12:AR21&amp;","&amp;AS12:AS21&amp;","&amp;AT12:AT21&amp;","&amp;AU12:AU21&amp;","&amp;AV12:AV21</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="3:50">
       <c r="C20" s="1">
-        <v>2000</v>
+        <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="13">
         <v>50</v>
       </c>
       <c r="F20" s="11">
         <v>0</v>
       </c>
-      <c r="G20" s="1">
-        <v>0</v>
+      <c r="G20" s="12">
+        <v>50</v>
       </c>
       <c r="H20" s="12">
         <v>0</v>
       </c>
-      <c r="I20" s="1">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1">
-        <v>0</v>
-      </c>
-      <c r="K20" s="1">
-        <v>0</v>
-      </c>
-      <c r="L20" s="1">
+      <c r="I20" s="12">
+        <v>0</v>
+      </c>
+      <c r="J20" s="12">
+        <v>500</v>
+      </c>
+      <c r="K20" s="12">
+        <v>5000</v>
+      </c>
+      <c r="L20" s="12">
         <v>0</v>
       </c>
       <c r="M20" s="12">
         <v>0</v>
       </c>
-      <c r="N20" s="1">
-        <v>0</v>
-      </c>
-      <c r="O20" s="1">
-        <v>0</v>
+      <c r="N20" s="12">
+        <v>0</v>
+      </c>
+      <c r="O20" s="12">
+        <v>10</v>
       </c>
       <c r="P20" s="12">
         <v>0</v>
       </c>
-      <c r="Q20" s="1">
-        <v>0</v>
+      <c r="Q20" s="12">
+        <v>0.3</v>
       </c>
       <c r="R20" s="12">
         <v>0</v>
       </c>
-      <c r="S20" s="1">
-        <v>0</v>
-      </c>
-      <c r="T20" s="1">
-        <v>0</v>
-      </c>
-      <c r="U20" s="1">
-        <v>0</v>
+      <c r="S20" s="12">
+        <v>5000</v>
+      </c>
+      <c r="T20" s="12">
+        <v>0</v>
+      </c>
+      <c r="U20" s="12">
+        <v>1000</v>
       </c>
       <c r="V20" s="12">
         <v>0</v>
       </c>
-      <c r="W20" s="1">
-        <v>0</v>
-      </c>
-      <c r="X20" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV20" s="1">
+      <c r="W20" s="12">
+        <v>2500</v>
+      </c>
+      <c r="X20" s="12">
+        <v>200</v>
+      </c>
+      <c r="Y20" s="16">
+        <v>1000</v>
+      </c>
+      <c r="Z20" s="16">
+        <v>10000</v>
+      </c>
+      <c r="AA20" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="16">
+        <v>10</v>
+      </c>
+      <c r="AC20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AO20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="12">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="12">
         <v>0</v>
       </c>
       <c r="AW20" s="10" t="str">
-        <f>AC16:AC21&amp;","&amp;AD16:AD21&amp;","&amp;AE16:AE21&amp;","&amp;AF16:AF21&amp;","&amp;AG16:AG21&amp;","&amp;AH16:AH21&amp;","&amp;AI16:AI21&amp;","&amp;AJ16:AJ21&amp;","&amp;AK16:AK21&amp;","&amp;AL16:AL21</f>
+        <f>AC14:AC24&amp;","&amp;AD14:AD24&amp;","&amp;AE14:AE24&amp;","&amp;AF14:AF24&amp;","&amp;AG14:AG24&amp;","&amp;AH14:AH24&amp;","&amp;AI14:AI24&amp;","&amp;AJ14:AJ24&amp;","&amp;AK14:AK24&amp;","&amp;AL14:AL24</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX20" s="10" t="str">
-        <f>AM16:AM21&amp;","&amp;AN16:AN21&amp;","&amp;AO16:AO21&amp;","&amp;AP16:AP21&amp;","&amp;AQ16:AQ21&amp;","&amp;AR16:AR21&amp;","&amp;AS16:AS21&amp;","&amp;AT16:AT21&amp;","&amp;AU16:AU21&amp;","&amp;AV16:AV21</f>
+        <f>AM14:AM24&amp;","&amp;AN14:AN24&amp;","&amp;AO14:AO24&amp;","&amp;AP14:AP24&amp;","&amp;AQ14:AQ24&amp;","&amp;AR14:AR24&amp;","&amp;AS14:AS24&amp;","&amp;AT14:AT24&amp;","&amp;AU14:AU24&amp;","&amp;AV14:AV24</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="3:50">
       <c r="C21" s="1">
-        <v>2001</v>
-      </c>
-      <c r="D21" s="14" t="s">
+        <v>2000</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>127</v>
       </c>
       <c r="E21" s="1">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1">
+        <v>50</v>
+      </c>
+      <c r="F21" s="11">
         <v>0</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="12">
         <v>0</v>
       </c>
       <c r="I21" s="1">
@@ -5475,7 +5525,7 @@
       <c r="L21" s="1">
         <v>0</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M21" s="12">
         <v>0</v>
       </c>
       <c r="N21" s="1">
@@ -5484,13 +5534,13 @@
       <c r="O21" s="1">
         <v>0</v>
       </c>
-      <c r="P21" s="1">
+      <c r="P21" s="12">
         <v>0</v>
       </c>
       <c r="Q21" s="1">
         <v>0</v>
       </c>
-      <c r="R21" s="1">
+      <c r="R21" s="12">
         <v>0</v>
       </c>
       <c r="S21" s="1">
@@ -5502,7 +5552,7 @@
       <c r="U21" s="1">
         <v>0</v>
       </c>
-      <c r="V21" s="1">
+      <c r="V21" s="12">
         <v>0</v>
       </c>
       <c r="W21" s="1">
@@ -5584,31 +5634,31 @@
         <v>0</v>
       </c>
       <c r="AW21" s="10" t="str">
-        <f>AC20:AC25&amp;","&amp;AD20:AD25&amp;","&amp;AE20:AE25&amp;","&amp;AF20:AF25&amp;","&amp;AG20:AG25&amp;","&amp;AH20:AH25&amp;","&amp;AI20:AI25&amp;","&amp;AJ20:AJ25&amp;","&amp;AK20:AK25&amp;","&amp;AL20:AL25</f>
+        <f>AC16:AC22&amp;","&amp;AD16:AD22&amp;","&amp;AE16:AE22&amp;","&amp;AF16:AF22&amp;","&amp;AG16:AG22&amp;","&amp;AH16:AH22&amp;","&amp;AI16:AI22&amp;","&amp;AJ16:AJ22&amp;","&amp;AK16:AK22&amp;","&amp;AL16:AL22</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX21" s="10" t="str">
-        <f>AM20:AM25&amp;","&amp;AN20:AN25&amp;","&amp;AO20:AO25&amp;","&amp;AP20:AP25&amp;","&amp;AQ20:AQ25&amp;","&amp;AR20:AR25&amp;","&amp;AS20:AS25&amp;","&amp;AT20:AT25&amp;","&amp;AU20:AU25&amp;","&amp;AV20:AV25</f>
+        <f>AM16:AM22&amp;","&amp;AN16:AN22&amp;","&amp;AO16:AO22&amp;","&amp;AP16:AP22&amp;","&amp;AQ16:AQ22&amp;","&amp;AR16:AR22&amp;","&amp;AS16:AS22&amp;","&amp;AT16:AT22&amp;","&amp;AU16:AU22&amp;","&amp;AV16:AV22</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="3:50">
       <c r="C22" s="1">
-        <v>2010</v>
-      </c>
-      <c r="D22" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>128</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="11">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1">
         <v>0</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="1">
         <v>0</v>
       </c>
       <c r="I22" s="1">
@@ -5623,7 +5673,7 @@
       <c r="L22" s="1">
         <v>0</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="1">
         <v>0</v>
       </c>
       <c r="N22" s="1">
@@ -5632,13 +5682,13 @@
       <c r="O22" s="1">
         <v>0</v>
       </c>
-      <c r="P22" s="12">
+      <c r="P22" s="1">
         <v>0</v>
       </c>
       <c r="Q22" s="1">
         <v>0</v>
       </c>
-      <c r="R22" s="12">
+      <c r="R22" s="1">
         <v>0</v>
       </c>
       <c r="S22" s="1">
@@ -5650,7 +5700,7 @@
       <c r="U22" s="1">
         <v>0</v>
       </c>
-      <c r="V22" s="12">
+      <c r="V22" s="1">
         <v>0</v>
       </c>
       <c r="W22" s="1">
@@ -5672,7 +5722,7 @@
         <v>0</v>
       </c>
       <c r="AC22" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="AD22" s="1">
         <v>0</v>
@@ -5732,17 +5782,17 @@
         <v>0</v>
       </c>
       <c r="AW22" s="10" t="str">
-        <f>AC20:AC26&amp;","&amp;AD20:AD26&amp;","&amp;AE20:AE26&amp;","&amp;AF20:AF26&amp;","&amp;AG20:AG26&amp;","&amp;AH20:AH26&amp;","&amp;AI20:AI26&amp;","&amp;AJ20:AJ26&amp;","&amp;AK20:AK26&amp;","&amp;AL20:AL26</f>
-        <v>0.05,0,0,0,0,0,0,0,0,0</v>
+        <f>AC21:AC26&amp;","&amp;AD21:AD26&amp;","&amp;AE21:AE26&amp;","&amp;AF21:AF26&amp;","&amp;AG21:AG26&amp;","&amp;AH21:AH26&amp;","&amp;AI21:AI26&amp;","&amp;AJ21:AJ26&amp;","&amp;AK21:AK26&amp;","&amp;AL21:AL26</f>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX22" s="10" t="str">
-        <f>AM20:AM26&amp;","&amp;AN20:AN26&amp;","&amp;AO20:AO26&amp;","&amp;AP20:AP26&amp;","&amp;AQ20:AQ26&amp;","&amp;AR20:AR26&amp;","&amp;AS20:AS26&amp;","&amp;AT20:AT26&amp;","&amp;AU20:AU26&amp;","&amp;AV20:AV26</f>
+        <f>AM21:AM26&amp;","&amp;AN21:AN26&amp;","&amp;AO21:AO26&amp;","&amp;AP21:AP26&amp;","&amp;AQ21:AQ26&amp;","&amp;AR21:AR26&amp;","&amp;AS21:AS26&amp;","&amp;AT21:AT26&amp;","&amp;AU21:AU26&amp;","&amp;AV21:AV26</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="3:50">
       <c r="C23" s="1">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>129</v>
@@ -5820,7 +5870,7 @@
         <v>0</v>
       </c>
       <c r="AC23" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="AD23" s="1">
         <v>0</v>
@@ -5880,17 +5930,17 @@
         <v>0</v>
       </c>
       <c r="AW23" s="10" t="str">
-        <f>AC20:AC27&amp;","&amp;AD20:AD27&amp;","&amp;AE20:AE27&amp;","&amp;AF20:AF27&amp;","&amp;AG20:AG27&amp;","&amp;AH20:AH27&amp;","&amp;AI20:AI27&amp;","&amp;AJ20:AJ27&amp;","&amp;AK20:AK27&amp;","&amp;AL20:AL27</f>
-        <v>0.1,0,0,0,0,0,0,0,0,0</v>
+        <f>AC21:AC27&amp;","&amp;AD21:AD27&amp;","&amp;AE21:AE27&amp;","&amp;AF21:AF27&amp;","&amp;AG21:AG27&amp;","&amp;AH21:AH27&amp;","&amp;AI21:AI27&amp;","&amp;AJ21:AJ27&amp;","&amp;AK21:AK27&amp;","&amp;AL21:AL27</f>
+        <v>0.05,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX23" s="10" t="str">
-        <f>AM20:AM27&amp;","&amp;AN20:AN27&amp;","&amp;AO20:AO27&amp;","&amp;AP20:AP27&amp;","&amp;AQ20:AQ27&amp;","&amp;AR20:AR27&amp;","&amp;AS20:AS27&amp;","&amp;AT20:AT27&amp;","&amp;AU20:AU27&amp;","&amp;AV20:AV27</f>
+        <f>AM21:AM27&amp;","&amp;AN21:AN27&amp;","&amp;AO21:AO27&amp;","&amp;AP21:AP27&amp;","&amp;AQ21:AQ27&amp;","&amp;AR21:AR27&amp;","&amp;AS21:AS27&amp;","&amp;AT21:AT27&amp;","&amp;AU21:AU27&amp;","&amp;AV21:AV27</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="3:50">
       <c r="C24" s="1">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>130</v>
@@ -5968,7 +6018,7 @@
         <v>0</v>
       </c>
       <c r="AC24" s="1">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="AD24" s="1">
         <v>0</v>
@@ -6029,7 +6079,7 @@
       </c>
       <c r="AW24" s="10" t="str">
         <f>AC21:AC28&amp;","&amp;AD21:AD28&amp;","&amp;AE21:AE28&amp;","&amp;AF21:AF28&amp;","&amp;AG21:AG28&amp;","&amp;AH21:AH28&amp;","&amp;AI21:AI28&amp;","&amp;AJ21:AJ28&amp;","&amp;AK21:AK28&amp;","&amp;AL21:AL28</f>
-        <v>0.15,0,0,0,0,0,0,0,0,0</v>
+        <v>0.1,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX24" s="10" t="str">
         <f>AM21:AM28&amp;","&amp;AN21:AN28&amp;","&amp;AO21:AO28&amp;","&amp;AP21:AP28&amp;","&amp;AQ21:AQ28&amp;","&amp;AR21:AR28&amp;","&amp;AS21:AS28&amp;","&amp;AT21:AT28&amp;","&amp;AU21:AU28&amp;","&amp;AV21:AV28</f>
@@ -6038,7 +6088,7 @@
     </row>
     <row r="25" customHeight="1" spans="3:50">
       <c r="C25" s="1">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>131</v>
@@ -6116,7 +6166,7 @@
         <v>0</v>
       </c>
       <c r="AC25" s="1">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="AD25" s="1">
         <v>0</v>
@@ -6176,17 +6226,17 @@
         <v>0</v>
       </c>
       <c r="AW25" s="10" t="str">
-        <f>AC21:AC29&amp;","&amp;AD21:AD29&amp;","&amp;AE21:AE29&amp;","&amp;AF21:AF29&amp;","&amp;AG21:AG29&amp;","&amp;AH21:AH29&amp;","&amp;AI21:AI29&amp;","&amp;AJ21:AJ29&amp;","&amp;AK21:AK29&amp;","&amp;AL21:AL29</f>
-        <v>0.2,0,0,0,0,0,0,0,0,0</v>
+        <f>AC22:AC29&amp;","&amp;AD22:AD29&amp;","&amp;AE22:AE29&amp;","&amp;AF22:AF29&amp;","&amp;AG22:AG29&amp;","&amp;AH22:AH29&amp;","&amp;AI22:AI29&amp;","&amp;AJ22:AJ29&amp;","&amp;AK22:AK29&amp;","&amp;AL22:AL29</f>
+        <v>0.15,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX25" s="10" t="str">
-        <f>AM21:AM29&amp;","&amp;AN21:AN29&amp;","&amp;AO21:AO29&amp;","&amp;AP21:AP29&amp;","&amp;AQ21:AQ29&amp;","&amp;AR21:AR29&amp;","&amp;AS21:AS29&amp;","&amp;AT21:AT29&amp;","&amp;AU21:AU29&amp;","&amp;AV21:AV29</f>
+        <f>AM22:AM29&amp;","&amp;AN22:AN29&amp;","&amp;AO22:AO29&amp;","&amp;AP22:AP29&amp;","&amp;AQ22:AQ29&amp;","&amp;AR22:AR29&amp;","&amp;AS22:AS29&amp;","&amp;AT22:AT29&amp;","&amp;AU22:AU29&amp;","&amp;AV22:AV29</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="3:50">
       <c r="C26" s="1">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>132</v>
@@ -6264,7 +6314,7 @@
         <v>0</v>
       </c>
       <c r="AC26" s="1">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="AD26" s="1">
         <v>0</v>
@@ -6324,17 +6374,17 @@
         <v>0</v>
       </c>
       <c r="AW26" s="10" t="str">
-        <f>AC21:AC30&amp;","&amp;AD21:AD30&amp;","&amp;AE21:AE30&amp;","&amp;AF21:AF30&amp;","&amp;AG21:AG30&amp;","&amp;AH21:AH30&amp;","&amp;AI21:AI30&amp;","&amp;AJ21:AJ30&amp;","&amp;AK21:AK30&amp;","&amp;AL21:AL30</f>
-        <v>0.25,0,0,0,0,0,0,0,0,0</v>
+        <f>AC22:AC30&amp;","&amp;AD22:AD30&amp;","&amp;AE22:AE30&amp;","&amp;AF22:AF30&amp;","&amp;AG22:AG30&amp;","&amp;AH22:AH30&amp;","&amp;AI22:AI30&amp;","&amp;AJ22:AJ30&amp;","&amp;AK22:AK30&amp;","&amp;AL22:AL30</f>
+        <v>0.2,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX26" s="10" t="str">
-        <f>AM21:AM30&amp;","&amp;AN21:AN30&amp;","&amp;AO21:AO30&amp;","&amp;AP21:AP30&amp;","&amp;AQ21:AQ30&amp;","&amp;AR21:AR30&amp;","&amp;AS21:AS30&amp;","&amp;AT21:AT30&amp;","&amp;AU21:AU30&amp;","&amp;AV21:AV30</f>
+        <f>AM22:AM30&amp;","&amp;AN22:AN30&amp;","&amp;AO22:AO30&amp;","&amp;AP22:AP30&amp;","&amp;AQ22:AQ30&amp;","&amp;AR22:AR30&amp;","&amp;AS22:AS30&amp;","&amp;AT22:AT30&amp;","&amp;AU22:AU30&amp;","&amp;AV22:AV30</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="3:50">
       <c r="C27" s="1">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>133</v>
@@ -6394,7 +6444,7 @@
         <v>0</v>
       </c>
       <c r="W27" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="X27" s="1">
         <v>0</v>
@@ -6412,7 +6462,7 @@
         <v>0</v>
       </c>
       <c r="AC27" s="1">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AD27" s="1">
         <v>0</v>
@@ -6472,17 +6522,17 @@
         <v>0</v>
       </c>
       <c r="AW27" s="10" t="str">
-        <f>AC21:AC31&amp;","&amp;AD21:AD31&amp;","&amp;AE21:AE31&amp;","&amp;AF21:AF31&amp;","&amp;AG21:AG31&amp;","&amp;AH21:AH31&amp;","&amp;AI21:AI31&amp;","&amp;AJ21:AJ31&amp;","&amp;AK21:AK31&amp;","&amp;AL21:AL31</f>
-        <v>0,0,0,0,0,0,0,0,0,0</v>
+        <f>AC22:AC31&amp;","&amp;AD22:AD31&amp;","&amp;AE22:AE31&amp;","&amp;AF22:AF31&amp;","&amp;AG22:AG31&amp;","&amp;AH22:AH31&amp;","&amp;AI22:AI31&amp;","&amp;AJ22:AJ31&amp;","&amp;AK22:AK31&amp;","&amp;AL22:AL31</f>
+        <v>0.25,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX27" s="10" t="str">
-        <f>AM21:AM31&amp;","&amp;AN21:AN31&amp;","&amp;AO21:AO31&amp;","&amp;AP21:AP31&amp;","&amp;AQ21:AQ31&amp;","&amp;AR21:AR31&amp;","&amp;AS21:AS31&amp;","&amp;AT21:AT31&amp;","&amp;AU21:AU31&amp;","&amp;AV21:AV31</f>
+        <f>AM22:AM31&amp;","&amp;AN22:AN31&amp;","&amp;AO22:AO31&amp;","&amp;AP22:AP31&amp;","&amp;AQ22:AQ31&amp;","&amp;AR22:AR31&amp;","&amp;AS22:AS31&amp;","&amp;AT22:AT31&amp;","&amp;AU22:AU31&amp;","&amp;AV22:AV31</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="3:50">
       <c r="C28" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>134</v>
@@ -6542,7 +6592,7 @@
         <v>0</v>
       </c>
       <c r="W28" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="X28" s="1">
         <v>0</v>
@@ -6620,17 +6670,17 @@
         <v>0</v>
       </c>
       <c r="AW28" s="10" t="str">
-        <f>AC22:AC31&amp;","&amp;AD22:AD31&amp;","&amp;AE22:AE31&amp;","&amp;AF22:AF31&amp;","&amp;AG22:AG31&amp;","&amp;AH22:AH31&amp;","&amp;AI22:AI31&amp;","&amp;AJ22:AJ31&amp;","&amp;AK22:AK31&amp;","&amp;AL22:AL31</f>
+        <f>AC22:AC32&amp;","&amp;AD22:AD32&amp;","&amp;AE22:AE32&amp;","&amp;AF22:AF32&amp;","&amp;AG22:AG32&amp;","&amp;AH22:AH32&amp;","&amp;AI22:AI32&amp;","&amp;AJ22:AJ32&amp;","&amp;AK22:AK32&amp;","&amp;AL22:AL32</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX28" s="10" t="str">
-        <f>AM22:AM31&amp;","&amp;AN22:AN31&amp;","&amp;AO22:AO31&amp;","&amp;AP22:AP31&amp;","&amp;AQ22:AQ31&amp;","&amp;AR22:AR31&amp;","&amp;AS22:AS31&amp;","&amp;AT22:AT31&amp;","&amp;AU22:AU31&amp;","&amp;AV22:AV31</f>
+        <f>AM22:AM32&amp;","&amp;AN22:AN32&amp;","&amp;AO22:AO32&amp;","&amp;AP22:AP32&amp;","&amp;AQ22:AQ32&amp;","&amp;AR22:AR32&amp;","&amp;AS22:AS32&amp;","&amp;AT22:AT32&amp;","&amp;AU22:AU32&amp;","&amp;AV22:AV32</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="3:50">
       <c r="C29" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>135</v>
@@ -6690,7 +6740,7 @@
         <v>0</v>
       </c>
       <c r="W29" s="1">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="X29" s="1">
         <v>0</v>
@@ -6768,17 +6818,17 @@
         <v>0</v>
       </c>
       <c r="AW29" s="10" t="str">
-        <f>AC23:AC31&amp;","&amp;AD23:AD31&amp;","&amp;AE23:AE31&amp;","&amp;AF23:AF31&amp;","&amp;AG23:AG31&amp;","&amp;AH23:AH31&amp;","&amp;AI23:AI31&amp;","&amp;AJ23:AJ31&amp;","&amp;AK23:AK31&amp;","&amp;AL23:AL31</f>
+        <f>AC23:AC32&amp;","&amp;AD23:AD32&amp;","&amp;AE23:AE32&amp;","&amp;AF23:AF32&amp;","&amp;AG23:AG32&amp;","&amp;AH23:AH32&amp;","&amp;AI23:AI32&amp;","&amp;AJ23:AJ32&amp;","&amp;AK23:AK32&amp;","&amp;AL23:AL32</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX29" s="10" t="str">
-        <f>AM23:AM31&amp;","&amp;AN23:AN31&amp;","&amp;AO23:AO31&amp;","&amp;AP23:AP31&amp;","&amp;AQ23:AQ31&amp;","&amp;AR23:AR31&amp;","&amp;AS23:AS31&amp;","&amp;AT23:AT31&amp;","&amp;AU23:AU31&amp;","&amp;AV23:AV31</f>
+        <f>AM23:AM32&amp;","&amp;AN23:AN32&amp;","&amp;AO23:AO32&amp;","&amp;AP23:AP32&amp;","&amp;AQ23:AQ32&amp;","&amp;AR23:AR32&amp;","&amp;AS23:AS32&amp;","&amp;AT23:AT32&amp;","&amp;AU23:AU32&amp;","&amp;AV23:AV32</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="3:50">
       <c r="C30" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>136</v>
@@ -6838,7 +6888,7 @@
         <v>0</v>
       </c>
       <c r="W30" s="1">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="X30" s="1">
         <v>0</v>
@@ -6926,7 +6976,7 @@
     </row>
     <row r="31" customHeight="1" spans="3:50">
       <c r="C31" s="1">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>137</v>
@@ -6986,7 +7036,7 @@
         <v>0</v>
       </c>
       <c r="W31" s="1">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="X31" s="1">
         <v>0</v>
@@ -7074,21 +7124,21 @@
     </row>
     <row r="32" customHeight="1" spans="3:50">
       <c r="C32" s="1">
-        <v>3000</v>
+        <v>2024</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E32" s="1">
-        <v>6</v>
-      </c>
-      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="11">
         <v>0</v>
       </c>
       <c r="G32" s="1">
         <v>0</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="12">
         <v>0</v>
       </c>
       <c r="I32" s="1">
@@ -7112,13 +7162,13 @@
       <c r="O32" s="1">
         <v>0</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P32" s="12">
         <v>0</v>
       </c>
       <c r="Q32" s="1">
         <v>0</v>
       </c>
-      <c r="R32" s="1">
+      <c r="R32" s="12">
         <v>0</v>
       </c>
       <c r="S32" s="1">
@@ -7130,11 +7180,11 @@
       <c r="U32" s="1">
         <v>0</v>
       </c>
-      <c r="V32" s="1">
+      <c r="V32" s="12">
         <v>0</v>
       </c>
       <c r="W32" s="1">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="X32" s="1">
         <v>0</v>
@@ -7212,23 +7262,23 @@
         <v>0</v>
       </c>
       <c r="AW32" s="10" t="str">
-        <f>AC28:AC36&amp;","&amp;AD28:AD36&amp;","&amp;AE28:AE36&amp;","&amp;AF28:AF36&amp;","&amp;AG28:AG36&amp;","&amp;AH28:AH36&amp;","&amp;AI28:AI36&amp;","&amp;AJ28:AJ36&amp;","&amp;AK28:AK36&amp;","&amp;AL28:AL36</f>
+        <f>AC26:AC34&amp;","&amp;AD26:AD34&amp;","&amp;AE26:AE34&amp;","&amp;AF26:AF34&amp;","&amp;AG26:AG34&amp;","&amp;AH26:AH34&amp;","&amp;AI26:AI34&amp;","&amp;AJ26:AJ34&amp;","&amp;AK26:AK34&amp;","&amp;AL26:AL34</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX32" s="10" t="str">
-        <f>AM28:AM36&amp;","&amp;AN28:AN36&amp;","&amp;AO28:AO36&amp;","&amp;AP28:AP36&amp;","&amp;AQ28:AQ36&amp;","&amp;AR28:AR36&amp;","&amp;AS28:AS36&amp;","&amp;AT28:AT36&amp;","&amp;AU28:AU36&amp;","&amp;AV28:AV36</f>
+        <f>AM26:AM34&amp;","&amp;AN26:AN34&amp;","&amp;AO26:AO34&amp;","&amp;AP26:AP34&amp;","&amp;AQ26:AQ34&amp;","&amp;AR26:AR34&amp;","&amp;AS26:AS34&amp;","&amp;AT26:AT34&amp;","&amp;AU26:AU34&amp;","&amp;AV26:AV34</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="3:50">
       <c r="C33" s="1">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E33" s="1">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
@@ -7370,7 +7420,7 @@
     </row>
     <row r="34" customHeight="1" spans="3:50">
       <c r="C34" s="1">
-        <v>3010</v>
+        <v>3001</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>140</v>
@@ -7518,13 +7568,13 @@
     </row>
     <row r="35" customHeight="1" spans="3:50">
       <c r="C35" s="1">
-        <v>3011</v>
+        <v>3010</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>141</v>
       </c>
       <c r="E35" s="1">
-        <v>600</v>
+        <v>120</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -7666,13 +7716,13 @@
     </row>
     <row r="36" customHeight="1" spans="3:50">
       <c r="C36" s="1">
-        <v>3020</v>
+        <v>3011</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>142</v>
       </c>
       <c r="E36" s="1">
-        <v>6</v>
+        <v>1200</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
@@ -7814,13 +7864,13 @@
     </row>
     <row r="37" customHeight="1" spans="3:50">
       <c r="C37" s="1">
-        <v>3021</v>
+        <v>3020</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E37" s="1">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -7952,23 +8002,23 @@
         <v>0</v>
       </c>
       <c r="AW37" s="10" t="str">
-        <f>AC32:AC41&amp;","&amp;AD32:AD41&amp;","&amp;AE32:AE41&amp;","&amp;AF32:AF41&amp;","&amp;AG32:AG41&amp;","&amp;AH32:AH41&amp;","&amp;AI32:AI41&amp;","&amp;AJ32:AJ41&amp;","&amp;AK32:AK41&amp;","&amp;AL32:AL41</f>
+        <f>AC33:AC41&amp;","&amp;AD33:AD41&amp;","&amp;AE33:AE41&amp;","&amp;AF33:AF41&amp;","&amp;AG33:AG41&amp;","&amp;AH33:AH41&amp;","&amp;AI33:AI41&amp;","&amp;AJ33:AJ41&amp;","&amp;AK33:AK41&amp;","&amp;AL33:AL41</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX37" s="10" t="str">
-        <f>AM32:AM41&amp;","&amp;AN32:AN41&amp;","&amp;AO32:AO41&amp;","&amp;AP32:AP41&amp;","&amp;AQ32:AQ41&amp;","&amp;AR32:AR41&amp;","&amp;AS32:AS41&amp;","&amp;AT32:AT41&amp;","&amp;AU32:AU41&amp;","&amp;AV32:AV41</f>
+        <f>AM33:AM41&amp;","&amp;AN33:AN41&amp;","&amp;AO33:AO41&amp;","&amp;AP33:AP41&amp;","&amp;AQ33:AQ41&amp;","&amp;AR33:AR41&amp;","&amp;AS33:AS41&amp;","&amp;AT33:AT41&amp;","&amp;AU33:AU41&amp;","&amp;AV33:AV41</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="38" customHeight="1" spans="3:50">
       <c r="C38" s="1">
-        <v>3030</v>
+        <v>3021</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E38" s="1">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
@@ -8007,7 +8057,7 @@
         <v>0</v>
       </c>
       <c r="R38" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="S38" s="1">
         <v>0</v>
@@ -8100,17 +8150,17 @@
         <v>0</v>
       </c>
       <c r="AW38" s="10" t="str">
-        <f>AC32:AC42&amp;","&amp;AD32:AD42&amp;","&amp;AE32:AE42&amp;","&amp;AF32:AF42&amp;","&amp;AG32:AG42&amp;","&amp;AH32:AH42&amp;","&amp;AI32:AI42&amp;","&amp;AJ32:AJ42&amp;","&amp;AK32:AK42&amp;","&amp;AL32:AL42</f>
+        <f>AC33:AC42&amp;","&amp;AD33:AD42&amp;","&amp;AE33:AE42&amp;","&amp;AF33:AF42&amp;","&amp;AG33:AG42&amp;","&amp;AH33:AH42&amp;","&amp;AI33:AI42&amp;","&amp;AJ33:AJ42&amp;","&amp;AK33:AK42&amp;","&amp;AL33:AL42</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX38" s="10" t="str">
-        <f>AM32:AM42&amp;","&amp;AN32:AN42&amp;","&amp;AO32:AO42&amp;","&amp;AP32:AP42&amp;","&amp;AQ32:AQ42&amp;","&amp;AR32:AR42&amp;","&amp;AS32:AS42&amp;","&amp;AT32:AT42&amp;","&amp;AU32:AU42&amp;","&amp;AV32:AV42</f>
+        <f>AM33:AM42&amp;","&amp;AN33:AN42&amp;","&amp;AO33:AO42&amp;","&amp;AP33:AP42&amp;","&amp;AQ33:AQ42&amp;","&amp;AR33:AR42&amp;","&amp;AS33:AS42&amp;","&amp;AT33:AT42&amp;","&amp;AU33:AU42&amp;","&amp;AV33:AV42</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="39" customHeight="1" spans="3:50">
       <c r="C39" s="1">
-        <v>3031</v>
+        <v>3030</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>145</v>
@@ -8155,7 +8205,7 @@
         <v>0</v>
       </c>
       <c r="R39" s="1">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="S39" s="1">
         <v>0</v>
@@ -8258,7 +8308,7 @@
     </row>
     <row r="40" customHeight="1" spans="3:50">
       <c r="C40" s="1">
-        <v>3032</v>
+        <v>3031</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>146</v>
@@ -8297,13 +8347,13 @@
         <v>0</v>
       </c>
       <c r="P40" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="Q40" s="1">
         <v>0</v>
       </c>
       <c r="R40" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="S40" s="1">
         <v>0</v>
@@ -8396,17 +8446,17 @@
         <v>0</v>
       </c>
       <c r="AW40" s="10" t="str">
-        <f t="shared" ref="AW40:AW45" si="2">AC34:AC46&amp;","&amp;AD34:AD46&amp;","&amp;AE34:AE46&amp;","&amp;AF34:AF46&amp;","&amp;AG34:AG46&amp;","&amp;AH34:AH46&amp;","&amp;AI34:AI46&amp;","&amp;AJ34:AJ46&amp;","&amp;AK34:AK46&amp;","&amp;AL34:AL46</f>
+        <f>AC34:AC44&amp;","&amp;AD34:AD44&amp;","&amp;AE34:AE44&amp;","&amp;AF34:AF44&amp;","&amp;AG34:AG44&amp;","&amp;AH34:AH44&amp;","&amp;AI34:AI44&amp;","&amp;AJ34:AJ44&amp;","&amp;AK34:AK44&amp;","&amp;AL34:AL44</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX40" s="10" t="str">
-        <f t="shared" ref="AX40:AX45" si="3">AM34:AM46&amp;","&amp;AN34:AN46&amp;","&amp;AO34:AO46&amp;","&amp;AP34:AP46&amp;","&amp;AQ34:AQ46&amp;","&amp;AR34:AR46&amp;","&amp;AS34:AS46&amp;","&amp;AT34:AT46&amp;","&amp;AU34:AU46&amp;","&amp;AV34:AV46</f>
+        <f>AM34:AM44&amp;","&amp;AN34:AN44&amp;","&amp;AO34:AO44&amp;","&amp;AP34:AP44&amp;","&amp;AQ34:AQ44&amp;","&amp;AR34:AR44&amp;","&amp;AS34:AS44&amp;","&amp;AT34:AT44&amp;","&amp;AU34:AU44&amp;","&amp;AV34:AV44</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="41" customHeight="1" spans="3:50">
       <c r="C41" s="1">
-        <v>3033</v>
+        <v>3032</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>147</v>
@@ -8445,7 +8495,7 @@
         <v>0</v>
       </c>
       <c r="P41" s="1">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="Q41" s="1">
         <v>0</v>
@@ -8544,17 +8594,17 @@
         <v>0</v>
       </c>
       <c r="AW41" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AW41:AW46" si="2">AC35:AC47&amp;","&amp;AD35:AD47&amp;","&amp;AE35:AE47&amp;","&amp;AF35:AF47&amp;","&amp;AG35:AG47&amp;","&amp;AH35:AH47&amp;","&amp;AI35:AI47&amp;","&amp;AJ35:AJ47&amp;","&amp;AK35:AK47&amp;","&amp;AL35:AL47</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX41" s="10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AX41:AX46" si="3">AM35:AM47&amp;","&amp;AN35:AN47&amp;","&amp;AO35:AO47&amp;","&amp;AP35:AP47&amp;","&amp;AQ35:AQ47&amp;","&amp;AR35:AR47&amp;","&amp;AS35:AS47&amp;","&amp;AT35:AT47&amp;","&amp;AU35:AU47&amp;","&amp;AV35:AV47</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="42" customHeight="1" spans="3:50">
       <c r="C42" s="1">
-        <v>3034</v>
+        <v>3033</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>148</v>
@@ -8584,7 +8634,7 @@
         <v>0</v>
       </c>
       <c r="M42" s="12">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="N42" s="1">
         <v>0</v>
@@ -8593,7 +8643,7 @@
         <v>0</v>
       </c>
       <c r="P42" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="Q42" s="1">
         <v>0</v>
@@ -8702,7 +8752,7 @@
     </row>
     <row r="43" customHeight="1" spans="3:50">
       <c r="C43" s="1">
-        <v>3035</v>
+        <v>3034</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>149</v>
@@ -8732,7 +8782,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="12">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="N43" s="1">
         <v>0</v>
@@ -8850,7 +8900,7 @@
     </row>
     <row r="44" customHeight="1" spans="3:50">
       <c r="C44" s="1">
-        <v>3036</v>
+        <v>3035</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>150</v>
@@ -8871,7 +8921,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K44" s="1">
         <v>0</v>
@@ -8879,8 +8929,8 @@
       <c r="L44" s="1">
         <v>0</v>
       </c>
-      <c r="M44" s="1">
-        <v>0</v>
+      <c r="M44" s="12">
+        <v>0.005</v>
       </c>
       <c r="N44" s="1">
         <v>0</v>
@@ -8998,7 +9048,7 @@
     </row>
     <row r="45" customHeight="1" spans="3:50">
       <c r="C45" s="1">
-        <v>3037</v>
+        <v>3036</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>151</v>
@@ -9019,7 +9069,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="1">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="K45" s="1">
         <v>0</v>
@@ -9146,7 +9196,7 @@
     </row>
     <row r="46" customHeight="1" spans="3:50">
       <c r="C46" s="1">
-        <v>3050</v>
+        <v>3037</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>152</v>
@@ -9167,7 +9217,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="K46" s="1">
         <v>0</v>
@@ -9175,7 +9225,7 @@
       <c r="L46" s="1">
         <v>0</v>
       </c>
-      <c r="M46" s="12">
+      <c r="M46" s="1">
         <v>0</v>
       </c>
       <c r="N46" s="1">
@@ -9227,7 +9277,7 @@
         <v>0</v>
       </c>
       <c r="AD46" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AE46" s="1">
         <v>0</v>
@@ -9284,17 +9334,17 @@
         <v>0</v>
       </c>
       <c r="AW46" s="10" t="str">
-        <f t="shared" ref="AW46:AW51" si="4">AC38:AC50&amp;","&amp;AD38:AD50&amp;","&amp;AE38:AE50&amp;","&amp;AF38:AF50&amp;","&amp;AG38:AG50&amp;","&amp;AH38:AH50&amp;","&amp;AI38:AI50&amp;","&amp;AJ38:AJ50&amp;","&amp;AK38:AK50&amp;","&amp;AL38:AL50</f>
-        <v>0,0.002,0,0,0,0,0,0,0,0</v>
+        <f t="shared" si="2"/>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX46" s="10" t="str">
-        <f t="shared" ref="AX46:AX51" si="5">AM38:AM50&amp;","&amp;AN38:AN50&amp;","&amp;AO38:AO50&amp;","&amp;AP38:AP50&amp;","&amp;AQ38:AQ50&amp;","&amp;AR38:AR50&amp;","&amp;AS38:AS50&amp;","&amp;AT38:AT50&amp;","&amp;AU38:AU50&amp;","&amp;AV38:AV50</f>
+        <f t="shared" si="3"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="47" customHeight="1" spans="3:50">
       <c r="C47" s="1">
-        <v>3051</v>
+        <v>3050</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>153</v>
@@ -9375,10 +9425,10 @@
         <v>0</v>
       </c>
       <c r="AD47" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="AE47" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AF47" s="1">
         <v>0</v>
@@ -9432,17 +9482,17 @@
         <v>0</v>
       </c>
       <c r="AW47" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>0,0,0.002,0,0,0,0,0,0,0</v>
+        <f t="shared" ref="AW47:AW52" si="4">AC39:AC51&amp;","&amp;AD39:AD51&amp;","&amp;AE39:AE51&amp;","&amp;AF39:AF51&amp;","&amp;AG39:AG51&amp;","&amp;AH39:AH51&amp;","&amp;AI39:AI51&amp;","&amp;AJ39:AJ51&amp;","&amp;AK39:AK51&amp;","&amp;AL39:AL51</f>
+        <v>0,0.002,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX47" s="10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AX47:AX52" si="5">AM39:AM51&amp;","&amp;AN39:AN51&amp;","&amp;AO39:AO51&amp;","&amp;AP39:AP51&amp;","&amp;AQ39:AQ51&amp;","&amp;AR39:AR51&amp;","&amp;AS39:AS51&amp;","&amp;AT39:AT51&amp;","&amp;AU39:AU51&amp;","&amp;AV39:AV51</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="48" customHeight="1" spans="3:50">
       <c r="C48" s="1">
-        <v>3052</v>
+        <v>3051</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>154</v>
@@ -9526,10 +9576,10 @@
         <v>0</v>
       </c>
       <c r="AE48" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="AF48" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AG48" s="1">
         <v>0</v>
@@ -9581,7 +9631,7 @@
       </c>
       <c r="AW48" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0.002,0,0,0,0,0,0</v>
+        <v>0,0,0.002,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX48" s="10" t="str">
         <f t="shared" si="5"/>
@@ -9590,7 +9640,7 @@
     </row>
     <row r="49" customHeight="1" spans="3:50">
       <c r="C49" s="1">
-        <v>3053</v>
+        <v>3052</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>155</v>
@@ -9677,10 +9727,10 @@
         <v>0</v>
       </c>
       <c r="AF49" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="AG49" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AH49" s="1">
         <v>0</v>
@@ -9729,7 +9779,7 @@
       </c>
       <c r="AW49" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,0.002,0,0,0,0,0</v>
+        <v>0,0,0,0.002,0,0,0,0,0,0</v>
       </c>
       <c r="AX49" s="10" t="str">
         <f t="shared" si="5"/>
@@ -9738,7 +9788,7 @@
     </row>
     <row r="50" customHeight="1" spans="3:50">
       <c r="C50" s="1">
-        <v>3054</v>
+        <v>3053</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>156</v>
@@ -9828,10 +9878,10 @@
         <v>0</v>
       </c>
       <c r="AG50" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="AH50" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AI50" s="1">
         <v>0</v>
@@ -9877,7 +9927,7 @@
       </c>
       <c r="AW50" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,0,0.002,0,0,0,0</v>
+        <v>0,0,0,0,0.002,0,0,0,0,0</v>
       </c>
       <c r="AX50" s="10" t="str">
         <f t="shared" si="5"/>
@@ -9886,7 +9936,7 @@
     </row>
     <row r="51" customHeight="1" spans="3:50">
       <c r="C51" s="1">
-        <v>3055</v>
+        <v>3054</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>157</v>
@@ -9979,10 +10029,10 @@
         <v>0</v>
       </c>
       <c r="AH51" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="AI51" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AJ51" s="1">
         <v>0</v>
@@ -10025,7 +10075,7 @@
       </c>
       <c r="AW51" s="10" t="str">
         <f t="shared" si="4"/>
-        <v>0,0,0,0,0,0,0.002,0,0,0</v>
+        <v>0,0,0,0,0,0.002,0,0,0,0</v>
       </c>
       <c r="AX51" s="10" t="str">
         <f t="shared" si="5"/>
@@ -10034,7 +10084,7 @@
     </row>
     <row r="52" customHeight="1" spans="3:50">
       <c r="C52" s="1">
-        <v>3056</v>
+        <v>3055</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>158</v>
@@ -10130,10 +10180,10 @@
         <v>0</v>
       </c>
       <c r="AI52" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="AJ52" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AK52" s="1">
         <v>0</v>
@@ -10172,17 +10222,17 @@
         <v>0</v>
       </c>
       <c r="AW52" s="10" t="str">
-        <f t="shared" ref="AW47:AW81" si="6">AC46:AC56&amp;","&amp;AD46:AD56&amp;","&amp;AE46:AE56&amp;","&amp;AF46:AF56&amp;","&amp;AG46:AG56&amp;","&amp;AH46:AH56&amp;","&amp;AI46:AI56&amp;","&amp;AJ46:AJ56&amp;","&amp;AK46:AK56&amp;","&amp;AL46:AL56</f>
-        <v>0,0,0,0,0,0,0,0.002,0,0</v>
+        <f t="shared" si="4"/>
+        <v>0,0,0,0,0,0,0.002,0,0,0</v>
       </c>
       <c r="AX52" s="10" t="str">
-        <f t="shared" ref="AX47:AX81" si="7">AM46:AM56&amp;","&amp;AN46:AN56&amp;","&amp;AO46:AO56&amp;","&amp;AP46:AP56&amp;","&amp;AQ46:AQ56&amp;","&amp;AR46:AR56&amp;","&amp;AS46:AS56&amp;","&amp;AT46:AT56&amp;","&amp;AU46:AU56&amp;","&amp;AV46:AV56</f>
+        <f t="shared" si="5"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="53" customHeight="1" spans="3:50">
       <c r="C53" s="1">
-        <v>3057</v>
+        <v>3056</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>159</v>
@@ -10281,10 +10331,10 @@
         <v>0</v>
       </c>
       <c r="AJ53" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="AK53" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AL53" s="1">
         <v>0</v>
@@ -10320,17 +10370,17 @@
         <v>0</v>
       </c>
       <c r="AW53" s="10" t="str">
-        <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0,0.002,0</v>
+        <f t="shared" ref="AW48:AW82" si="6">AC47:AC57&amp;","&amp;AD47:AD57&amp;","&amp;AE47:AE57&amp;","&amp;AF47:AF57&amp;","&amp;AG47:AG57&amp;","&amp;AH47:AH57&amp;","&amp;AI47:AI57&amp;","&amp;AJ47:AJ57&amp;","&amp;AK47:AK57&amp;","&amp;AL47:AL57</f>
+        <v>0,0,0,0,0,0,0,0.002,0,0</v>
       </c>
       <c r="AX53" s="10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="AX48:AX82" si="7">AM47:AM57&amp;","&amp;AN47:AN57&amp;","&amp;AO47:AO57&amp;","&amp;AP47:AP57&amp;","&amp;AQ47:AQ57&amp;","&amp;AR47:AR57&amp;","&amp;AS47:AS57&amp;","&amp;AT47:AT57&amp;","&amp;AU47:AU57&amp;","&amp;AV47:AV57</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="54" customHeight="1" spans="3:50">
       <c r="C54" s="1">
-        <v>3058</v>
+        <v>3057</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>160</v>
@@ -10432,10 +10482,10 @@
         <v>0</v>
       </c>
       <c r="AK54" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="AL54" s="1">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AM54" s="1">
         <v>0</v>
@@ -10469,7 +10519,7 @@
       </c>
       <c r="AW54" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0,0,0.002</v>
+        <v>0,0,0,0,0,0,0,0,0.002,0</v>
       </c>
       <c r="AX54" s="10" t="str">
         <f t="shared" si="7"/>
@@ -10478,7 +10528,7 @@
     </row>
     <row r="55" customHeight="1" spans="3:50">
       <c r="C55" s="1">
-        <v>3059</v>
+        <v>3058</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>161</v>
@@ -10559,7 +10609,7 @@
         <v>0</v>
       </c>
       <c r="AD55" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="AE55" s="1">
         <v>0</v>
@@ -10583,7 +10633,7 @@
         <v>0</v>
       </c>
       <c r="AL55" s="1">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="AM55" s="1">
         <v>0</v>
@@ -10617,7 +10667,7 @@
       </c>
       <c r="AW55" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0.005,0,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0,0.002</v>
       </c>
       <c r="AX55" s="10" t="str">
         <f t="shared" si="7"/>
@@ -10626,7 +10676,7 @@
     </row>
     <row r="56" customHeight="1" spans="3:50">
       <c r="C56" s="1">
-        <v>3060</v>
+        <v>3059</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>162</v>
@@ -10707,10 +10757,10 @@
         <v>0</v>
       </c>
       <c r="AD56" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="AE56" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="AF56" s="1">
         <v>0</v>
@@ -10765,7 +10815,7 @@
       </c>
       <c r="AW56" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0.005,0,0,0,0,0,0,0</v>
+        <v>0,0.005,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX56" s="10" t="str">
         <f t="shared" si="7"/>
@@ -10774,7 +10824,7 @@
     </row>
     <row r="57" customHeight="1" spans="3:50">
       <c r="C57" s="1">
-        <v>3061</v>
+        <v>3060</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>163</v>
@@ -10858,10 +10908,10 @@
         <v>0</v>
       </c>
       <c r="AE57" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="AF57" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="AG57" s="1">
         <v>0</v>
@@ -10913,7 +10963,7 @@
       </c>
       <c r="AW57" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0.005,0,0,0,0,0,0</v>
+        <v>0,0,0.005,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX57" s="10" t="str">
         <f t="shared" si="7"/>
@@ -10922,7 +10972,7 @@
     </row>
     <row r="58" customHeight="1" spans="3:50">
       <c r="C58" s="1">
-        <v>3062</v>
+        <v>3061</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>164</v>
@@ -11009,10 +11059,10 @@
         <v>0</v>
       </c>
       <c r="AF58" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="AG58" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="AH58" s="1">
         <v>0</v>
@@ -11061,7 +11111,7 @@
       </c>
       <c r="AW58" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0.005,0,0,0,0,0</v>
+        <v>0,0,0,0.005,0,0,0,0,0,0</v>
       </c>
       <c r="AX58" s="10" t="str">
         <f t="shared" si="7"/>
@@ -11070,7 +11120,7 @@
     </row>
     <row r="59" customHeight="1" spans="3:50">
       <c r="C59" s="1">
-        <v>3063</v>
+        <v>3062</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>165</v>
@@ -11160,10 +11210,10 @@
         <v>0</v>
       </c>
       <c r="AG59" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="AH59" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="AI59" s="1">
         <v>0</v>
@@ -11209,7 +11259,7 @@
       </c>
       <c r="AW59" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0.005,0,0,0,0</v>
+        <v>0,0,0,0,0.005,0,0,0,0,0</v>
       </c>
       <c r="AX59" s="10" t="str">
         <f t="shared" si="7"/>
@@ -11218,7 +11268,7 @@
     </row>
     <row r="60" customHeight="1" spans="3:50">
       <c r="C60" s="1">
-        <v>3064</v>
+        <v>3063</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>166</v>
@@ -11311,10 +11361,10 @@
         <v>0</v>
       </c>
       <c r="AH60" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="AI60" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="AJ60" s="1">
         <v>0</v>
@@ -11357,7 +11407,7 @@
       </c>
       <c r="AW60" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0.005,0,0,0</v>
+        <v>0,0,0,0,0,0.005,0,0,0,0</v>
       </c>
       <c r="AX60" s="10" t="str">
         <f t="shared" si="7"/>
@@ -11366,7 +11416,7 @@
     </row>
     <row r="61" customHeight="1" spans="3:50">
       <c r="C61" s="1">
-        <v>3065</v>
+        <v>3064</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>167</v>
@@ -11462,10 +11512,10 @@
         <v>0</v>
       </c>
       <c r="AI61" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="AJ61" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="AK61" s="1">
         <v>0</v>
@@ -11505,7 +11555,7 @@
       </c>
       <c r="AW61" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0.005,0,0</v>
+        <v>0,0,0,0,0,0,0.005,0,0,0</v>
       </c>
       <c r="AX61" s="10" t="str">
         <f t="shared" si="7"/>
@@ -11514,7 +11564,7 @@
     </row>
     <row r="62" customHeight="1" spans="3:50">
       <c r="C62" s="1">
-        <v>3066</v>
+        <v>3065</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>168</v>
@@ -11613,10 +11663,10 @@
         <v>0</v>
       </c>
       <c r="AJ62" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="AK62" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="AL62" s="1">
         <v>0</v>
@@ -11653,7 +11703,7 @@
       </c>
       <c r="AW62" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0,0.005,0</v>
+        <v>0,0,0,0,0,0,0,0.005,0,0</v>
       </c>
       <c r="AX62" s="10" t="str">
         <f t="shared" si="7"/>
@@ -11662,7 +11712,7 @@
     </row>
     <row r="63" customHeight="1" spans="3:50">
       <c r="C63" s="1">
-        <v>3067</v>
+        <v>3066</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>169</v>
@@ -11764,10 +11814,10 @@
         <v>0</v>
       </c>
       <c r="AK63" s="1">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="AL63" s="1">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="AM63" s="1">
         <v>0</v>
@@ -11801,164 +11851,164 @@
       </c>
       <c r="AW63" s="10" t="str">
         <f t="shared" si="6"/>
-        <v>0,0,0,0,0,0,0,0,0,0.005</v>
+        <v>0,0,0,0,0,0,0,0,0.005,0</v>
       </c>
       <c r="AX63" s="10" t="str">
         <f t="shared" si="7"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="64" s="2" customFormat="1" customHeight="1" spans="3:50">
-      <c r="C64" s="2">
-        <v>3068</v>
-      </c>
-      <c r="D64" s="2" t="s">
+    <row r="64" customHeight="1" spans="3:50">
+      <c r="C64" s="1">
+        <v>3067</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E64" s="2">
-        <v>0</v>
-      </c>
-      <c r="F64" s="2">
-        <v>0</v>
-      </c>
-      <c r="G64" s="2">
-        <v>0</v>
-      </c>
-      <c r="H64" s="2">
-        <v>0</v>
-      </c>
-      <c r="I64" s="2">
-        <v>0</v>
-      </c>
-      <c r="J64" s="2">
-        <v>0</v>
-      </c>
-      <c r="K64" s="2">
-        <v>0</v>
-      </c>
-      <c r="L64" s="2">
-        <v>0</v>
-      </c>
-      <c r="M64" s="16">
-        <v>0</v>
-      </c>
-      <c r="N64" s="2">
-        <v>0</v>
-      </c>
-      <c r="O64" s="2">
-        <v>0</v>
-      </c>
-      <c r="P64" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q64" s="2">
-        <v>0</v>
-      </c>
-      <c r="R64" s="2">
-        <v>0</v>
-      </c>
-      <c r="S64" s="2">
-        <v>0</v>
-      </c>
-      <c r="T64" s="2">
-        <v>0</v>
-      </c>
-      <c r="U64" s="2">
-        <v>0</v>
-      </c>
-      <c r="V64" s="2">
-        <v>0</v>
-      </c>
-      <c r="W64" s="2">
-        <v>0</v>
-      </c>
-      <c r="X64" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y64" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA64" s="2">
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0</v>
+      </c>
+      <c r="K64" s="1">
+        <v>0</v>
+      </c>
+      <c r="L64" s="1">
+        <v>0</v>
+      </c>
+      <c r="M64" s="12">
+        <v>0</v>
+      </c>
+      <c r="N64" s="1">
+        <v>0</v>
+      </c>
+      <c r="O64" s="1">
+        <v>0</v>
+      </c>
+      <c r="P64" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>0</v>
+      </c>
+      <c r="R64" s="1">
+        <v>0</v>
+      </c>
+      <c r="S64" s="1">
+        <v>0</v>
+      </c>
+      <c r="T64" s="1">
+        <v>0</v>
+      </c>
+      <c r="U64" s="1">
+        <v>0</v>
+      </c>
+      <c r="V64" s="1">
+        <v>0</v>
+      </c>
+      <c r="W64" s="1">
+        <v>0</v>
+      </c>
+      <c r="X64" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y64" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA64" s="1">
         <v>0</v>
       </c>
       <c r="AB64" s="1">
         <v>0</v>
       </c>
-      <c r="AC64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM64" s="2">
+      <c r="AC64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL64" s="1">
+        <v>0.005</v>
+      </c>
+      <c r="AM64" s="1">
         <v>0</v>
       </c>
       <c r="AN64" s="1">
-        <v>0.002</v>
-      </c>
-      <c r="AO64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV64" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW64" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="AO64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV64" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW64" s="10" t="str">
         <f t="shared" si="6"/>
+        <v>0,0,0,0,0,0,0,0,0,0.005</v>
+      </c>
+      <c r="AX64" s="10" t="str">
+        <f t="shared" si="7"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
-      </c>
-      <c r="AX64" s="19" t="str">
-        <f t="shared" si="7"/>
-        <v>0,0.002,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="65" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C65" s="2">
-        <v>3069</v>
+        <v>3068</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>171</v>
@@ -11987,7 +12037,7 @@
       <c r="L65" s="2">
         <v>0</v>
       </c>
-      <c r="M65" s="16">
+      <c r="M65" s="19">
         <v>0</v>
       </c>
       <c r="N65" s="2">
@@ -12068,12 +12118,12 @@
       <c r="AM65" s="2">
         <v>0</v>
       </c>
-      <c r="AN65" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO65" s="1">
+      <c r="AN65" s="1">
         <v>0.002</v>
       </c>
+      <c r="AO65" s="2">
+        <v>0</v>
+      </c>
       <c r="AP65" s="2">
         <v>0</v>
       </c>
@@ -12095,18 +12145,18 @@
       <c r="AV65" s="2">
         <v>0</v>
       </c>
-      <c r="AW65" s="19" t="str">
+      <c r="AW65" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX65" s="19" t="str">
+      <c r="AX65" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0.002,0,0,0,0,0,0,0</v>
+        <v>0,0.002,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="66" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C66" s="2">
-        <v>3070</v>
+        <v>3069</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>172</v>
@@ -12135,7 +12185,7 @@
       <c r="L66" s="2">
         <v>0</v>
       </c>
-      <c r="M66" s="16">
+      <c r="M66" s="19">
         <v>0</v>
       </c>
       <c r="N66" s="2">
@@ -12219,12 +12269,12 @@
       <c r="AN66" s="2">
         <v>0</v>
       </c>
-      <c r="AO66" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP66" s="1">
+      <c r="AO66" s="1">
         <v>0.002</v>
       </c>
+      <c r="AP66" s="2">
+        <v>0</v>
+      </c>
       <c r="AQ66" s="2">
         <v>0</v>
       </c>
@@ -12243,18 +12293,18 @@
       <c r="AV66" s="2">
         <v>0</v>
       </c>
-      <c r="AW66" s="19" t="str">
+      <c r="AW66" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX66" s="19" t="str">
+      <c r="AX66" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0.002,0,0,0,0,0,0</v>
+        <v>0,0,0.002,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="67" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C67" s="2">
-        <v>3071</v>
+        <v>3070</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>173</v>
@@ -12283,7 +12333,7 @@
       <c r="L67" s="2">
         <v>0</v>
       </c>
-      <c r="M67" s="16">
+      <c r="M67" s="19">
         <v>0</v>
       </c>
       <c r="N67" s="2">
@@ -12370,12 +12420,12 @@
       <c r="AO67" s="2">
         <v>0</v>
       </c>
-      <c r="AP67" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ67" s="1">
+      <c r="AP67" s="1">
         <v>0.002</v>
       </c>
+      <c r="AQ67" s="2">
+        <v>0</v>
+      </c>
       <c r="AR67" s="2">
         <v>0</v>
       </c>
@@ -12391,18 +12441,18 @@
       <c r="AV67" s="2">
         <v>0</v>
       </c>
-      <c r="AW67" s="19" t="str">
+      <c r="AW67" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX67" s="19" t="str">
+      <c r="AX67" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0.002,0,0,0,0,0</v>
+        <v>0,0,0,0.002,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="68" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C68" s="2">
-        <v>3072</v>
+        <v>3071</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>174</v>
@@ -12431,7 +12481,7 @@
       <c r="L68" s="2">
         <v>0</v>
       </c>
-      <c r="M68" s="16">
+      <c r="M68" s="19">
         <v>0</v>
       </c>
       <c r="N68" s="2">
@@ -12521,12 +12571,12 @@
       <c r="AP68" s="2">
         <v>0</v>
       </c>
-      <c r="AQ68" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR68" s="1">
+      <c r="AQ68" s="1">
         <v>0.002</v>
       </c>
+      <c r="AR68" s="2">
+        <v>0</v>
+      </c>
       <c r="AS68" s="2">
         <v>0</v>
       </c>
@@ -12539,18 +12589,18 @@
       <c r="AV68" s="2">
         <v>0</v>
       </c>
-      <c r="AW68" s="19" t="str">
+      <c r="AW68" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX68" s="19" t="str">
+      <c r="AX68" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0.002,0,0,0,0</v>
+        <v>0,0,0,0,0.002,0,0,0,0,0</v>
       </c>
     </row>
     <row r="69" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C69" s="2">
-        <v>3073</v>
+        <v>3072</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>175</v>
@@ -12579,7 +12629,7 @@
       <c r="L69" s="2">
         <v>0</v>
       </c>
-      <c r="M69" s="16">
+      <c r="M69" s="19">
         <v>0</v>
       </c>
       <c r="N69" s="2">
@@ -12672,12 +12722,12 @@
       <c r="AQ69" s="2">
         <v>0</v>
       </c>
-      <c r="AR69" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS69" s="1">
+      <c r="AR69" s="1">
         <v>0.002</v>
       </c>
+      <c r="AS69" s="2">
+        <v>0</v>
+      </c>
       <c r="AT69" s="2">
         <v>0</v>
       </c>
@@ -12687,18 +12737,18 @@
       <c r="AV69" s="2">
         <v>0</v>
       </c>
-      <c r="AW69" s="19" t="str">
+      <c r="AW69" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX69" s="19" t="str">
+      <c r="AX69" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0.002,0,0,0</v>
+        <v>0,0,0,0,0,0.002,0,0,0,0</v>
       </c>
     </row>
     <row r="70" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C70" s="2">
-        <v>3074</v>
+        <v>3073</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>176</v>
@@ -12727,7 +12777,7 @@
       <c r="L70" s="2">
         <v>0</v>
       </c>
-      <c r="M70" s="16">
+      <c r="M70" s="19">
         <v>0</v>
       </c>
       <c r="N70" s="2">
@@ -12823,30 +12873,30 @@
       <c r="AR70" s="2">
         <v>0</v>
       </c>
-      <c r="AS70" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT70" s="1">
+      <c r="AS70" s="1">
         <v>0.002</v>
       </c>
+      <c r="AT70" s="2">
+        <v>0</v>
+      </c>
       <c r="AU70" s="2">
         <v>0</v>
       </c>
       <c r="AV70" s="2">
         <v>0</v>
       </c>
-      <c r="AW70" s="19" t="str">
+      <c r="AW70" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX70" s="19" t="str">
+      <c r="AX70" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0.002,0,0</v>
+        <v>0,0,0,0,0,0,0.002,0,0,0</v>
       </c>
     </row>
     <row r="71" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C71" s="2">
-        <v>3075</v>
+        <v>3074</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>177</v>
@@ -12875,7 +12925,7 @@
       <c r="L71" s="2">
         <v>0</v>
       </c>
-      <c r="M71" s="16">
+      <c r="M71" s="19">
         <v>0</v>
       </c>
       <c r="N71" s="2">
@@ -12974,27 +13024,27 @@
       <c r="AS71" s="2">
         <v>0</v>
       </c>
-      <c r="AT71" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU71" s="1">
+      <c r="AT71" s="1">
         <v>0.002</v>
       </c>
+      <c r="AU71" s="2">
+        <v>0</v>
+      </c>
       <c r="AV71" s="2">
         <v>0</v>
       </c>
-      <c r="AW71" s="19" t="str">
+      <c r="AW71" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX71" s="19" t="str">
+      <c r="AX71" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0,0.002,0</v>
+        <v>0,0,0,0,0,0,0,0.002,0,0</v>
       </c>
     </row>
     <row r="72" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C72" s="2">
-        <v>3076</v>
+        <v>3075</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>178</v>
@@ -13023,7 +13073,7 @@
       <c r="L72" s="2">
         <v>0</v>
       </c>
-      <c r="M72" s="16">
+      <c r="M72" s="19">
         <v>0</v>
       </c>
       <c r="N72" s="2">
@@ -13125,24 +13175,24 @@
       <c r="AT72" s="2">
         <v>0</v>
       </c>
-      <c r="AU72" s="2">
-        <v>0</v>
+      <c r="AU72" s="1">
+        <v>0.002</v>
       </c>
       <c r="AV72" s="2">
-        <v>20</v>
-      </c>
-      <c r="AW72" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="AW72" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX72" s="19" t="str">
+      <c r="AX72" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0,0,20</v>
+        <v>0,0,0,0,0,0,0,0,0.002,0</v>
       </c>
     </row>
     <row r="73" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C73" s="2">
-        <v>3077</v>
+        <v>3076</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>179</v>
@@ -13171,7 +13221,7 @@
       <c r="L73" s="2">
         <v>0</v>
       </c>
-      <c r="M73" s="12">
+      <c r="M73" s="19">
         <v>0</v>
       </c>
       <c r="N73" s="2">
@@ -13252,8 +13302,8 @@
       <c r="AM73" s="2">
         <v>0</v>
       </c>
-      <c r="AN73" s="1">
-        <v>0.005</v>
+      <c r="AN73" s="2">
+        <v>0</v>
       </c>
       <c r="AO73" s="2">
         <v>0</v>
@@ -13277,20 +13327,20 @@
         <v>0</v>
       </c>
       <c r="AV73" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW73" s="19" t="str">
+        <v>20</v>
+      </c>
+      <c r="AW73" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX73" s="19" t="str">
+      <c r="AX73" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0.005,0,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0,20</v>
       </c>
     </row>
     <row r="74" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C74" s="2">
-        <v>3078</v>
+        <v>3077</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>180</v>
@@ -13400,12 +13450,12 @@
       <c r="AM74" s="2">
         <v>0</v>
       </c>
-      <c r="AN74" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO74" s="1">
+      <c r="AN74" s="1">
         <v>0.005</v>
       </c>
+      <c r="AO74" s="2">
+        <v>0</v>
+      </c>
       <c r="AP74" s="2">
         <v>0</v>
       </c>
@@ -13427,18 +13477,18 @@
       <c r="AV74" s="2">
         <v>0</v>
       </c>
-      <c r="AW74" s="19" t="str">
+      <c r="AW74" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX74" s="19" t="str">
+      <c r="AX74" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0.005,0,0,0,0,0,0,0</v>
+        <v>0,0.005,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="75" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C75" s="2">
-        <v>3079</v>
+        <v>3078</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>181</v>
@@ -13551,12 +13601,12 @@
       <c r="AN75" s="2">
         <v>0</v>
       </c>
-      <c r="AO75" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP75" s="1">
+      <c r="AO75" s="1">
         <v>0.005</v>
       </c>
+      <c r="AP75" s="2">
+        <v>0</v>
+      </c>
       <c r="AQ75" s="2">
         <v>0</v>
       </c>
@@ -13575,18 +13625,18 @@
       <c r="AV75" s="2">
         <v>0</v>
       </c>
-      <c r="AW75" s="19" t="str">
+      <c r="AW75" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX75" s="19" t="str">
+      <c r="AX75" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0.005,0,0,0,0,0,0</v>
+        <v>0,0,0.005,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="76" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C76" s="2">
-        <v>3080</v>
+        <v>3079</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>182</v>
@@ -13702,12 +13752,12 @@
       <c r="AO76" s="2">
         <v>0</v>
       </c>
-      <c r="AP76" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ76" s="1">
+      <c r="AP76" s="1">
         <v>0.005</v>
       </c>
+      <c r="AQ76" s="2">
+        <v>0</v>
+      </c>
       <c r="AR76" s="2">
         <v>0</v>
       </c>
@@ -13723,18 +13773,18 @@
       <c r="AV76" s="2">
         <v>0</v>
       </c>
-      <c r="AW76" s="19" t="str">
+      <c r="AW76" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX76" s="19" t="str">
+      <c r="AX76" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0.005,0,0,0,0,0</v>
+        <v>0,0,0,0.005,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="77" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C77" s="2">
-        <v>3081</v>
+        <v>3080</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>183</v>
@@ -13853,12 +13903,12 @@
       <c r="AP77" s="2">
         <v>0</v>
       </c>
-      <c r="AQ77" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR77" s="1">
+      <c r="AQ77" s="1">
         <v>0.005</v>
       </c>
+      <c r="AR77" s="2">
+        <v>0</v>
+      </c>
       <c r="AS77" s="2">
         <v>0</v>
       </c>
@@ -13871,18 +13921,18 @@
       <c r="AV77" s="2">
         <v>0</v>
       </c>
-      <c r="AW77" s="19" t="str">
+      <c r="AW77" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX77" s="19" t="str">
+      <c r="AX77" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0.005,0,0,0,0</v>
+        <v>0,0,0,0,0.005,0,0,0,0,0</v>
       </c>
     </row>
     <row r="78" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C78" s="2">
-        <v>3082</v>
+        <v>3081</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>184</v>
@@ -14004,12 +14054,12 @@
       <c r="AQ78" s="2">
         <v>0</v>
       </c>
-      <c r="AR78" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS78" s="1">
+      <c r="AR78" s="1">
         <v>0.005</v>
       </c>
+      <c r="AS78" s="2">
+        <v>0</v>
+      </c>
       <c r="AT78" s="2">
         <v>0</v>
       </c>
@@ -14019,18 +14069,18 @@
       <c r="AV78" s="2">
         <v>0</v>
       </c>
-      <c r="AW78" s="19" t="str">
+      <c r="AW78" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX78" s="19" t="str">
+      <c r="AX78" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0.005,0,0,0</v>
+        <v>0,0,0,0,0,0.005,0,0,0,0</v>
       </c>
     </row>
     <row r="79" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C79" s="2">
-        <v>3083</v>
+        <v>3082</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>185</v>
@@ -14155,30 +14205,30 @@
       <c r="AR79" s="2">
         <v>0</v>
       </c>
-      <c r="AS79" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT79" s="1">
+      <c r="AS79" s="1">
         <v>0.005</v>
       </c>
+      <c r="AT79" s="2">
+        <v>0</v>
+      </c>
       <c r="AU79" s="2">
         <v>0</v>
       </c>
       <c r="AV79" s="2">
         <v>0</v>
       </c>
-      <c r="AW79" s="19" t="str">
+      <c r="AW79" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX79" s="19" t="str">
+      <c r="AX79" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0.005,0,0</v>
+        <v>0,0,0,0,0,0,0.005,0,0,0</v>
       </c>
     </row>
     <row r="80" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C80" s="2">
-        <v>3084</v>
+        <v>3083</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>186</v>
@@ -14306,27 +14356,27 @@
       <c r="AS80" s="2">
         <v>0</v>
       </c>
-      <c r="AT80" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU80" s="1">
+      <c r="AT80" s="1">
         <v>0.005</v>
       </c>
+      <c r="AU80" s="2">
+        <v>0</v>
+      </c>
       <c r="AV80" s="2">
         <v>0</v>
       </c>
-      <c r="AW80" s="19" t="str">
+      <c r="AW80" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX80" s="19" t="str">
+      <c r="AX80" s="20" t="str">
         <f t="shared" si="7"/>
-        <v>0,0,0,0,0,0,0,0,0.005,0</v>
+        <v>0,0,0,0,0,0,0,0.005,0,0</v>
       </c>
     </row>
     <row r="81" s="2" customFormat="1" customHeight="1" spans="3:50">
       <c r="C81" s="2">
-        <v>3085</v>
+        <v>3084</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>187</v>
@@ -14457,184 +14507,184 @@
       <c r="AT81" s="2">
         <v>0</v>
       </c>
-      <c r="AU81" s="2">
-        <v>0</v>
+      <c r="AU81" s="1">
+        <v>0.005</v>
       </c>
       <c r="AV81" s="2">
-        <v>50</v>
-      </c>
-      <c r="AW81" s="19" t="str">
+        <v>0</v>
+      </c>
+      <c r="AW81" s="20" t="str">
         <f t="shared" si="6"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
-      <c r="AX81" s="19" t="str">
+      <c r="AX81" s="20" t="str">
+        <f t="shared" si="7"/>
+        <v>0,0,0,0,0,0,0,0,0.005,0</v>
+      </c>
+    </row>
+    <row r="82" s="2" customFormat="1" customHeight="1" spans="3:50">
+      <c r="C82" s="2">
+        <v>3085</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E82" s="2">
+        <v>0</v>
+      </c>
+      <c r="F82" s="2">
+        <v>0</v>
+      </c>
+      <c r="G82" s="2">
+        <v>0</v>
+      </c>
+      <c r="H82" s="2">
+        <v>0</v>
+      </c>
+      <c r="I82" s="2">
+        <v>0</v>
+      </c>
+      <c r="J82" s="2">
+        <v>0</v>
+      </c>
+      <c r="K82" s="2">
+        <v>0</v>
+      </c>
+      <c r="L82" s="2">
+        <v>0</v>
+      </c>
+      <c r="M82" s="12">
+        <v>0</v>
+      </c>
+      <c r="N82" s="2">
+        <v>0</v>
+      </c>
+      <c r="O82" s="2">
+        <v>0</v>
+      </c>
+      <c r="P82" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="2">
+        <v>0</v>
+      </c>
+      <c r="R82" s="2">
+        <v>0</v>
+      </c>
+      <c r="S82" s="2">
+        <v>0</v>
+      </c>
+      <c r="T82" s="2">
+        <v>0</v>
+      </c>
+      <c r="U82" s="2">
+        <v>0</v>
+      </c>
+      <c r="V82" s="2">
+        <v>0</v>
+      </c>
+      <c r="W82" s="2">
+        <v>0</v>
+      </c>
+      <c r="X82" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y82" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB82" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU82" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV82" s="2">
+        <v>50</v>
+      </c>
+      <c r="AW82" s="20" t="str">
+        <f t="shared" si="6"/>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
+      </c>
+      <c r="AX82" s="20" t="str">
         <f t="shared" si="7"/>
         <v>0,0,0,0,0,0,0,0,0,50</v>
-      </c>
-    </row>
-    <row r="82" customHeight="1" spans="3:50">
-      <c r="C82" s="1">
-        <v>3200</v>
-      </c>
-      <c r="D82" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="E82" s="1">
-        <v>180</v>
-      </c>
-      <c r="F82" s="1">
-        <v>0</v>
-      </c>
-      <c r="G82" s="1">
-        <v>0</v>
-      </c>
-      <c r="H82" s="1">
-        <v>0</v>
-      </c>
-      <c r="I82" s="1">
-        <v>0</v>
-      </c>
-      <c r="J82" s="1">
-        <v>0</v>
-      </c>
-      <c r="K82" s="1">
-        <v>0</v>
-      </c>
-      <c r="L82" s="1">
-        <v>0</v>
-      </c>
-      <c r="M82" s="12">
-        <v>0</v>
-      </c>
-      <c r="N82" s="1">
-        <v>0</v>
-      </c>
-      <c r="O82" s="1">
-        <v>0</v>
-      </c>
-      <c r="P82" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q82" s="1">
-        <v>0</v>
-      </c>
-      <c r="R82" s="1">
-        <v>0</v>
-      </c>
-      <c r="S82" s="1">
-        <v>0</v>
-      </c>
-      <c r="T82" s="1">
-        <v>0</v>
-      </c>
-      <c r="U82" s="1">
-        <v>0</v>
-      </c>
-      <c r="V82" s="1">
-        <v>0</v>
-      </c>
-      <c r="W82" s="1">
-        <v>0</v>
-      </c>
-      <c r="X82" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y82" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD82" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV82" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW82" s="10" t="str">
-        <f t="shared" ref="AW82:AW95" si="8">AC76:AC86&amp;","&amp;AD76:AD86&amp;","&amp;AE76:AE86&amp;","&amp;AF76:AF86&amp;","&amp;AG76:AG86&amp;","&amp;AH76:AH86&amp;","&amp;AI76:AI86&amp;","&amp;AJ76:AJ86&amp;","&amp;AK76:AK86&amp;","&amp;AL76:AL86</f>
-        <v>0,0,0,0,0,0,0,0,0,0</v>
-      </c>
-      <c r="AX82" s="10" t="str">
-        <f t="shared" ref="AX82:AX95" si="9">AM76:AM86&amp;","&amp;AN76:AN86&amp;","&amp;AO76:AO86&amp;","&amp;AP76:AP86&amp;","&amp;AQ76:AQ86&amp;","&amp;AR76:AR86&amp;","&amp;AS76:AS86&amp;","&amp;AT76:AT86&amp;","&amp;AU76:AU86&amp;","&amp;AV76:AV86</f>
-        <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="83" customHeight="1" spans="3:50">
       <c r="C83" s="1">
-        <v>3201</v>
-      </c>
-      <c r="D83" s="1" t="s">
+        <v>3200</v>
+      </c>
+      <c r="D83" s="18" t="s">
         <v>189</v>
       </c>
       <c r="E83" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F83" s="1">
         <v>0</v>
       </c>
       <c r="G83" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="H83" s="1">
         <v>0</v>
@@ -14760,17 +14810,17 @@
         <v>0</v>
       </c>
       <c r="AW83" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="AW83:AW96" si="8">AC77:AC87&amp;","&amp;AD77:AD87&amp;","&amp;AE77:AE87&amp;","&amp;AF77:AF87&amp;","&amp;AG77:AG87&amp;","&amp;AH77:AH87&amp;","&amp;AI77:AI87&amp;","&amp;AJ77:AJ87&amp;","&amp;AK77:AK87&amp;","&amp;AL77:AL87</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX83" s="10" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="AX83:AX96" si="9">AM77:AM87&amp;","&amp;AN77:AN87&amp;","&amp;AO77:AO87&amp;","&amp;AP77:AP87&amp;","&amp;AQ77:AQ87&amp;","&amp;AR77:AR87&amp;","&amp;AS77:AS87&amp;","&amp;AT77:AT87&amp;","&amp;AU77:AU87&amp;","&amp;AV77:AV87</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="84" customHeight="1" spans="3:50">
       <c r="C84" s="1">
-        <v>3202</v>
+        <v>3201</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>190</v>
@@ -14782,7 +14832,7 @@
         <v>0</v>
       </c>
       <c r="G84" s="1">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="H84" s="1">
         <v>0</v>
@@ -14824,7 +14874,7 @@
         <v>0</v>
       </c>
       <c r="U84" s="1">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="V84" s="1">
         <v>0</v>
@@ -14918,7 +14968,7 @@
     </row>
     <row r="85" customHeight="1" spans="3:50">
       <c r="C85" s="1">
-        <v>3203</v>
+        <v>3202</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>191</v>
@@ -14927,7 +14977,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="1">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="G85" s="1">
         <v>0</v>
@@ -14972,7 +15022,7 @@
         <v>0</v>
       </c>
       <c r="U85" s="1">
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="V85" s="1">
         <v>0</v>
@@ -14998,7 +15048,7 @@
       <c r="AC85" s="1">
         <v>0</v>
       </c>
-      <c r="AD85" s="1">
+      <c r="AD85" s="2">
         <v>0</v>
       </c>
       <c r="AE85" s="1">
@@ -15066,7 +15116,7 @@
     </row>
     <row r="86" customHeight="1" spans="3:50">
       <c r="C86" s="1">
-        <v>3204</v>
+        <v>3203</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>192</v>
@@ -15075,13 +15125,13 @@
         <v>0</v>
       </c>
       <c r="F86" s="1">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="G86" s="1">
         <v>0</v>
       </c>
       <c r="H86" s="1">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="I86" s="1">
         <v>0</v>
@@ -15214,7 +15264,7 @@
     </row>
     <row r="87" customHeight="1" spans="3:50">
       <c r="C87" s="1">
-        <v>3205</v>
+        <v>3204</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>193</v>
@@ -15229,7 +15279,7 @@
         <v>0</v>
       </c>
       <c r="H87" s="1">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="I87" s="1">
         <v>0</v>
@@ -15271,7 +15321,7 @@
         <v>0</v>
       </c>
       <c r="V87" s="1">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="W87" s="1">
         <v>0</v>
@@ -15362,7 +15412,7 @@
     </row>
     <row r="88" customHeight="1" spans="3:50">
       <c r="C88" s="1">
-        <v>3206</v>
+        <v>3205</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>194</v>
@@ -15410,7 +15460,7 @@
         <v>0</v>
       </c>
       <c r="S88" s="1">
-        <v>850</v>
+        <v>0</v>
       </c>
       <c r="T88" s="1">
         <v>0</v>
@@ -15419,7 +15469,7 @@
         <v>0</v>
       </c>
       <c r="V88" s="1">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="W88" s="1">
         <v>0</v>
@@ -15510,7 +15560,7 @@
     </row>
     <row r="89" customHeight="1" spans="3:50">
       <c r="C89" s="1">
-        <v>3207</v>
+        <v>3206</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>195</v>
@@ -15558,10 +15608,10 @@
         <v>0</v>
       </c>
       <c r="S89" s="1">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="T89" s="1">
-        <v>850</v>
+        <v>0</v>
       </c>
       <c r="U89" s="1">
         <v>0</v>
@@ -15658,7 +15708,7 @@
     </row>
     <row r="90" customHeight="1" spans="3:50">
       <c r="C90" s="1">
-        <v>3208</v>
+        <v>3207</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>196</v>
@@ -15676,7 +15726,7 @@
         <v>0</v>
       </c>
       <c r="I90" s="1">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="J90" s="1">
         <v>0</v>
@@ -15709,7 +15759,7 @@
         <v>0</v>
       </c>
       <c r="T90" s="1">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="U90" s="1">
         <v>0</v>
@@ -15806,7 +15856,7 @@
     </row>
     <row r="91" customHeight="1" spans="3:50">
       <c r="C91" s="1">
-        <v>3209</v>
+        <v>3208</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>197</v>
@@ -15824,10 +15874,10 @@
         <v>0</v>
       </c>
       <c r="I91" s="1">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="J91" s="1">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="K91" s="1">
         <v>0</v>
@@ -15954,7 +16004,7 @@
     </row>
     <row r="92" customHeight="1" spans="3:50">
       <c r="C92" s="1">
-        <v>3210</v>
+        <v>3209</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>198</v>
@@ -15975,7 +16025,7 @@
         <v>0</v>
       </c>
       <c r="J92" s="1">
-        <v>1025</v>
+        <v>210</v>
       </c>
       <c r="K92" s="1">
         <v>0</v>
@@ -16102,7 +16152,7 @@
     </row>
     <row r="93" customHeight="1" spans="3:50">
       <c r="C93" s="1">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>199</v>
@@ -16123,7 +16173,7 @@
         <v>0</v>
       </c>
       <c r="J93" s="1">
-        <v>0</v>
+        <v>1025</v>
       </c>
       <c r="K93" s="1">
         <v>0</v>
@@ -16147,7 +16197,7 @@
         <v>0</v>
       </c>
       <c r="R93" s="1">
-        <v>0.045</v>
+        <v>0</v>
       </c>
       <c r="S93" s="1">
         <v>0</v>
@@ -16250,7 +16300,7 @@
     </row>
     <row r="94" customHeight="1" spans="3:50">
       <c r="C94" s="1">
-        <v>3212</v>
+        <v>3211</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>200</v>
@@ -16289,13 +16339,13 @@
         <v>0</v>
       </c>
       <c r="P94" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="1">
+        <v>0</v>
+      </c>
+      <c r="R94" s="1">
         <v>0.045</v>
-      </c>
-      <c r="Q94" s="1">
-        <v>0</v>
-      </c>
-      <c r="R94" s="1">
-        <v>0</v>
       </c>
       <c r="S94" s="1">
         <v>0</v>
@@ -16398,7 +16448,7 @@
     </row>
     <row r="95" customHeight="1" spans="3:50">
       <c r="C95" s="1">
-        <v>3213</v>
+        <v>3212</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>201</v>
@@ -16428,16 +16478,16 @@
         <v>0</v>
       </c>
       <c r="M95" s="12">
+        <v>0</v>
+      </c>
+      <c r="N95" s="1">
+        <v>0</v>
+      </c>
+      <c r="O95" s="1">
+        <v>0</v>
+      </c>
+      <c r="P95" s="1">
         <v>0.045</v>
-      </c>
-      <c r="N95" s="1">
-        <v>0</v>
-      </c>
-      <c r="O95" s="1">
-        <v>0</v>
-      </c>
-      <c r="P95" s="1">
-        <v>0</v>
       </c>
       <c r="Q95" s="1">
         <v>0</v>
@@ -16540,6 +16590,154 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX95" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
+      </c>
+    </row>
+    <row r="96" customHeight="1" spans="3:50">
+      <c r="C96" s="1">
+        <v>3213</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E96" s="1">
+        <v>0</v>
+      </c>
+      <c r="F96" s="1">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1">
+        <v>0</v>
+      </c>
+      <c r="H96" s="1">
+        <v>0</v>
+      </c>
+      <c r="I96" s="1">
+        <v>0</v>
+      </c>
+      <c r="J96" s="1">
+        <v>0</v>
+      </c>
+      <c r="K96" s="1">
+        <v>0</v>
+      </c>
+      <c r="L96" s="1">
+        <v>0</v>
+      </c>
+      <c r="M96" s="12">
+        <v>0.045</v>
+      </c>
+      <c r="N96" s="1">
+        <v>0</v>
+      </c>
+      <c r="O96" s="1">
+        <v>0</v>
+      </c>
+      <c r="P96" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="1">
+        <v>0</v>
+      </c>
+      <c r="R96" s="1">
+        <v>0</v>
+      </c>
+      <c r="S96" s="1">
+        <v>0</v>
+      </c>
+      <c r="T96" s="1">
+        <v>0</v>
+      </c>
+      <c r="U96" s="1">
+        <v>0</v>
+      </c>
+      <c r="V96" s="1">
+        <v>0</v>
+      </c>
+      <c r="W96" s="1">
+        <v>0</v>
+      </c>
+      <c r="X96" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y96" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV96" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW96" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
+      </c>
+      <c r="AX96" s="10" t="str">
         <f t="shared" si="9"/>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:a0a1d8f commit_msg:修改卡牌突破数值 ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -807,11 +807,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -847,10 +847,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -863,6 +871,29 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
@@ -871,7 +902,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -885,29 +923,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -922,7 +938,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -937,24 +953,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -963,13 +963,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -985,6 +978,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1040,7 +1040,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1052,7 +1100,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1070,7 +1154,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1082,133 +1208,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1260,16 +1260,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1284,16 +1284,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1330,20 +1330,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1353,10 +1353,10 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1365,133 +1365,133 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2739,8 +2739,8 @@
   <sheetPr/>
   <dimension ref="A1:AX96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83:K96"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -4472,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
@@ -4620,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="1">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
@@ -4768,7 +4768,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
@@ -4916,7 +4916,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -5064,7 +5064,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -15022,7 +15022,7 @@
         <v>0</v>
       </c>
       <c r="U85" s="1">
-        <v>1800</v>
+        <v>3600</v>
       </c>
       <c r="V85" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:ae469e6 commit_msg:Merge branch 'dev' of https://bitbucket.org/funplus/excel into dev ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="205">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -580,34 +580,40 @@
     <t>武器升级攻击力成长率</t>
   </si>
   <si>
-    <t>单手剑1突破1次物理伤害加成值</t>
-  </si>
-  <si>
-    <t>单手剑1突破2次物理伤害加成值</t>
-  </si>
-  <si>
-    <t>单手剑1突破3次物理伤害加成值</t>
-  </si>
-  <si>
-    <t>单手剑1突破4次物理伤害加成值</t>
-  </si>
-  <si>
-    <t>单手剑1突破5次物理伤害加成值</t>
-  </si>
-  <si>
-    <t>单手剑2突破1次mp值增加固定值</t>
-  </si>
-  <si>
-    <t>单手剑2突破2次mp值增加固定值</t>
-  </si>
-  <si>
-    <t>单手剑2突破3次mp值增加固定值</t>
-  </si>
-  <si>
-    <t>单手剑2突破4次mp值增加固定值</t>
-  </si>
-  <si>
-    <t>单手剑2突破5次mp值增加固定值</t>
+    <t>百分比防御力</t>
+  </si>
+  <si>
+    <t>单手剑1突破1次</t>
+  </si>
+  <si>
+    <t>单手剑1突破2次</t>
+  </si>
+  <si>
+    <t>单手剑1突破3次</t>
+  </si>
+  <si>
+    <t>单手剑1突破4次</t>
+  </si>
+  <si>
+    <t>单手剑1突破5次</t>
+  </si>
+  <si>
+    <t>百分比时速</t>
+  </si>
+  <si>
+    <t>单手剑2突破1次</t>
+  </si>
+  <si>
+    <t>单手剑2突破2次</t>
+  </si>
+  <si>
+    <t>单手剑2突破3次</t>
+  </si>
+  <si>
+    <t>单手剑2突破4次</t>
+  </si>
+  <si>
+    <t>单手剑2突破5次</t>
   </si>
   <si>
     <t>晶石位置1攻击力成长率</t>
@@ -807,11 +813,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -846,17 +852,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -864,14 +868,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -886,6 +905,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
@@ -893,11 +943,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -908,30 +972,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -945,46 +988,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1028,7 +1034,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1040,13 +1130,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,55 +1172,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,97 +1214,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1250,69 +1256,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1342,8 +1285,71 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1353,10 +1359,10 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1365,133 +1371,133 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2739,8 +2745,8 @@
   <sheetPr/>
   <dimension ref="A1:AX96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E32" sqref="$A32:$XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -5790,12 +5796,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="23" customHeight="1" spans="3:50">
+    <row r="23" customHeight="1" spans="2:50">
+      <c r="B23" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="C23" s="1">
         <v>2010</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -5807,7 +5816,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="12">
-        <v>0</v>
+        <v>0.047</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -5870,7 +5879,7 @@
         <v>0</v>
       </c>
       <c r="AC23" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="AD23" s="1">
         <v>0</v>
@@ -5931,19 +5940,22 @@
       </c>
       <c r="AW23" s="10" t="str">
         <f>AC21:AC27&amp;","&amp;AD21:AD27&amp;","&amp;AE21:AE27&amp;","&amp;AF21:AF27&amp;","&amp;AG21:AG27&amp;","&amp;AH21:AH27&amp;","&amp;AI21:AI27&amp;","&amp;AJ21:AJ27&amp;","&amp;AK21:AK27&amp;","&amp;AL21:AL27</f>
-        <v>0.05,0,0,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX23" s="10" t="str">
         <f>AM21:AM27&amp;","&amp;AN21:AN27&amp;","&amp;AO21:AO27&amp;","&amp;AP21:AP27&amp;","&amp;AQ21:AQ27&amp;","&amp;AR21:AR27&amp;","&amp;AS21:AS27&amp;","&amp;AT21:AT27&amp;","&amp;AU21:AU27&amp;","&amp;AV21:AV27</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="24" customHeight="1" spans="3:50">
+    <row r="24" customHeight="1" spans="2:50">
+      <c r="B24" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="C24" s="1">
         <v>2011</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -5955,7 +5967,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="12">
-        <v>0</v>
+        <v>0.072</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -6018,7 +6030,7 @@
         <v>0</v>
       </c>
       <c r="AC24" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AD24" s="1">
         <v>0</v>
@@ -6079,19 +6091,22 @@
       </c>
       <c r="AW24" s="10" t="str">
         <f>AC21:AC28&amp;","&amp;AD21:AD28&amp;","&amp;AE21:AE28&amp;","&amp;AF21:AF28&amp;","&amp;AG21:AG28&amp;","&amp;AH21:AH28&amp;","&amp;AI21:AI28&amp;","&amp;AJ21:AJ28&amp;","&amp;AK21:AK28&amp;","&amp;AL21:AL28</f>
-        <v>0.1,0,0,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX24" s="10" t="str">
         <f>AM21:AM28&amp;","&amp;AN21:AN28&amp;","&amp;AO21:AO28&amp;","&amp;AP21:AP28&amp;","&amp;AQ21:AQ28&amp;","&amp;AR21:AR28&amp;","&amp;AS21:AS28&amp;","&amp;AT21:AT28&amp;","&amp;AU21:AU28&amp;","&amp;AV21:AV28</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="25" customHeight="1" spans="3:50">
+    <row r="25" customHeight="1" spans="2:50">
+      <c r="B25" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="C25" s="1">
         <v>2012</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -6103,7 +6118,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="12">
-        <v>0</v>
+        <v>0.097</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -6166,7 +6181,7 @@
         <v>0</v>
       </c>
       <c r="AC25" s="1">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="AD25" s="1">
         <v>0</v>
@@ -6227,19 +6242,22 @@
       </c>
       <c r="AW25" s="10" t="str">
         <f>AC22:AC29&amp;","&amp;AD22:AD29&amp;","&amp;AE22:AE29&amp;","&amp;AF22:AF29&amp;","&amp;AG22:AG29&amp;","&amp;AH22:AH29&amp;","&amp;AI22:AI29&amp;","&amp;AJ22:AJ29&amp;","&amp;AK22:AK29&amp;","&amp;AL22:AL29</f>
-        <v>0.15,0,0,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX25" s="10" t="str">
         <f>AM22:AM29&amp;","&amp;AN22:AN29&amp;","&amp;AO22:AO29&amp;","&amp;AP22:AP29&amp;","&amp;AQ22:AQ29&amp;","&amp;AR22:AR29&amp;","&amp;AS22:AS29&amp;","&amp;AT22:AT29&amp;","&amp;AU22:AU29&amp;","&amp;AV22:AV29</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="26" customHeight="1" spans="3:50">
+    <row r="26" customHeight="1" spans="2:50">
+      <c r="B26" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="C26" s="1">
         <v>2013</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -6251,7 +6269,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="12">
-        <v>0</v>
+        <v>0.122</v>
       </c>
       <c r="I26" s="1">
         <v>0</v>
@@ -6314,7 +6332,7 @@
         <v>0</v>
       </c>
       <c r="AC26" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="AD26" s="1">
         <v>0</v>
@@ -6375,19 +6393,22 @@
       </c>
       <c r="AW26" s="10" t="str">
         <f>AC22:AC30&amp;","&amp;AD22:AD30&amp;","&amp;AE22:AE30&amp;","&amp;AF22:AF30&amp;","&amp;AG22:AG30&amp;","&amp;AH22:AH30&amp;","&amp;AI22:AI30&amp;","&amp;AJ22:AJ30&amp;","&amp;AK22:AK30&amp;","&amp;AL22:AL30</f>
-        <v>0.2,0,0,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX26" s="10" t="str">
         <f>AM22:AM30&amp;","&amp;AN22:AN30&amp;","&amp;AO22:AO30&amp;","&amp;AP22:AP30&amp;","&amp;AQ22:AQ30&amp;","&amp;AR22:AR30&amp;","&amp;AS22:AS30&amp;","&amp;AT22:AT30&amp;","&amp;AU22:AU30&amp;","&amp;AV22:AV30</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="27" customHeight="1" spans="3:50">
+    <row r="27" customHeight="1" spans="2:50">
+      <c r="B27" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="C27" s="1">
         <v>2014</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -6399,7 +6420,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="12">
-        <v>0</v>
+        <v>0.147</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -6462,7 +6483,7 @@
         <v>0</v>
       </c>
       <c r="AC27" s="1">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="AD27" s="1">
         <v>0</v>
@@ -6523,19 +6544,22 @@
       </c>
       <c r="AW27" s="10" t="str">
         <f>AC22:AC31&amp;","&amp;AD22:AD31&amp;","&amp;AE22:AE31&amp;","&amp;AF22:AF31&amp;","&amp;AG22:AG31&amp;","&amp;AH22:AH31&amp;","&amp;AI22:AI31&amp;","&amp;AJ22:AJ31&amp;","&amp;AK22:AK31&amp;","&amp;AL22:AL31</f>
-        <v>0.25,0,0,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="AX27" s="10" t="str">
         <f>AM22:AM31&amp;","&amp;AN22:AN31&amp;","&amp;AO22:AO31&amp;","&amp;AP22:AP31&amp;","&amp;AQ22:AQ31&amp;","&amp;AR22:AR31&amp;","&amp;AS22:AS31&amp;","&amp;AT22:AT31&amp;","&amp;AU22:AU31&amp;","&amp;AV22:AV31</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="28" customHeight="1" spans="3:50">
+    <row r="28" customHeight="1" spans="2:50">
+      <c r="B28" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="C28" s="1">
         <v>2020</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -6577,7 +6601,7 @@
         <v>0</v>
       </c>
       <c r="R28" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="S28" s="1">
         <v>0</v>
@@ -6592,7 +6616,7 @@
         <v>0</v>
       </c>
       <c r="W28" s="1">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="X28" s="1">
         <v>0</v>
@@ -6678,12 +6702,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="29" customHeight="1" spans="3:50">
+    <row r="29" customHeight="1" spans="2:50">
+      <c r="B29" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="C29" s="1">
         <v>2021</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -6725,7 +6752,7 @@
         <v>0</v>
       </c>
       <c r="R29" s="12">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="S29" s="1">
         <v>0</v>
@@ -6740,7 +6767,7 @@
         <v>0</v>
       </c>
       <c r="W29" s="1">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="X29" s="1">
         <v>0</v>
@@ -6826,12 +6853,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="30" customHeight="1" spans="3:50">
+    <row r="30" customHeight="1" spans="2:50">
+      <c r="B30" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="C30" s="1">
         <v>2022</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -6873,7 +6903,7 @@
         <v>0</v>
       </c>
       <c r="R30" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="S30" s="1">
         <v>0</v>
@@ -6888,7 +6918,7 @@
         <v>0</v>
       </c>
       <c r="W30" s="1">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="X30" s="1">
         <v>0</v>
@@ -6974,12 +7004,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="31" customHeight="1" spans="3:50">
+    <row r="31" customHeight="1" spans="2:50">
+      <c r="B31" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="C31" s="1">
         <v>2023</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -7021,7 +7054,7 @@
         <v>0</v>
       </c>
       <c r="R31" s="12">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="S31" s="1">
         <v>0</v>
@@ -7036,7 +7069,7 @@
         <v>0</v>
       </c>
       <c r="W31" s="1">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="X31" s="1">
         <v>0</v>
@@ -7122,12 +7155,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="32" customHeight="1" spans="3:50">
+    <row r="32" customHeight="1" spans="2:50">
+      <c r="B32" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="C32" s="1">
         <v>2024</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -7169,7 +7205,7 @@
         <v>0</v>
       </c>
       <c r="R32" s="12">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="S32" s="1">
         <v>0</v>
@@ -7184,7 +7220,7 @@
         <v>0</v>
       </c>
       <c r="W32" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="X32" s="1">
         <v>0</v>
@@ -7275,7 +7311,7 @@
         <v>3000</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E33" s="1">
         <v>6</v>
@@ -7423,7 +7459,7 @@
         <v>3001</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E34" s="1">
         <v>60</v>
@@ -7571,7 +7607,7 @@
         <v>3010</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E35" s="1">
         <v>120</v>
@@ -7719,7 +7755,7 @@
         <v>3011</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E36" s="1">
         <v>1200</v>
@@ -7867,7 +7903,7 @@
         <v>3020</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E37" s="1">
         <v>6</v>
@@ -8015,7 +8051,7 @@
         <v>3021</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E38" s="1">
         <v>60</v>
@@ -8163,7 +8199,7 @@
         <v>3030</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -8311,7 +8347,7 @@
         <v>3031</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -8459,7 +8495,7 @@
         <v>3032</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -8607,7 +8643,7 @@
         <v>3033</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
@@ -8755,7 +8791,7 @@
         <v>3034</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
@@ -8903,7 +8939,7 @@
         <v>3035</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -9051,7 +9087,7 @@
         <v>3036</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -9199,7 +9235,7 @@
         <v>3037</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -9347,7 +9383,7 @@
         <v>3050</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -9495,7 +9531,7 @@
         <v>3051</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -9643,7 +9679,7 @@
         <v>3052</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
@@ -9791,7 +9827,7 @@
         <v>3053</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
@@ -9939,7 +9975,7 @@
         <v>3054</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -10087,7 +10123,7 @@
         <v>3055</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -10235,7 +10271,7 @@
         <v>3056</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -10383,7 +10419,7 @@
         <v>3057</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -10531,7 +10567,7 @@
         <v>3058</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -10679,7 +10715,7 @@
         <v>3059</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -10827,7 +10863,7 @@
         <v>3060</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -10975,7 +11011,7 @@
         <v>3061</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
@@ -11123,7 +11159,7 @@
         <v>3062</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E59" s="1">
         <v>0</v>
@@ -11271,7 +11307,7 @@
         <v>3063</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
@@ -11419,7 +11455,7 @@
         <v>3064</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>
@@ -11567,7 +11603,7 @@
         <v>3065</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E62" s="1">
         <v>0</v>
@@ -11715,7 +11751,7 @@
         <v>3066</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E63" s="1">
         <v>0</v>
@@ -11863,7 +11899,7 @@
         <v>3067</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E64" s="1">
         <v>0</v>
@@ -12011,7 +12047,7 @@
         <v>3068</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E65" s="2">
         <v>0</v>
@@ -12159,7 +12195,7 @@
         <v>3069</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E66" s="2">
         <v>0</v>
@@ -12307,7 +12343,7 @@
         <v>3070</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E67" s="2">
         <v>0</v>
@@ -12455,7 +12491,7 @@
         <v>3071</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E68" s="2">
         <v>0</v>
@@ -12603,7 +12639,7 @@
         <v>3072</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E69" s="2">
         <v>0</v>
@@ -12751,7 +12787,7 @@
         <v>3073</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E70" s="2">
         <v>0</v>
@@ -12899,7 +12935,7 @@
         <v>3074</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E71" s="2">
         <v>0</v>
@@ -13047,7 +13083,7 @@
         <v>3075</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E72" s="2">
         <v>0</v>
@@ -13195,7 +13231,7 @@
         <v>3076</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E73" s="2">
         <v>0</v>
@@ -13343,7 +13379,7 @@
         <v>3077</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E74" s="2">
         <v>0</v>
@@ -13491,7 +13527,7 @@
         <v>3078</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E75" s="2">
         <v>0</v>
@@ -13639,7 +13675,7 @@
         <v>3079</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E76" s="2">
         <v>0</v>
@@ -13787,7 +13823,7 @@
         <v>3080</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E77" s="2">
         <v>0</v>
@@ -13935,7 +13971,7 @@
         <v>3081</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E78" s="2">
         <v>0</v>
@@ -14083,7 +14119,7 @@
         <v>3082</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E79" s="2">
         <v>0</v>
@@ -14231,7 +14267,7 @@
         <v>3083</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E80" s="2">
         <v>0</v>
@@ -14379,7 +14415,7 @@
         <v>3084</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E81" s="2">
         <v>0</v>
@@ -14527,7 +14563,7 @@
         <v>3085</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E82" s="2">
         <v>0</v>
@@ -14675,7 +14711,7 @@
         <v>3200</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E83" s="1">
         <v>180</v>
@@ -14823,7 +14859,7 @@
         <v>3201</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E84" s="1">
         <v>0</v>
@@ -14971,7 +15007,7 @@
         <v>3202</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E85" s="1">
         <v>0</v>
@@ -15119,7 +15155,7 @@
         <v>3203</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E86" s="1">
         <v>0</v>
@@ -15267,7 +15303,7 @@
         <v>3204</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E87" s="1">
         <v>0</v>
@@ -15415,7 +15451,7 @@
         <v>3205</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E88" s="1">
         <v>0</v>
@@ -15563,7 +15599,7 @@
         <v>3206</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E89" s="1">
         <v>0</v>
@@ -15711,7 +15747,7 @@
         <v>3207</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E90" s="1">
         <v>0</v>
@@ -15859,7 +15895,7 @@
         <v>3208</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E91" s="1">
         <v>0</v>
@@ -16007,7 +16043,7 @@
         <v>3209</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E92" s="1">
         <v>0</v>
@@ -16155,7 +16191,7 @@
         <v>3210</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E93" s="1">
         <v>0</v>
@@ -16303,7 +16339,7 @@
         <v>3211</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E94" s="1">
         <v>0</v>
@@ -16451,7 +16487,7 @@
         <v>3212</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E95" s="1">
         <v>0</v>
@@ -16599,7 +16635,7 @@
         <v>3213</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E96" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:7ecffbe commit_msg:修改了韧性的位置 ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12540"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="AttProto" sheetId="1" r:id="rId1"/>
@@ -272,12 +272,12 @@
     <t>crit</t>
   </si>
   <si>
+    <t>critInc</t>
+  </si>
+  <si>
     <t>tenacity</t>
   </si>
   <si>
-    <t>critInc</t>
-  </si>
-  <si>
     <t>heal</t>
   </si>
   <si>
@@ -419,10 +419,10 @@
     <t>暴击值</t>
   </si>
   <si>
+    <t>暴击倍数加成</t>
+  </si>
+  <si>
     <t>韧性值</t>
-  </si>
-  <si>
-    <t>暴击倍数加成</t>
   </si>
   <si>
     <t>治疗强度</t>
@@ -841,9 +841,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
@@ -882,14 +882,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -898,17 +890,32 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -921,7 +928,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -936,52 +973,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1003,14 +995,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -1074,7 +1074,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1086,7 +1098,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1098,7 +1110,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1116,7 +1146,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1128,37 +1158,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1170,7 +1182,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1182,25 +1206,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1212,19 +1218,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1237,12 +1243,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1284,6 +1284,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1308,15 +1317,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1328,32 +1328,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1376,8 +1350,34 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1387,10 +1387,10 @@
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1399,133 +1399,133 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2774,7 +2774,7 @@
   <dimension ref="A1:AY96"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7:K96"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -2786,8 +2786,9 @@
     <col min="5" max="6" width="12.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.6166666666667" style="1" customWidth="1"/>
-    <col min="9" max="11" width="13.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.75" style="1" customWidth="1"/>
+    <col min="9" max="10" width="13.875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.75" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.875" style="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="7.5" style="1" customWidth="1"/>
@@ -3489,10 +3490,10 @@
         <v>1000</v>
       </c>
       <c r="K7" s="12">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="L7" s="12">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="M7" s="12">
         <v>0</v>
@@ -3642,10 +3643,10 @@
         <v>3000</v>
       </c>
       <c r="K8" s="12">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="L8" s="12">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="M8" s="12">
         <v>0</v>
@@ -3795,10 +3796,10 @@
         <v>1000</v>
       </c>
       <c r="K9" s="12">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="L9" s="12">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="M9" s="12">
         <v>500</v>
@@ -3948,10 +3949,10 @@
         <v>1000</v>
       </c>
       <c r="K10" s="12">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="L10" s="12">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="M10" s="12">
         <v>0</v>
@@ -4101,10 +4102,10 @@
         <v>1500</v>
       </c>
       <c r="K11" s="12">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="L11" s="12">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="M11" s="12">
         <v>0</v>
@@ -4252,10 +4253,10 @@
         <v>1500</v>
       </c>
       <c r="K12" s="12">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="L12" s="12">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="M12" s="12">
         <v>0</v>
@@ -4403,10 +4404,10 @@
         <v>1500</v>
       </c>
       <c r="K13" s="12">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="L13" s="12">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="M13" s="12">
         <v>0</v>
@@ -4553,10 +4554,10 @@
       <c r="J14" s="1">
         <v>150</v>
       </c>
-      <c r="K14" s="12">
-        <v>0</v>
-      </c>
-      <c r="L14" s="1">
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
         <v>0</v>
       </c>
       <c r="M14" s="1">
@@ -4704,10 +4705,10 @@
       <c r="J15" s="1">
         <v>250</v>
       </c>
-      <c r="K15" s="12">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1">
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
         <v>0</v>
       </c>
       <c r="M15" s="1">
@@ -4855,10 +4856,10 @@
       <c r="J16" s="1">
         <v>350</v>
       </c>
-      <c r="K16" s="12">
-        <v>0</v>
-      </c>
-      <c r="L16" s="1">
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="12">
         <v>0</v>
       </c>
       <c r="M16" s="1">
@@ -5006,10 +5007,10 @@
       <c r="J17" s="1">
         <v>450</v>
       </c>
-      <c r="K17" s="12">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
         <v>0</v>
       </c>
       <c r="M17" s="1">
@@ -5157,10 +5158,10 @@
       <c r="J18" s="1">
         <v>550</v>
       </c>
-      <c r="K18" s="12">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1">
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
         <v>0</v>
       </c>
       <c r="M18" s="1">
@@ -5308,10 +5309,10 @@
       <c r="J19" s="1">
         <v>0</v>
       </c>
-      <c r="K19" s="12">
-        <v>0</v>
-      </c>
-      <c r="L19" s="1">
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
         <v>0</v>
       </c>
       <c r="M19" s="1">
@@ -5460,10 +5461,10 @@
         <v>500</v>
       </c>
       <c r="K20" s="12">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="L20" s="12">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="M20" s="12">
         <v>0</v>
@@ -5610,10 +5611,10 @@
       <c r="J21" s="1">
         <v>0</v>
       </c>
-      <c r="K21" s="12">
-        <v>0</v>
-      </c>
-      <c r="L21" s="1">
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="12">
         <v>0</v>
       </c>
       <c r="M21" s="1">
@@ -5761,10 +5762,10 @@
       <c r="J22" s="1">
         <v>0</v>
       </c>
-      <c r="K22" s="12">
-        <v>0</v>
-      </c>
-      <c r="L22" s="1">
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
         <v>0</v>
       </c>
       <c r="M22" s="1">
@@ -5915,10 +5916,10 @@
       <c r="J23" s="1">
         <v>0</v>
       </c>
-      <c r="K23" s="12">
-        <v>0</v>
-      </c>
-      <c r="L23" s="1">
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="12">
         <v>0</v>
       </c>
       <c r="M23" s="1">
@@ -6069,10 +6070,10 @@
       <c r="J24" s="1">
         <v>0</v>
       </c>
-      <c r="K24" s="12">
-        <v>0</v>
-      </c>
-      <c r="L24" s="1">
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
         <v>0</v>
       </c>
       <c r="M24" s="1">
@@ -6223,10 +6224,10 @@
       <c r="J25" s="1">
         <v>0</v>
       </c>
-      <c r="K25" s="12">
-        <v>0</v>
-      </c>
-      <c r="L25" s="1">
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="12">
         <v>0</v>
       </c>
       <c r="M25" s="1">
@@ -6377,10 +6378,10 @@
       <c r="J26" s="1">
         <v>0</v>
       </c>
-      <c r="K26" s="12">
-        <v>0</v>
-      </c>
-      <c r="L26" s="1">
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="12">
         <v>0</v>
       </c>
       <c r="M26" s="1">
@@ -6531,10 +6532,10 @@
       <c r="J27" s="1">
         <v>0</v>
       </c>
-      <c r="K27" s="12">
-        <v>0</v>
-      </c>
-      <c r="L27" s="1">
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="12">
         <v>0</v>
       </c>
       <c r="M27" s="1">
@@ -6685,10 +6686,10 @@
       <c r="J28" s="1">
         <v>0</v>
       </c>
-      <c r="K28" s="12">
-        <v>0</v>
-      </c>
-      <c r="L28" s="1">
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="12">
         <v>0</v>
       </c>
       <c r="M28" s="1">
@@ -6839,10 +6840,10 @@
       <c r="J29" s="1">
         <v>0</v>
       </c>
-      <c r="K29" s="12">
-        <v>0</v>
-      </c>
-      <c r="L29" s="1">
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="12">
         <v>0</v>
       </c>
       <c r="M29" s="1">
@@ -6993,10 +6994,10 @@
       <c r="J30" s="1">
         <v>0</v>
       </c>
-      <c r="K30" s="12">
-        <v>0</v>
-      </c>
-      <c r="L30" s="1">
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="12">
         <v>0</v>
       </c>
       <c r="M30" s="1">
@@ -7147,10 +7148,10 @@
       <c r="J31" s="1">
         <v>0</v>
       </c>
-      <c r="K31" s="12">
-        <v>0</v>
-      </c>
-      <c r="L31" s="1">
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="12">
         <v>0</v>
       </c>
       <c r="M31" s="1">
@@ -7301,10 +7302,10 @@
       <c r="J32" s="1">
         <v>0</v>
       </c>
-      <c r="K32" s="12">
-        <v>0</v>
-      </c>
-      <c r="L32" s="1">
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="12">
         <v>0</v>
       </c>
       <c r="M32" s="1">
@@ -7452,10 +7453,10 @@
       <c r="J33" s="1">
         <v>0</v>
       </c>
-      <c r="K33" s="12">
-        <v>0</v>
-      </c>
-      <c r="L33" s="1">
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="12">
         <v>0</v>
       </c>
       <c r="M33" s="1">
@@ -7603,10 +7604,10 @@
       <c r="J34" s="1">
         <v>0</v>
       </c>
-      <c r="K34" s="12">
-        <v>0</v>
-      </c>
-      <c r="L34" s="1">
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="12">
         <v>0</v>
       </c>
       <c r="M34" s="1">
@@ -7754,10 +7755,10 @@
       <c r="J35" s="1">
         <v>0</v>
       </c>
-      <c r="K35" s="12">
-        <v>0</v>
-      </c>
-      <c r="L35" s="1">
+      <c r="K35" s="1">
+        <v>0</v>
+      </c>
+      <c r="L35" s="12">
         <v>0</v>
       </c>
       <c r="M35" s="1">
@@ -7905,10 +7906,10 @@
       <c r="J36" s="1">
         <v>0</v>
       </c>
-      <c r="K36" s="12">
-        <v>0</v>
-      </c>
-      <c r="L36" s="1">
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="12">
         <v>0</v>
       </c>
       <c r="M36" s="1">
@@ -8056,10 +8057,10 @@
       <c r="J37" s="1">
         <v>0</v>
       </c>
-      <c r="K37" s="12">
-        <v>0</v>
-      </c>
-      <c r="L37" s="1">
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+      <c r="L37" s="12">
         <v>0</v>
       </c>
       <c r="M37" s="1">
@@ -8207,10 +8208,10 @@
       <c r="J38" s="1">
         <v>0</v>
       </c>
-      <c r="K38" s="12">
-        <v>0</v>
-      </c>
-      <c r="L38" s="1">
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="12">
         <v>0</v>
       </c>
       <c r="M38" s="1">
@@ -8358,10 +8359,10 @@
       <c r="J39" s="1">
         <v>0</v>
       </c>
-      <c r="K39" s="12">
-        <v>0</v>
-      </c>
-      <c r="L39" s="1">
+      <c r="K39" s="1">
+        <v>0</v>
+      </c>
+      <c r="L39" s="12">
         <v>0</v>
       </c>
       <c r="M39" s="1">
@@ -8509,10 +8510,10 @@
       <c r="J40" s="1">
         <v>0</v>
       </c>
-      <c r="K40" s="12">
-        <v>0</v>
-      </c>
-      <c r="L40" s="1">
+      <c r="K40" s="1">
+        <v>0</v>
+      </c>
+      <c r="L40" s="12">
         <v>0</v>
       </c>
       <c r="M40" s="1">
@@ -8660,10 +8661,10 @@
       <c r="J41" s="1">
         <v>0</v>
       </c>
-      <c r="K41" s="12">
-        <v>0</v>
-      </c>
-      <c r="L41" s="1">
+      <c r="K41" s="1">
+        <v>0</v>
+      </c>
+      <c r="L41" s="12">
         <v>0</v>
       </c>
       <c r="M41" s="1">
@@ -8811,10 +8812,10 @@
       <c r="J42" s="1">
         <v>0</v>
       </c>
-      <c r="K42" s="12">
-        <v>0</v>
-      </c>
-      <c r="L42" s="1">
+      <c r="K42" s="1">
+        <v>0</v>
+      </c>
+      <c r="L42" s="12">
         <v>0</v>
       </c>
       <c r="M42" s="1">
@@ -8962,10 +8963,10 @@
       <c r="J43" s="1">
         <v>0</v>
       </c>
-      <c r="K43" s="12">
-        <v>0</v>
-      </c>
-      <c r="L43" s="1">
+      <c r="K43" s="1">
+        <v>0</v>
+      </c>
+      <c r="L43" s="12">
         <v>0</v>
       </c>
       <c r="M43" s="1">
@@ -9113,10 +9114,10 @@
       <c r="J44" s="1">
         <v>0</v>
       </c>
-      <c r="K44" s="12">
-        <v>0</v>
-      </c>
-      <c r="L44" s="1">
+      <c r="K44" s="1">
+        <v>0</v>
+      </c>
+      <c r="L44" s="12">
         <v>0</v>
       </c>
       <c r="M44" s="1">
@@ -9264,10 +9265,10 @@
       <c r="J45" s="1">
         <v>6</v>
       </c>
-      <c r="K45" s="12">
-        <v>0</v>
-      </c>
-      <c r="L45" s="1">
+      <c r="K45" s="1">
+        <v>0</v>
+      </c>
+      <c r="L45" s="12">
         <v>0</v>
       </c>
       <c r="M45" s="1">
@@ -9415,10 +9416,10 @@
       <c r="J46" s="1">
         <v>90</v>
       </c>
-      <c r="K46" s="12">
-        <v>0</v>
-      </c>
-      <c r="L46" s="1">
+      <c r="K46" s="1">
+        <v>0</v>
+      </c>
+      <c r="L46" s="12">
         <v>0</v>
       </c>
       <c r="M46" s="1">
@@ -9566,10 +9567,10 @@
       <c r="J47" s="1">
         <v>0</v>
       </c>
-      <c r="K47" s="12">
-        <v>0</v>
-      </c>
-      <c r="L47" s="1">
+      <c r="K47" s="1">
+        <v>0</v>
+      </c>
+      <c r="L47" s="12">
         <v>0</v>
       </c>
       <c r="M47" s="1">
@@ -9717,10 +9718,10 @@
       <c r="J48" s="1">
         <v>0</v>
       </c>
-      <c r="K48" s="12">
-        <v>0</v>
-      </c>
-      <c r="L48" s="1">
+      <c r="K48" s="1">
+        <v>0</v>
+      </c>
+      <c r="L48" s="12">
         <v>0</v>
       </c>
       <c r="M48" s="1">
@@ -9868,10 +9869,10 @@
       <c r="J49" s="1">
         <v>0</v>
       </c>
-      <c r="K49" s="12">
-        <v>0</v>
-      </c>
-      <c r="L49" s="1">
+      <c r="K49" s="1">
+        <v>0</v>
+      </c>
+      <c r="L49" s="12">
         <v>0</v>
       </c>
       <c r="M49" s="1">
@@ -10019,10 +10020,10 @@
       <c r="J50" s="1">
         <v>0</v>
       </c>
-      <c r="K50" s="12">
-        <v>0</v>
-      </c>
-      <c r="L50" s="1">
+      <c r="K50" s="1">
+        <v>0</v>
+      </c>
+      <c r="L50" s="12">
         <v>0</v>
       </c>
       <c r="M50" s="1">
@@ -10170,10 +10171,10 @@
       <c r="J51" s="1">
         <v>0</v>
       </c>
-      <c r="K51" s="12">
-        <v>0</v>
-      </c>
-      <c r="L51" s="1">
+      <c r="K51" s="1">
+        <v>0</v>
+      </c>
+      <c r="L51" s="12">
         <v>0</v>
       </c>
       <c r="M51" s="1">
@@ -10321,10 +10322,10 @@
       <c r="J52" s="1">
         <v>0</v>
       </c>
-      <c r="K52" s="12">
-        <v>0</v>
-      </c>
-      <c r="L52" s="1">
+      <c r="K52" s="1">
+        <v>0</v>
+      </c>
+      <c r="L52" s="12">
         <v>0</v>
       </c>
       <c r="M52" s="1">
@@ -10472,10 +10473,10 @@
       <c r="J53" s="1">
         <v>0</v>
       </c>
-      <c r="K53" s="12">
-        <v>0</v>
-      </c>
-      <c r="L53" s="1">
+      <c r="K53" s="1">
+        <v>0</v>
+      </c>
+      <c r="L53" s="12">
         <v>0</v>
       </c>
       <c r="M53" s="1">
@@ -10623,10 +10624,10 @@
       <c r="J54" s="1">
         <v>0</v>
       </c>
-      <c r="K54" s="12">
-        <v>0</v>
-      </c>
-      <c r="L54" s="1">
+      <c r="K54" s="1">
+        <v>0</v>
+      </c>
+      <c r="L54" s="12">
         <v>0</v>
       </c>
       <c r="M54" s="1">
@@ -10774,10 +10775,10 @@
       <c r="J55" s="1">
         <v>0</v>
       </c>
-      <c r="K55" s="12">
-        <v>0</v>
-      </c>
-      <c r="L55" s="1">
+      <c r="K55" s="1">
+        <v>0</v>
+      </c>
+      <c r="L55" s="12">
         <v>0</v>
       </c>
       <c r="M55" s="1">
@@ -10925,10 +10926,10 @@
       <c r="J56" s="1">
         <v>0</v>
       </c>
-      <c r="K56" s="12">
-        <v>0</v>
-      </c>
-      <c r="L56" s="1">
+      <c r="K56" s="1">
+        <v>0</v>
+      </c>
+      <c r="L56" s="12">
         <v>0</v>
       </c>
       <c r="M56" s="1">
@@ -11076,10 +11077,10 @@
       <c r="J57" s="1">
         <v>0</v>
       </c>
-      <c r="K57" s="12">
-        <v>0</v>
-      </c>
-      <c r="L57" s="1">
+      <c r="K57" s="1">
+        <v>0</v>
+      </c>
+      <c r="L57" s="12">
         <v>0</v>
       </c>
       <c r="M57" s="1">
@@ -11227,10 +11228,10 @@
       <c r="J58" s="1">
         <v>0</v>
       </c>
-      <c r="K58" s="12">
-        <v>0</v>
-      </c>
-      <c r="L58" s="1">
+      <c r="K58" s="1">
+        <v>0</v>
+      </c>
+      <c r="L58" s="12">
         <v>0</v>
       </c>
       <c r="M58" s="1">
@@ -11378,10 +11379,10 @@
       <c r="J59" s="1">
         <v>0</v>
       </c>
-      <c r="K59" s="12">
-        <v>0</v>
-      </c>
-      <c r="L59" s="1">
+      <c r="K59" s="1">
+        <v>0</v>
+      </c>
+      <c r="L59" s="12">
         <v>0</v>
       </c>
       <c r="M59" s="1">
@@ -11529,10 +11530,10 @@
       <c r="J60" s="1">
         <v>0</v>
       </c>
-      <c r="K60" s="12">
-        <v>0</v>
-      </c>
-      <c r="L60" s="1">
+      <c r="K60" s="1">
+        <v>0</v>
+      </c>
+      <c r="L60" s="12">
         <v>0</v>
       </c>
       <c r="M60" s="1">
@@ -11680,10 +11681,10 @@
       <c r="J61" s="1">
         <v>0</v>
       </c>
-      <c r="K61" s="12">
-        <v>0</v>
-      </c>
-      <c r="L61" s="1">
+      <c r="K61" s="1">
+        <v>0</v>
+      </c>
+      <c r="L61" s="12">
         <v>0</v>
       </c>
       <c r="M61" s="1">
@@ -11831,10 +11832,10 @@
       <c r="J62" s="1">
         <v>0</v>
       </c>
-      <c r="K62" s="12">
-        <v>0</v>
-      </c>
-      <c r="L62" s="1">
+      <c r="K62" s="1">
+        <v>0</v>
+      </c>
+      <c r="L62" s="12">
         <v>0</v>
       </c>
       <c r="M62" s="1">
@@ -11982,10 +11983,10 @@
       <c r="J63" s="1">
         <v>0</v>
       </c>
-      <c r="K63" s="12">
-        <v>0</v>
-      </c>
-      <c r="L63" s="1">
+      <c r="K63" s="1">
+        <v>0</v>
+      </c>
+      <c r="L63" s="12">
         <v>0</v>
       </c>
       <c r="M63" s="1">
@@ -12133,10 +12134,10 @@
       <c r="J64" s="1">
         <v>0</v>
       </c>
-      <c r="K64" s="12">
-        <v>0</v>
-      </c>
-      <c r="L64" s="1">
+      <c r="K64" s="1">
+        <v>0</v>
+      </c>
+      <c r="L64" s="12">
         <v>0</v>
       </c>
       <c r="M64" s="1">
@@ -12284,10 +12285,10 @@
       <c r="J65" s="2">
         <v>0</v>
       </c>
-      <c r="K65" s="12">
-        <v>0</v>
-      </c>
-      <c r="L65" s="2">
+      <c r="K65" s="2">
+        <v>0</v>
+      </c>
+      <c r="L65" s="12">
         <v>0</v>
       </c>
       <c r="M65" s="2">
@@ -12435,10 +12436,10 @@
       <c r="J66" s="2">
         <v>0</v>
       </c>
-      <c r="K66" s="12">
-        <v>0</v>
-      </c>
-      <c r="L66" s="2">
+      <c r="K66" s="2">
+        <v>0</v>
+      </c>
+      <c r="L66" s="12">
         <v>0</v>
       </c>
       <c r="M66" s="2">
@@ -12586,10 +12587,10 @@
       <c r="J67" s="2">
         <v>0</v>
       </c>
-      <c r="K67" s="12">
-        <v>0</v>
-      </c>
-      <c r="L67" s="2">
+      <c r="K67" s="2">
+        <v>0</v>
+      </c>
+      <c r="L67" s="12">
         <v>0</v>
       </c>
       <c r="M67" s="2">
@@ -12737,10 +12738,10 @@
       <c r="J68" s="2">
         <v>0</v>
       </c>
-      <c r="K68" s="12">
-        <v>0</v>
-      </c>
-      <c r="L68" s="2">
+      <c r="K68" s="2">
+        <v>0</v>
+      </c>
+      <c r="L68" s="12">
         <v>0</v>
       </c>
       <c r="M68" s="2">
@@ -12888,10 +12889,10 @@
       <c r="J69" s="2">
         <v>0</v>
       </c>
-      <c r="K69" s="12">
-        <v>0</v>
-      </c>
-      <c r="L69" s="2">
+      <c r="K69" s="2">
+        <v>0</v>
+      </c>
+      <c r="L69" s="12">
         <v>0</v>
       </c>
       <c r="M69" s="2">
@@ -13039,10 +13040,10 @@
       <c r="J70" s="2">
         <v>0</v>
       </c>
-      <c r="K70" s="12">
-        <v>0</v>
-      </c>
-      <c r="L70" s="2">
+      <c r="K70" s="2">
+        <v>0</v>
+      </c>
+      <c r="L70" s="12">
         <v>0</v>
       </c>
       <c r="M70" s="2">
@@ -13190,10 +13191,10 @@
       <c r="J71" s="2">
         <v>0</v>
       </c>
-      <c r="K71" s="12">
-        <v>0</v>
-      </c>
-      <c r="L71" s="2">
+      <c r="K71" s="2">
+        <v>0</v>
+      </c>
+      <c r="L71" s="12">
         <v>0</v>
       </c>
       <c r="M71" s="2">
@@ -13341,10 +13342,10 @@
       <c r="J72" s="2">
         <v>0</v>
       </c>
-      <c r="K72" s="12">
-        <v>0</v>
-      </c>
-      <c r="L72" s="2">
+      <c r="K72" s="2">
+        <v>0</v>
+      </c>
+      <c r="L72" s="12">
         <v>0</v>
       </c>
       <c r="M72" s="2">
@@ -13492,10 +13493,10 @@
       <c r="J73" s="2">
         <v>0</v>
       </c>
-      <c r="K73" s="12">
-        <v>0</v>
-      </c>
-      <c r="L73" s="2">
+      <c r="K73" s="2">
+        <v>0</v>
+      </c>
+      <c r="L73" s="12">
         <v>0</v>
       </c>
       <c r="M73" s="2">
@@ -13643,10 +13644,10 @@
       <c r="J74" s="2">
         <v>0</v>
       </c>
-      <c r="K74" s="12">
-        <v>0</v>
-      </c>
-      <c r="L74" s="2">
+      <c r="K74" s="2">
+        <v>0</v>
+      </c>
+      <c r="L74" s="12">
         <v>0</v>
       </c>
       <c r="M74" s="2">
@@ -13794,10 +13795,10 @@
       <c r="J75" s="2">
         <v>0</v>
       </c>
-      <c r="K75" s="12">
-        <v>0</v>
-      </c>
-      <c r="L75" s="2">
+      <c r="K75" s="2">
+        <v>0</v>
+      </c>
+      <c r="L75" s="12">
         <v>0</v>
       </c>
       <c r="M75" s="2">
@@ -13945,10 +13946,10 @@
       <c r="J76" s="2">
         <v>0</v>
       </c>
-      <c r="K76" s="12">
-        <v>0</v>
-      </c>
-      <c r="L76" s="2">
+      <c r="K76" s="2">
+        <v>0</v>
+      </c>
+      <c r="L76" s="12">
         <v>0</v>
       </c>
       <c r="M76" s="2">
@@ -14096,10 +14097,10 @@
       <c r="J77" s="2">
         <v>0</v>
       </c>
-      <c r="K77" s="12">
-        <v>0</v>
-      </c>
-      <c r="L77" s="2">
+      <c r="K77" s="2">
+        <v>0</v>
+      </c>
+      <c r="L77" s="12">
         <v>0</v>
       </c>
       <c r="M77" s="2">
@@ -14247,10 +14248,10 @@
       <c r="J78" s="2">
         <v>0</v>
       </c>
-      <c r="K78" s="12">
-        <v>0</v>
-      </c>
-      <c r="L78" s="2">
+      <c r="K78" s="2">
+        <v>0</v>
+      </c>
+      <c r="L78" s="12">
         <v>0</v>
       </c>
       <c r="M78" s="2">
@@ -14398,10 +14399,10 @@
       <c r="J79" s="2">
         <v>0</v>
       </c>
-      <c r="K79" s="12">
-        <v>0</v>
-      </c>
-      <c r="L79" s="2">
+      <c r="K79" s="2">
+        <v>0</v>
+      </c>
+      <c r="L79" s="12">
         <v>0</v>
       </c>
       <c r="M79" s="2">
@@ -14549,10 +14550,10 @@
       <c r="J80" s="2">
         <v>0</v>
       </c>
-      <c r="K80" s="12">
-        <v>0</v>
-      </c>
-      <c r="L80" s="2">
+      <c r="K80" s="2">
+        <v>0</v>
+      </c>
+      <c r="L80" s="12">
         <v>0</v>
       </c>
       <c r="M80" s="2">
@@ -14700,10 +14701,10 @@
       <c r="J81" s="2">
         <v>0</v>
       </c>
-      <c r="K81" s="12">
-        <v>0</v>
-      </c>
-      <c r="L81" s="2">
+      <c r="K81" s="2">
+        <v>0</v>
+      </c>
+      <c r="L81" s="12">
         <v>0</v>
       </c>
       <c r="M81" s="2">
@@ -14851,10 +14852,10 @@
       <c r="J82" s="2">
         <v>0</v>
       </c>
-      <c r="K82" s="12">
-        <v>0</v>
-      </c>
-      <c r="L82" s="2">
+      <c r="K82" s="2">
+        <v>0</v>
+      </c>
+      <c r="L82" s="12">
         <v>0</v>
       </c>
       <c r="M82" s="2">
@@ -15002,10 +15003,10 @@
       <c r="J83" s="1">
         <v>0</v>
       </c>
-      <c r="K83" s="12">
-        <v>0</v>
-      </c>
-      <c r="L83" s="1">
+      <c r="K83" s="1">
+        <v>0</v>
+      </c>
+      <c r="L83" s="12">
         <v>0</v>
       </c>
       <c r="M83" s="1">
@@ -15153,10 +15154,10 @@
       <c r="J84" s="1">
         <v>0</v>
       </c>
-      <c r="K84" s="12">
-        <v>0</v>
-      </c>
-      <c r="L84" s="1">
+      <c r="K84" s="1">
+        <v>0</v>
+      </c>
+      <c r="L84" s="12">
         <v>0</v>
       </c>
       <c r="M84" s="1">
@@ -15304,10 +15305,10 @@
       <c r="J85" s="1">
         <v>0</v>
       </c>
-      <c r="K85" s="12">
-        <v>0</v>
-      </c>
-      <c r="L85" s="1">
+      <c r="K85" s="1">
+        <v>0</v>
+      </c>
+      <c r="L85" s="12">
         <v>0</v>
       </c>
       <c r="M85" s="1">
@@ -15455,10 +15456,10 @@
       <c r="J86" s="1">
         <v>0</v>
       </c>
-      <c r="K86" s="12">
-        <v>0</v>
-      </c>
-      <c r="L86" s="1">
+      <c r="K86" s="1">
+        <v>0</v>
+      </c>
+      <c r="L86" s="12">
         <v>0</v>
       </c>
       <c r="M86" s="1">
@@ -15606,10 +15607,10 @@
       <c r="J87" s="1">
         <v>0</v>
       </c>
-      <c r="K87" s="12">
-        <v>0</v>
-      </c>
-      <c r="L87" s="1">
+      <c r="K87" s="1">
+        <v>0</v>
+      </c>
+      <c r="L87" s="12">
         <v>0</v>
       </c>
       <c r="M87" s="1">
@@ -15757,10 +15758,10 @@
       <c r="J88" s="1">
         <v>0</v>
       </c>
-      <c r="K88" s="12">
-        <v>0</v>
-      </c>
-      <c r="L88" s="1">
+      <c r="K88" s="1">
+        <v>0</v>
+      </c>
+      <c r="L88" s="12">
         <v>0</v>
       </c>
       <c r="M88" s="1">
@@ -15908,10 +15909,10 @@
       <c r="J89" s="1">
         <v>0</v>
       </c>
-      <c r="K89" s="12">
-        <v>0</v>
-      </c>
-      <c r="L89" s="1">
+      <c r="K89" s="1">
+        <v>0</v>
+      </c>
+      <c r="L89" s="12">
         <v>0</v>
       </c>
       <c r="M89" s="1">
@@ -16059,10 +16060,10 @@
       <c r="J90" s="1">
         <v>0</v>
       </c>
-      <c r="K90" s="12">
-        <v>0</v>
-      </c>
-      <c r="L90" s="1">
+      <c r="K90" s="1">
+        <v>0</v>
+      </c>
+      <c r="L90" s="12">
         <v>0</v>
       </c>
       <c r="M90" s="1">
@@ -16210,10 +16211,10 @@
       <c r="J91" s="1">
         <v>0</v>
       </c>
-      <c r="K91" s="12">
-        <v>0</v>
-      </c>
-      <c r="L91" s="1">
+      <c r="K91" s="1">
+        <v>0</v>
+      </c>
+      <c r="L91" s="12">
         <v>0</v>
       </c>
       <c r="M91" s="1">
@@ -16361,10 +16362,10 @@
       <c r="J92" s="1">
         <v>39</v>
       </c>
-      <c r="K92" s="12">
-        <v>0</v>
-      </c>
-      <c r="L92" s="1">
+      <c r="K92" s="1">
+        <v>0</v>
+      </c>
+      <c r="L92" s="12">
         <v>0</v>
       </c>
       <c r="M92" s="1">
@@ -16512,10 +16513,10 @@
       <c r="J93" s="1">
         <v>260</v>
       </c>
-      <c r="K93" s="12">
-        <v>0</v>
-      </c>
-      <c r="L93" s="1">
+      <c r="K93" s="1">
+        <v>0</v>
+      </c>
+      <c r="L93" s="12">
         <v>0</v>
       </c>
       <c r="M93" s="1">
@@ -16663,10 +16664,10 @@
       <c r="J94" s="1">
         <v>0</v>
       </c>
-      <c r="K94" s="12">
-        <v>0</v>
-      </c>
-      <c r="L94" s="1">
+      <c r="K94" s="1">
+        <v>0</v>
+      </c>
+      <c r="L94" s="12">
         <v>0</v>
       </c>
       <c r="M94" s="1">
@@ -16814,10 +16815,10 @@
       <c r="J95" s="1">
         <v>0</v>
       </c>
-      <c r="K95" s="12">
-        <v>0</v>
-      </c>
-      <c r="L95" s="1">
+      <c r="K95" s="1">
+        <v>0</v>
+      </c>
+      <c r="L95" s="12">
         <v>0</v>
       </c>
       <c r="M95" s="1">
@@ -16965,10 +16966,10 @@
       <c r="J96" s="1">
         <v>0</v>
       </c>
-      <c r="K96" s="12">
-        <v>0</v>
-      </c>
-      <c r="L96" s="1">
+      <c r="K96" s="1">
+        <v>0</v>
+      </c>
+      <c r="L96" s="12">
         <v>0</v>
       </c>
       <c r="M96" s="1">

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:7eb54fa commit_msg:移动参数修改 ...
</commit_message>
<xml_diff>
--- a/config/excel/Att.xlsx
+++ b/config/excel/Att.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BF31FE-D05E-425A-97DB-44B8E1FD75CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12540"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AttProto" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Admin</author>
   </authors>
   <commentList>
-    <comment ref="P2" authorId="0">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -34,6 +41,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -41,13 +49,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -56,6 +65,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -66,13 +76,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -81,6 +92,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -88,13 +100,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -103,6 +116,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -110,13 +124,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0">
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -125,6 +140,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -133,13 +149,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -148,6 +165,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -158,13 +176,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -173,6 +192,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -180,13 +200,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="D83" authorId="0">
+    <comment ref="D83" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Admin:</t>
@@ -195,6 +216,7 @@
           <rPr>
             <sz val="9"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -335,12 +357,6 @@
     <t>dodge</t>
   </si>
   <si>
-    <t>movescope</t>
-  </si>
-  <si>
-    <t>movetime</t>
-  </si>
-  <si>
     <t>dmgPhysics</t>
   </si>
   <si>
@@ -855,20 +871,24 @@
   </si>
   <si>
     <t>晶石副属性百分比治疗量固定值</t>
+  </si>
+  <si>
+    <t>moveScope</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>moveTime</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -891,172 +911,36 @@
       <sz val="9"/>
       <color indexed="8"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="SimSun"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1077,198 +961,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1304,251 +1002,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1593,57 +1049,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
@@ -1716,6 +1125,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1947,7 +1359,7 @@
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2237,7 +1649,7 @@
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2513,7 +1925,7 @@
           <a:miter lim="400000"/>
         </a:ln>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2786,51 +2198,52 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB96"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.35" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.35" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.625" style="1" customWidth="1"/>
     <col min="5" max="6" width="12.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6166666666667" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.625" style="1" customWidth="1"/>
     <col min="9" max="10" width="13.875" style="1" customWidth="1"/>
     <col min="11" max="11" width="17.75" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.875" style="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="1" customWidth="1"/>
     <col min="14" max="14" width="14.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="7.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5416666666667" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" style="1" customWidth="1"/>
     <col min="17" max="17" width="15.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5416666666667" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.15" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.125" style="1" customWidth="1"/>
     <col min="20" max="20" width="12.75" style="1" customWidth="1"/>
     <col min="21" max="21" width="12" style="1" customWidth="1"/>
     <col min="22" max="22" width="16.5" style="1" customWidth="1"/>
-    <col min="23" max="23" width="14.925" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.875" style="1" customWidth="1"/>
     <col min="24" max="26" width="8" style="1" customWidth="1"/>
     <col min="27" max="28" width="14.5" style="1" customWidth="1"/>
     <col min="29" max="29" width="12.375" style="1" customWidth="1"/>
     <col min="30" max="32" width="14.375" style="1" customWidth="1"/>
     <col min="33" max="52" width="13" style="1" customWidth="1"/>
-    <col min="53" max="54" width="17.35" style="1" customWidth="1"/>
-    <col min="55" max="16384" width="6" style="1" customWidth="1"/>
+    <col min="53" max="54" width="17.375" style="1" customWidth="1"/>
+    <col min="55" max="55" width="6" style="1" customWidth="1"/>
+    <col min="56" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14" customHeight="1" spans="1:54">
+    <row r="1" spans="1:54" ht="14.1" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2890,7 +2303,7 @@
       <c r="BA1" s="3"/>
       <c r="BB1" s="3"/>
     </row>
-    <row r="2" ht="113" customHeight="1" spans="1:54">
+    <row r="2" spans="1:54" ht="113.1" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
@@ -3022,7 +2435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="16.15" customHeight="1" spans="1:54">
+    <row r="3" spans="1:54" ht="16.149999999999999" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
         <v>11</v>
@@ -3112,244 +2525,244 @@
         <v>39</v>
       </c>
       <c r="AE3" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="AG3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AH3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AI3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AK3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AJ3" s="8" t="s">
+      <c r="AL3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AM3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AL3" s="8" t="s">
+      <c r="AN3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AO3" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AP3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AO3" s="8" t="s">
+      <c r="AQ3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AP3" s="8" t="s">
+      <c r="AR3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AQ3" s="8" t="s">
+      <c r="AS3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AR3" s="8" t="s">
+      <c r="AT3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AS3" s="8" t="s">
+      <c r="AU3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AT3" s="8" t="s">
+      <c r="AV3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AU3" s="8" t="s">
+      <c r="AW3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AV3" s="8" t="s">
+      <c r="AX3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AW3" s="8" t="s">
+      <c r="AY3" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AX3" s="8" t="s">
+      <c r="AZ3" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AY3" s="8" t="s">
+      <c r="BA3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AZ3" s="8" t="s">
+      <c r="BB3" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="BA3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="BB3" s="8" t="s">
-        <v>63</v>
-      </c>
     </row>
-    <row r="4" ht="16.15" customHeight="1" spans="1:54">
+    <row r="4" spans="1:54" ht="16.149999999999999" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="T4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="X4" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="W4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="Z4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="AA4" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AB4" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AC4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AD4" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AF4" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="AE4" s="8" t="s">
+      <c r="AG4" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AH4" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="AG4" s="8" t="s">
+      <c r="AI4" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="AH4" s="8" t="s">
+      <c r="AJ4" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="AI4" s="8" t="s">
+      <c r="AK4" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AJ4" s="8" t="s">
+      <c r="AL4" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="AK4" s="8" t="s">
+      <c r="AM4" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AL4" s="8" t="s">
+      <c r="AN4" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AM4" s="8" t="s">
+      <c r="AO4" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="AN4" s="8" t="s">
+      <c r="AP4" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="AO4" s="8" t="s">
+      <c r="AQ4" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AP4" s="8" t="s">
+      <c r="AR4" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AQ4" s="8" t="s">
+      <c r="AS4" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="AR4" s="8" t="s">
+      <c r="AT4" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AS4" s="8" t="s">
+      <c r="AU4" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="AT4" s="8" t="s">
+      <c r="AV4" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AU4" s="8" t="s">
+      <c r="AW4" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="AV4" s="8" t="s">
+      <c r="AX4" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="AW4" s="8" t="s">
+      <c r="AY4" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AX4" s="8" t="s">
+      <c r="AZ4" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="AY4" s="8" t="s">
+      <c r="BA4" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="AZ4" s="8" t="s">
+      <c r="BB4" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="BA4" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="BB4" s="8" t="s">
-        <v>115</v>
-      </c>
     </row>
-    <row r="5" ht="16.15" customHeight="1" spans="1:54">
+    <row r="5" spans="1:54" ht="16.149999999999999" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -3404,98 +2817,98 @@
       <c r="BA5" s="8"/>
       <c r="BB5" s="8"/>
     </row>
-    <row r="6" ht="16.15" customHeight="1" spans="1:54">
+    <row r="6" spans="1:54" ht="16.149999999999999" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="X6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Z6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AA6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AB6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AD6" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AF6" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="AG6" s="8"/>
       <c r="AH6" s="8"/>
@@ -3518,20 +2931,20 @@
       <c r="AY6" s="8"/>
       <c r="AZ6" s="8"/>
       <c r="BA6" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="BB6" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="7" ht="25" customHeight="1" spans="1:54">
+    <row r="7" spans="1:54" ht="24.95" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="9">
         <v>1</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E7" s="11">
         <v>550</v>
@@ -3686,14 +3099,14 @@
         <v>0.15,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="8" ht="25" customHeight="1" spans="1:54">
+    <row r="8" spans="1:54" ht="24.95" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="9">
         <v>2</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E8" s="11">
         <v>550</v>
@@ -3848,14 +3261,14 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="9" ht="25" customHeight="1" spans="1:54">
+    <row r="9" spans="1:54" ht="24.95" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="9">
         <v>3</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E9" s="11">
         <v>550</v>
@@ -3972,31 +3385,31 @@
         <v>0</v>
       </c>
       <c r="AQ9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AR9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AS9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AT9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AU9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AV9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AW9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AX9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AY9" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AZ9" s="12">
         <v>0</v>
@@ -4010,14 +3423,14 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="10" ht="25" customHeight="1" spans="1:54">
+    <row r="10" spans="1:54" ht="24.95" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="9">
         <v>4</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" s="11">
         <v>550</v>
@@ -4110,7 +3523,7 @@
         <v>0</v>
       </c>
       <c r="AI10" s="12">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AJ10" s="12">
         <v>0</v>
@@ -4172,14 +3585,14 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="11" ht="16.15" customHeight="1" spans="1:54">
+    <row r="11" spans="1:54" ht="16.149999999999999" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="9">
         <v>5</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E11" s="13">
         <v>300</v>
@@ -4334,12 +3747,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="12" customHeight="1" spans="3:54">
+    <row r="12" spans="1:54" ht="13.35" customHeight="1">
       <c r="C12" s="1">
         <v>6</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E12" s="13">
         <v>450</v>
@@ -4494,12 +3907,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" customHeight="1" spans="3:54">
+    <row r="13" spans="1:54" ht="13.35" customHeight="1">
       <c r="C13" s="1">
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E13" s="13">
         <v>550</v>
@@ -4654,12 +4067,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="14" customHeight="1" spans="3:54">
+    <row r="14" spans="1:54" ht="13.35" customHeight="1">
       <c r="C14" s="1">
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E14" s="1">
         <v>75</v>
@@ -4814,12 +4227,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="15" customHeight="1" spans="3:54">
+    <row r="15" spans="1:54" ht="13.35" customHeight="1">
       <c r="C15" s="1">
         <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E15" s="1">
         <v>125</v>
@@ -4974,12 +4387,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="16" customHeight="1" spans="3:54">
+    <row r="16" spans="1:54" ht="13.35" customHeight="1">
       <c r="C16" s="1">
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E16" s="1">
         <v>175</v>
@@ -5134,12 +4547,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="17" customHeight="1" spans="3:54">
+    <row r="17" spans="2:54" ht="13.35" customHeight="1">
       <c r="C17" s="1">
         <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E17" s="1">
         <v>225</v>
@@ -5294,12 +4707,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="18" customHeight="1" spans="3:54">
+    <row r="18" spans="2:54" ht="13.35" customHeight="1">
       <c r="C18" s="1">
         <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E18" s="1">
         <v>275</v>
@@ -5454,12 +4867,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="19" customHeight="1" spans="3:54">
+    <row r="19" spans="2:54" ht="13.35" customHeight="1">
       <c r="C19" s="1">
         <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E19" s="1">
         <v>10</v>
@@ -5614,12 +5027,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="20" customHeight="1" spans="3:54">
+    <row r="20" spans="2:54" ht="13.35" customHeight="1">
       <c r="C20" s="1">
         <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E20" s="13">
         <v>50</v>
@@ -5774,12 +5187,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="21" customHeight="1" spans="3:54">
+    <row r="21" spans="2:54" ht="13.35" customHeight="1">
       <c r="C21" s="1">
         <v>2000</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E21" s="1">
         <v>50</v>
@@ -5934,12 +5347,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="22" customHeight="1" spans="3:54">
+    <row r="22" spans="2:54" ht="13.35" customHeight="1">
       <c r="C22" s="1">
         <v>2001</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E22" s="1">
         <v>10</v>
@@ -6094,15 +5507,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="23" customHeight="1" spans="2:54">
+    <row r="23" spans="2:54" ht="13.35" customHeight="1">
       <c r="B23" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C23" s="1">
         <v>2010</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -6114,7 +5527,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="12">
-        <v>0.047</v>
+        <v>4.7E-2</v>
       </c>
       <c r="I23" s="1">
         <v>0</v>
@@ -6257,15 +5670,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="24" customHeight="1" spans="2:54">
+    <row r="24" spans="2:54" ht="13.35" customHeight="1">
       <c r="B24" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" s="1">
         <v>2011</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -6277,7 +5690,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="12">
-        <v>0.072</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="I24" s="1">
         <v>0</v>
@@ -6420,15 +5833,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="25" customHeight="1" spans="2:54">
+    <row r="25" spans="2:54" ht="13.35" customHeight="1">
       <c r="B25" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C25" s="1">
         <v>2012</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -6440,7 +5853,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="12">
-        <v>0.097</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -6583,15 +5996,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="26" customHeight="1" spans="2:54">
+    <row r="26" spans="2:54" ht="13.35" customHeight="1">
       <c r="B26" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C26" s="1">
         <v>2013</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -6746,15 +6159,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="27" customHeight="1" spans="2:54">
+    <row r="27" spans="2:54" ht="13.35" customHeight="1">
       <c r="B27" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C27" s="1">
         <v>2014</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -6766,7 +6179,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="12">
-        <v>0.147</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -6909,15 +6322,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="28" customHeight="1" spans="2:54">
+    <row r="28" spans="2:54" ht="13.35" customHeight="1">
       <c r="B28" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C28" s="1">
         <v>2020</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -7072,15 +6485,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="29" customHeight="1" spans="2:54">
+    <row r="29" spans="2:54" ht="13.35" customHeight="1">
       <c r="B29" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C29" s="1">
         <v>2021</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -7235,15 +6648,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="30" customHeight="1" spans="2:54">
+    <row r="30" spans="2:54" ht="13.35" customHeight="1">
       <c r="B30" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C30" s="1">
         <v>2022</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -7398,15 +6811,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="31" customHeight="1" spans="2:54">
+    <row r="31" spans="2:54" ht="13.35" customHeight="1">
       <c r="B31" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C31" s="1">
         <v>2023</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -7561,15 +6974,15 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="32" customHeight="1" spans="2:54">
+    <row r="32" spans="2:54" ht="13.35" customHeight="1">
       <c r="B32" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C32" s="1">
         <v>2024</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -7724,12 +7137,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="33" customHeight="1" spans="3:54">
+    <row r="33" spans="3:54" ht="13.35" customHeight="1">
       <c r="C33" s="1">
         <v>3000</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E33" s="1">
         <v>6</v>
@@ -7884,12 +7297,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="34" customHeight="1" spans="3:54">
+    <row r="34" spans="3:54" ht="13.35" customHeight="1">
       <c r="C34" s="1">
         <v>3001</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E34" s="1">
         <v>60</v>
@@ -8044,12 +7457,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="35" customHeight="1" spans="3:54">
+    <row r="35" spans="3:54" ht="13.35" customHeight="1">
       <c r="C35" s="1">
         <v>3010</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E35" s="1">
         <v>120</v>
@@ -8204,12 +7617,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="36" customHeight="1" spans="3:54">
+    <row r="36" spans="3:54" ht="13.35" customHeight="1">
       <c r="C36" s="1">
         <v>3011</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E36" s="1">
         <v>1200</v>
@@ -8364,12 +7777,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="37" customHeight="1" spans="3:54">
+    <row r="37" spans="3:54" ht="13.35" customHeight="1">
       <c r="C37" s="1">
         <v>3020</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E37" s="1">
         <v>6</v>
@@ -8524,12 +7937,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="38" customHeight="1" spans="3:54">
+    <row r="38" spans="3:54" ht="13.35" customHeight="1">
       <c r="C38" s="1">
         <v>3021</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E38" s="1">
         <v>60</v>
@@ -8684,12 +8097,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="39" customHeight="1" spans="3:54">
+    <row r="39" spans="3:54" ht="13.35" customHeight="1">
       <c r="C39" s="1">
         <v>3030</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
@@ -8734,7 +8147,7 @@
         <v>0</v>
       </c>
       <c r="S39" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="T39" s="1">
         <v>0</v>
@@ -8844,12 +8257,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="40" customHeight="1" spans="3:54">
+    <row r="40" spans="3:54" ht="13.35" customHeight="1">
       <c r="C40" s="1">
         <v>3031</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -8894,7 +8307,7 @@
         <v>0</v>
       </c>
       <c r="S40" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="T40" s="1">
         <v>0</v>
@@ -9004,12 +8417,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="41" customHeight="1" spans="3:54">
+    <row r="41" spans="3:54" ht="13.35" customHeight="1">
       <c r="C41" s="1">
         <v>3032</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
@@ -9048,7 +8461,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="R41" s="1">
         <v>0</v>
@@ -9164,12 +8577,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="42" customHeight="1" spans="3:54">
+    <row r="42" spans="3:54" ht="13.35" customHeight="1">
       <c r="C42" s="1">
         <v>3033</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
@@ -9208,7 +8621,7 @@
         <v>0</v>
       </c>
       <c r="Q42" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="R42" s="1">
         <v>0</v>
@@ -9324,12 +8737,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="43" customHeight="1" spans="3:54">
+    <row r="43" spans="3:54" ht="13.35" customHeight="1">
       <c r="C43" s="1">
         <v>3034</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E43" s="1">
         <v>0</v>
@@ -9359,7 +8772,7 @@
         <v>0</v>
       </c>
       <c r="N43" s="12">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="O43" s="1">
         <v>0</v>
@@ -9484,12 +8897,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="44" customHeight="1" spans="3:54">
+    <row r="44" spans="3:54" ht="13.35" customHeight="1">
       <c r="C44" s="1">
         <v>3035</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -9519,7 +8932,7 @@
         <v>0</v>
       </c>
       <c r="N44" s="12">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O44" s="1">
         <v>0</v>
@@ -9644,12 +9057,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="45" customHeight="1" spans="3:54">
+    <row r="45" spans="3:54" ht="13.35" customHeight="1">
       <c r="C45" s="1">
         <v>3036</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
@@ -9804,12 +9217,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="46" customHeight="1" spans="3:54">
+    <row r="46" spans="3:54" ht="13.35" customHeight="1">
       <c r="C46" s="1">
         <v>3037</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -9964,12 +9377,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="47" customHeight="1" spans="3:54">
+    <row r="47" spans="3:54" ht="13.35" customHeight="1">
       <c r="C47" s="1">
         <v>3050</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
@@ -10059,7 +9472,7 @@
         <v>0</v>
       </c>
       <c r="AH47" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AI47" s="1">
         <v>0</v>
@@ -10124,12 +9537,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="48" customHeight="1" spans="3:54">
+    <row r="48" spans="3:54" ht="13.35" customHeight="1">
       <c r="C48" s="1">
         <v>3051</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -10222,7 +9635,7 @@
         <v>0</v>
       </c>
       <c r="AI48" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AJ48" s="1">
         <v>0</v>
@@ -10284,12 +9697,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="49" customHeight="1" spans="3:54">
+    <row r="49" spans="3:54" ht="13.35" customHeight="1">
       <c r="C49" s="1">
         <v>3052</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
@@ -10385,7 +9798,7 @@
         <v>0</v>
       </c>
       <c r="AJ49" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AK49" s="1">
         <v>0</v>
@@ -10444,12 +9857,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="50" customHeight="1" spans="3:54">
+    <row r="50" spans="3:54" ht="13.35" customHeight="1">
       <c r="C50" s="1">
         <v>3053</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
@@ -10548,7 +9961,7 @@
         <v>0</v>
       </c>
       <c r="AK50" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AL50" s="1">
         <v>0</v>
@@ -10604,12 +10017,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="51" customHeight="1" spans="3:54">
+    <row r="51" spans="3:54" ht="13.35" customHeight="1">
       <c r="C51" s="1">
         <v>3054</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -10711,7 +10124,7 @@
         <v>0</v>
       </c>
       <c r="AL51" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AM51" s="1">
         <v>0</v>
@@ -10764,12 +10177,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="52" customHeight="1" spans="3:54">
+    <row r="52" spans="3:54" ht="13.35" customHeight="1">
       <c r="C52" s="1">
         <v>3055</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
@@ -10874,7 +10287,7 @@
         <v>0</v>
       </c>
       <c r="AM52" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AN52" s="1">
         <v>0</v>
@@ -10924,12 +10337,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="53" customHeight="1" spans="3:54">
+    <row r="53" spans="3:54" ht="13.35" customHeight="1">
       <c r="C53" s="1">
         <v>3056</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
@@ -11037,7 +10450,7 @@
         <v>0</v>
       </c>
       <c r="AN53" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AO53" s="1">
         <v>0</v>
@@ -11076,20 +10489,20 @@
         <v>0</v>
       </c>
       <c r="BA53" s="10" t="str">
-        <f t="shared" ref="BA48:BA82" si="6">AG47:AG57&amp;","&amp;AH47:AH57&amp;","&amp;AI47:AI57&amp;","&amp;AJ47:AJ57&amp;","&amp;AK47:AK57&amp;","&amp;AL47:AL57&amp;","&amp;AM47:AM57&amp;","&amp;AN47:AN57&amp;","&amp;AO47:AO57&amp;","&amp;AP47:AP57</f>
+        <f t="shared" ref="BA53:BA82" si="6">AG47:AG57&amp;","&amp;AH47:AH57&amp;","&amp;AI47:AI57&amp;","&amp;AJ47:AJ57&amp;","&amp;AK47:AK57&amp;","&amp;AL47:AL57&amp;","&amp;AM47:AM57&amp;","&amp;AN47:AN57&amp;","&amp;AO47:AO57&amp;","&amp;AP47:AP57</f>
         <v>0,0,0,0,0,0,0,0.002,0,0</v>
       </c>
       <c r="BB53" s="10" t="str">
-        <f t="shared" ref="BB48:BB82" si="7">AQ47:AQ57&amp;","&amp;AR47:AR57&amp;","&amp;AS47:AS57&amp;","&amp;AT47:AT57&amp;","&amp;AU47:AU57&amp;","&amp;AV47:AV57&amp;","&amp;AW47:AW57&amp;","&amp;AX47:AX57&amp;","&amp;AY47:AY57&amp;","&amp;AZ47:AZ57</f>
+        <f t="shared" ref="BB53:BB82" si="7">AQ47:AQ57&amp;","&amp;AR47:AR57&amp;","&amp;AS47:AS57&amp;","&amp;AT47:AT57&amp;","&amp;AU47:AU57&amp;","&amp;AV47:AV57&amp;","&amp;AW47:AW57&amp;","&amp;AX47:AX57&amp;","&amp;AY47:AY57&amp;","&amp;AZ47:AZ57</f>
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="54" customHeight="1" spans="3:54">
+    <row r="54" spans="3:54" ht="13.35" customHeight="1">
       <c r="C54" s="1">
         <v>3057</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -11200,7 +10613,7 @@
         <v>0</v>
       </c>
       <c r="AO54" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AP54" s="1">
         <v>0</v>
@@ -11244,12 +10657,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="55" customHeight="1" spans="3:54">
+    <row r="55" spans="3:54" ht="13.35" customHeight="1">
       <c r="C55" s="1">
         <v>3058</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -11363,7 +10776,7 @@
         <v>0</v>
       </c>
       <c r="AP55" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AQ55" s="1">
         <v>0</v>
@@ -11404,12 +10817,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="56" customHeight="1" spans="3:54">
+    <row r="56" spans="3:54" ht="13.35" customHeight="1">
       <c r="C56" s="1">
         <v>3059</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -11499,7 +10912,7 @@
         <v>0</v>
       </c>
       <c r="AH56" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AI56" s="1">
         <v>0</v>
@@ -11564,12 +10977,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="57" customHeight="1" spans="3:54">
+    <row r="57" spans="3:54" ht="13.35" customHeight="1">
       <c r="C57" s="1">
         <v>3060</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -11662,7 +11075,7 @@
         <v>0</v>
       </c>
       <c r="AI57" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AJ57" s="1">
         <v>0</v>
@@ -11724,12 +11137,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="58" customHeight="1" spans="3:54">
+    <row r="58" spans="3:54" ht="13.35" customHeight="1">
       <c r="C58" s="1">
         <v>3061</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
@@ -11825,7 +11238,7 @@
         <v>0</v>
       </c>
       <c r="AJ58" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AK58" s="1">
         <v>0</v>
@@ -11884,12 +11297,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="59" customHeight="1" spans="3:54">
+    <row r="59" spans="3:54" ht="13.35" customHeight="1">
       <c r="C59" s="1">
         <v>3062</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E59" s="1">
         <v>0</v>
@@ -11988,7 +11401,7 @@
         <v>0</v>
       </c>
       <c r="AK59" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AL59" s="1">
         <v>0</v>
@@ -12044,12 +11457,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="60" customHeight="1" spans="3:54">
+    <row r="60" spans="3:54" ht="13.35" customHeight="1">
       <c r="C60" s="1">
         <v>3063</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
@@ -12151,7 +11564,7 @@
         <v>0</v>
       </c>
       <c r="AL60" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AM60" s="1">
         <v>0</v>
@@ -12204,12 +11617,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="61" customHeight="1" spans="3:54">
+    <row r="61" spans="3:54" ht="13.35" customHeight="1">
       <c r="C61" s="1">
         <v>3064</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>
@@ -12314,7 +11727,7 @@
         <v>0</v>
       </c>
       <c r="AM61" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AN61" s="1">
         <v>0</v>
@@ -12364,12 +11777,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="62" customHeight="1" spans="3:54">
+    <row r="62" spans="3:54" ht="13.35" customHeight="1">
       <c r="C62" s="1">
         <v>3065</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E62" s="1">
         <v>0</v>
@@ -12477,7 +11890,7 @@
         <v>0</v>
       </c>
       <c r="AN62" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AO62" s="1">
         <v>0</v>
@@ -12524,12 +11937,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="63" customHeight="1" spans="3:54">
+    <row r="63" spans="3:54" ht="13.35" customHeight="1">
       <c r="C63" s="1">
         <v>3066</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E63" s="1">
         <v>0</v>
@@ -12640,7 +12053,7 @@
         <v>0</v>
       </c>
       <c r="AO63" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AP63" s="1">
         <v>0</v>
@@ -12684,12 +12097,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="64" customHeight="1" spans="3:54">
+    <row r="64" spans="3:54" ht="13.35" customHeight="1">
       <c r="C64" s="1">
         <v>3067</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E64" s="1">
         <v>0</v>
@@ -12803,7 +12216,7 @@
         <v>0</v>
       </c>
       <c r="AP64" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AQ64" s="1">
         <v>0</v>
@@ -12844,12 +12257,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="65" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="65" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C65" s="2">
         <v>3068</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E65" s="2">
         <v>0</v>
@@ -12969,7 +12382,7 @@
         <v>0</v>
       </c>
       <c r="AR65" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AS65" s="2">
         <v>0</v>
@@ -13004,12 +12417,12 @@
         <v>0,0.002,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="66" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="66" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C66" s="2">
         <v>3069</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E66" s="2">
         <v>0</v>
@@ -13132,7 +12545,7 @@
         <v>0</v>
       </c>
       <c r="AS66" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AT66" s="2">
         <v>0</v>
@@ -13164,12 +12577,12 @@
         <v>0,0,0.002,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="67" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="67" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C67" s="2">
         <v>3070</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E67" s="2">
         <v>0</v>
@@ -13295,7 +12708,7 @@
         <v>0</v>
       </c>
       <c r="AT67" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AU67" s="2">
         <v>0</v>
@@ -13324,12 +12737,12 @@
         <v>0,0,0,0.002,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="68" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="68" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C68" s="2">
         <v>3071</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E68" s="2">
         <v>0</v>
@@ -13458,7 +12871,7 @@
         <v>0</v>
       </c>
       <c r="AU68" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AV68" s="2">
         <v>0</v>
@@ -13484,12 +12897,12 @@
         <v>0,0,0,0,0.002,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="69" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="69" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C69" s="2">
         <v>3072</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E69" s="2">
         <v>0</v>
@@ -13621,7 +13034,7 @@
         <v>0</v>
       </c>
       <c r="AV69" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AW69" s="2">
         <v>0</v>
@@ -13644,12 +13057,12 @@
         <v>0,0,0,0,0,0.002,0,0,0,0</v>
       </c>
     </row>
-    <row r="70" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="70" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C70" s="2">
         <v>3073</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E70" s="2">
         <v>0</v>
@@ -13784,7 +13197,7 @@
         <v>0</v>
       </c>
       <c r="AW70" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AX70" s="2">
         <v>0</v>
@@ -13804,12 +13217,12 @@
         <v>0,0,0,0,0,0,0.002,0,0,0</v>
       </c>
     </row>
-    <row r="71" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="71" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C71" s="2">
         <v>3074</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E71" s="2">
         <v>0</v>
@@ -13947,7 +13360,7 @@
         <v>0</v>
       </c>
       <c r="AX71" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AY71" s="2">
         <v>0</v>
@@ -13964,12 +13377,12 @@
         <v>0,0,0,0,0,0,0,0.002,0,0</v>
       </c>
     </row>
-    <row r="72" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="72" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C72" s="2">
         <v>3075</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E72" s="2">
         <v>0</v>
@@ -14110,7 +13523,7 @@
         <v>0</v>
       </c>
       <c r="AY72" s="1">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AZ72" s="2">
         <v>0</v>
@@ -14124,12 +13537,12 @@
         <v>0,0,0,0,0,0,0,0,0.002,0</v>
       </c>
     </row>
-    <row r="73" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="73" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C73" s="2">
         <v>3076</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E73" s="2">
         <v>0</v>
@@ -14284,12 +13697,12 @@
         <v>0,0,0,0,0,0,0,0,0,20</v>
       </c>
     </row>
-    <row r="74" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="74" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C74" s="2">
         <v>3077</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E74" s="2">
         <v>0</v>
@@ -14409,7 +13822,7 @@
         <v>0</v>
       </c>
       <c r="AR74" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AS74" s="2">
         <v>0</v>
@@ -14444,12 +13857,12 @@
         <v>0,0.005,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="75" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="75" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C75" s="2">
         <v>3078</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E75" s="2">
         <v>0</v>
@@ -14572,7 +13985,7 @@
         <v>0</v>
       </c>
       <c r="AS75" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AT75" s="2">
         <v>0</v>
@@ -14604,12 +14017,12 @@
         <v>0,0,0.005,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="76" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="76" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C76" s="2">
         <v>3079</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E76" s="2">
         <v>0</v>
@@ -14735,7 +14148,7 @@
         <v>0</v>
       </c>
       <c r="AT76" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AU76" s="2">
         <v>0</v>
@@ -14764,12 +14177,12 @@
         <v>0,0,0,0.005,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="77" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="77" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C77" s="2">
         <v>3080</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E77" s="2">
         <v>0</v>
@@ -14898,7 +14311,7 @@
         <v>0</v>
       </c>
       <c r="AU77" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AV77" s="2">
         <v>0</v>
@@ -14924,12 +14337,12 @@
         <v>0,0,0,0,0.005,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="78" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="78" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C78" s="2">
         <v>3081</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E78" s="2">
         <v>0</v>
@@ -15061,7 +14474,7 @@
         <v>0</v>
       </c>
       <c r="AV78" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AW78" s="2">
         <v>0</v>
@@ -15084,12 +14497,12 @@
         <v>0,0,0,0,0,0.005,0,0,0,0</v>
       </c>
     </row>
-    <row r="79" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="79" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C79" s="2">
         <v>3082</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E79" s="2">
         <v>0</v>
@@ -15224,7 +14637,7 @@
         <v>0</v>
       </c>
       <c r="AW79" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AX79" s="2">
         <v>0</v>
@@ -15244,12 +14657,12 @@
         <v>0,0,0,0,0,0,0.005,0,0,0</v>
       </c>
     </row>
-    <row r="80" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="80" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C80" s="2">
         <v>3083</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E80" s="2">
         <v>0</v>
@@ -15387,7 +14800,7 @@
         <v>0</v>
       </c>
       <c r="AX80" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AY80" s="2">
         <v>0</v>
@@ -15404,12 +14817,12 @@
         <v>0,0,0,0,0,0,0,0.005,0,0</v>
       </c>
     </row>
-    <row r="81" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="81" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C81" s="2">
         <v>3084</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E81" s="2">
         <v>0</v>
@@ -15550,7 +14963,7 @@
         <v>0</v>
       </c>
       <c r="AY81" s="1">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AZ81" s="2">
         <v>0</v>
@@ -15564,12 +14977,12 @@
         <v>0,0,0,0,0,0,0,0,0.005,0</v>
       </c>
     </row>
-    <row r="82" s="2" customFormat="1" customHeight="1" spans="3:54">
+    <row r="82" spans="3:54" s="2" customFormat="1" ht="13.35" customHeight="1">
       <c r="C82" s="2">
         <v>3085</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E82" s="2">
         <v>0</v>
@@ -15724,12 +15137,12 @@
         <v>0,0,0,0,0,0,0,0,0,50</v>
       </c>
     </row>
-    <row r="83" customHeight="1" spans="3:54">
+    <row r="83" spans="3:54" ht="13.35" customHeight="1">
       <c r="C83" s="1">
         <v>3200</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E83" s="1">
         <v>36</v>
@@ -15884,12 +15297,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="84" customHeight="1" spans="3:54">
+    <row r="84" spans="3:54" ht="13.35" customHeight="1">
       <c r="C84" s="1">
         <v>3201</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E84" s="1">
         <v>0</v>
@@ -16044,12 +15457,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="85" customHeight="1" spans="3:54">
+    <row r="85" spans="3:54" ht="13.35" customHeight="1">
       <c r="C85" s="1">
         <v>3202</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E85" s="1">
         <v>0</v>
@@ -16204,18 +15617,18 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="86" customHeight="1" spans="3:54">
+    <row r="86" spans="3:54" ht="13.35" customHeight="1">
       <c r="C86" s="1">
         <v>3203</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E86" s="1">
         <v>0</v>
       </c>
       <c r="F86" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="G86" s="1">
         <v>0</v>
@@ -16364,12 +15777,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="87" customHeight="1" spans="3:54">
+    <row r="87" spans="3:54" ht="13.35" customHeight="1">
       <c r="C87" s="1">
         <v>3204</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E87" s="1">
         <v>0</v>
@@ -16381,7 +15794,7 @@
         <v>0</v>
       </c>
       <c r="H87" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I87" s="1">
         <v>0</v>
@@ -16524,12 +15937,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="88" customHeight="1" spans="3:54">
+    <row r="88" spans="3:54" ht="13.35" customHeight="1">
       <c r="C88" s="1">
         <v>3205</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E88" s="1">
         <v>0</v>
@@ -16586,7 +15999,7 @@
         <v>0</v>
       </c>
       <c r="W88" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="X88" s="1">
         <v>0</v>
@@ -16684,12 +16097,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="89" customHeight="1" spans="3:54">
+    <row r="89" spans="3:54" ht="13.35" customHeight="1">
       <c r="C89" s="1">
         <v>3206</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E89" s="1">
         <v>0</v>
@@ -16844,12 +16257,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="90" customHeight="1" spans="3:54">
+    <row r="90" spans="3:54" ht="13.35" customHeight="1">
       <c r="C90" s="1">
         <v>3207</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E90" s="1">
         <v>0</v>
@@ -17004,12 +16417,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="91" customHeight="1" spans="3:54">
+    <row r="91" spans="3:54" ht="13.35" customHeight="1">
       <c r="C91" s="1">
         <v>3208</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E91" s="1">
         <v>0</v>
@@ -17164,12 +16577,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="92" customHeight="1" spans="3:54">
+    <row r="92" spans="3:54" ht="13.35" customHeight="1">
       <c r="C92" s="1">
         <v>3209</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E92" s="1">
         <v>0</v>
@@ -17324,12 +16737,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="93" customHeight="1" spans="3:54">
+    <row r="93" spans="3:54" ht="13.35" customHeight="1">
       <c r="C93" s="1">
         <v>3210</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E93" s="1">
         <v>0</v>
@@ -17484,12 +16897,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="94" customHeight="1" spans="3:54">
+    <row r="94" spans="3:54" ht="13.35" customHeight="1">
       <c r="C94" s="1">
         <v>3211</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E94" s="1">
         <v>0</v>
@@ -17534,7 +16947,7 @@
         <v>0</v>
       </c>
       <c r="S94" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="T94" s="1">
         <v>0</v>
@@ -17644,12 +17057,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="95" customHeight="1" spans="3:54">
+    <row r="95" spans="3:54" ht="13.35" customHeight="1">
       <c r="C95" s="1">
         <v>3212</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E95" s="1">
         <v>0</v>
@@ -17688,7 +17101,7 @@
         <v>0</v>
       </c>
       <c r="Q95" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="R95" s="1">
         <v>0</v>
@@ -17804,12 +17217,12 @@
         <v>0,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
-    <row r="96" customHeight="1" spans="3:54">
+    <row r="96" spans="3:54" ht="13.35" customHeight="1">
       <c r="C96" s="1">
         <v>3213</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E96" s="1">
         <v>0</v>
@@ -17839,7 +17252,7 @@
         <v>0</v>
       </c>
       <c r="N96" s="1">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="O96" s="1">
         <v>0</v>
@@ -17965,11 +17378,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>